<commit_message>
update plan and use case
</commit_message>
<xml_diff>
--- a/PlanExcel/plan.xlsx
+++ b/PlanExcel/plan.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\~project\AndroidKotlin\MUSIC\PlanExcel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0FF71DD-C672-438D-BCFD-E83A9C3928C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7AD5799-44B8-43A3-B718-2893208BBCBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="14880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -266,13 +266,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -288,9 +281,16 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -561,36 +561,36 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Y1003"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.6640625" customWidth="1"/>
-    <col min="2" max="2" width="46.5546875" customWidth="1"/>
-    <col min="3" max="3" width="79.21875" customWidth="1"/>
-    <col min="4" max="4" width="26.21875" customWidth="1"/>
-    <col min="5" max="5" width="27.88671875" customWidth="1"/>
-    <col min="6" max="6" width="28.21875" customWidth="1"/>
-    <col min="7" max="7" width="26.33203125" customWidth="1"/>
-    <col min="8" max="8" width="27.21875" customWidth="1"/>
-    <col min="9" max="9" width="11.21875" customWidth="1"/>
-    <col min="10" max="25" width="8.6640625" customWidth="1"/>
+    <col min="1" max="1" width="8.7109375" customWidth="1"/>
+    <col min="2" max="2" width="46.5703125" customWidth="1"/>
+    <col min="3" max="3" width="79.28515625" customWidth="1"/>
+    <col min="4" max="4" width="26.28515625" customWidth="1"/>
+    <col min="5" max="5" width="27.85546875" customWidth="1"/>
+    <col min="6" max="6" width="28.28515625" customWidth="1"/>
+    <col min="7" max="7" width="26.28515625" customWidth="1"/>
+    <col min="8" max="8" width="27.28515625" customWidth="1"/>
+    <col min="9" max="9" width="11.28515625" customWidth="1"/>
+    <col min="10" max="25" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" ht="33.6" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="11" t="s">
+    <row r="1" spans="1:25" ht="33.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
-      <c r="G1" s="12"/>
-      <c r="H1" s="12"/>
-      <c r="I1" s="12"/>
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
+      <c r="H1" s="17"/>
+      <c r="I1" s="17"/>
       <c r="J1" s="1"/>
       <c r="K1" s="1"/>
       <c r="L1" s="1"/>
@@ -608,18 +608,18 @@
       <c r="X1" s="1"/>
       <c r="Y1" s="1"/>
     </row>
-    <row r="2" spans="1:25" ht="31.8" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="11" t="s">
+    <row r="2" spans="1:25" ht="31.9" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="12"/>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12"/>
-      <c r="E2" s="12"/>
-      <c r="F2" s="12"/>
-      <c r="G2" s="12"/>
-      <c r="H2" s="12"/>
-      <c r="I2" s="12"/>
+      <c r="B2" s="17"/>
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="17"/>
+      <c r="G2" s="17"/>
+      <c r="H2" s="17"/>
+      <c r="I2" s="17"/>
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
       <c r="L2" s="1"/>
@@ -637,18 +637,18 @@
       <c r="X2" s="1"/>
       <c r="Y2" s="1"/>
     </row>
-    <row r="3" spans="1:25" ht="25.8" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="11" t="s">
+    <row r="3" spans="1:25" ht="25.9" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="12"/>
-      <c r="C3" s="12"/>
-      <c r="D3" s="12"/>
-      <c r="E3" s="12"/>
-      <c r="F3" s="12"/>
-      <c r="G3" s="12"/>
-      <c r="H3" s="12"/>
-      <c r="I3" s="12"/>
+      <c r="B3" s="17"/>
+      <c r="C3" s="17"/>
+      <c r="D3" s="17"/>
+      <c r="E3" s="17"/>
+      <c r="F3" s="17"/>
+      <c r="G3" s="17"/>
+      <c r="H3" s="17"/>
+      <c r="I3" s="17"/>
       <c r="J3" s="1"/>
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
@@ -666,20 +666,20 @@
       <c r="X3" s="1"/>
       <c r="Y3" s="1"/>
     </row>
-    <row r="4" spans="1:25" ht="138.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:25" ht="138.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2"/>
       <c r="B4" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="19" t="s">
+      <c r="C4" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="D4" s="13"/>
-      <c r="E4" s="13"/>
-      <c r="F4" s="13"/>
-      <c r="G4" s="13"/>
-      <c r="H4" s="13"/>
-      <c r="I4" s="13"/>
+      <c r="D4" s="19"/>
+      <c r="E4" s="19"/>
+      <c r="F4" s="19"/>
+      <c r="G4" s="19"/>
+      <c r="H4" s="19"/>
+      <c r="I4" s="19"/>
       <c r="J4" s="3"/>
       <c r="K4" s="3"/>
       <c r="L4" s="3"/>
@@ -697,35 +697,35 @@
       <c r="X4" s="3"/>
       <c r="Y4" s="3"/>
     </row>
-    <row r="5" spans="1:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C5" s="4"/>
     </row>
-    <row r="6" spans="1:25" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="14" t="s">
+    <row r="6" spans="1:25" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="14" t="s">
+      <c r="B6" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="14" t="s">
+      <c r="C6" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="D6" s="14" t="s">
+      <c r="D6" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="E6" s="14" t="s">
+      <c r="E6" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="F6" s="14" t="s">
+      <c r="F6" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="G6" s="14" t="s">
+      <c r="G6" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="H6" s="14" t="s">
+      <c r="H6" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="I6" s="14" t="s">
+      <c r="I6" s="11" t="s">
         <v>12</v>
       </c>
       <c r="J6" s="5"/>
@@ -745,30 +745,30 @@
       <c r="X6" s="5"/>
       <c r="Y6" s="5"/>
     </row>
-    <row r="7" spans="1:25" ht="45.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="14">
+    <row r="7" spans="1:25" ht="45.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="11">
         <v>1</v>
       </c>
-      <c r="B7" s="15" t="s">
+      <c r="B7" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="16" t="s">
+      <c r="C7" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="D7" s="14" t="s">
+      <c r="D7" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="E7" s="17">
+      <c r="E7" s="14">
         <v>44809</v>
       </c>
-      <c r="F7" s="17">
+      <c r="F7" s="14">
         <v>44813</v>
       </c>
-      <c r="G7" s="17">
+      <c r="G7" s="14">
         <v>44809</v>
       </c>
-      <c r="H7" s="17"/>
-      <c r="I7" s="14"/>
+      <c r="H7" s="14"/>
+      <c r="I7" s="11"/>
       <c r="J7" s="5"/>
       <c r="K7" s="5"/>
       <c r="L7" s="5"/>
@@ -786,28 +786,28 @@
       <c r="X7" s="5"/>
       <c r="Y7" s="5"/>
     </row>
-    <row r="8" spans="1:25" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="14">
+    <row r="8" spans="1:25" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="11">
         <v>2</v>
       </c>
-      <c r="B8" s="15" t="s">
+      <c r="B8" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="C8" s="16" t="s">
+      <c r="C8" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="D8" s="14" t="s">
+      <c r="D8" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="E8" s="17">
+      <c r="E8" s="14">
         <v>44814</v>
       </c>
-      <c r="F8" s="17">
+      <c r="F8" s="14">
         <v>44816</v>
       </c>
-      <c r="G8" s="17"/>
-      <c r="H8" s="17"/>
-      <c r="I8" s="14"/>
+      <c r="G8" s="14"/>
+      <c r="H8" s="14"/>
+      <c r="I8" s="11"/>
       <c r="J8" s="5"/>
       <c r="K8" s="5"/>
       <c r="L8" s="5"/>
@@ -825,24 +825,26 @@
       <c r="X8" s="5"/>
       <c r="Y8" s="5"/>
     </row>
-    <row r="9" spans="1:25" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="14"/>
-      <c r="B9" s="14"/>
-      <c r="C9" s="15" t="s">
+    <row r="9" spans="1:25" ht="20.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="11"/>
+      <c r="B9" s="11"/>
+      <c r="C9" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="D9" s="14" t="s">
+      <c r="D9" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="E9" s="17">
+      <c r="E9" s="14">
         <v>44817</v>
       </c>
-      <c r="F9" s="17">
+      <c r="F9" s="14">
         <v>44819</v>
       </c>
-      <c r="G9" s="17"/>
-      <c r="H9" s="17"/>
-      <c r="I9" s="14"/>
+      <c r="G9" s="14">
+        <v>44817</v>
+      </c>
+      <c r="H9" s="14"/>
+      <c r="I9" s="11"/>
       <c r="J9" s="5"/>
       <c r="K9" s="5"/>
       <c r="L9" s="5"/>
@@ -860,24 +862,26 @@
       <c r="X9" s="5"/>
       <c r="Y9" s="5"/>
     </row>
-    <row r="10" spans="1:25" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="14"/>
-      <c r="B10" s="14"/>
-      <c r="C10" s="15" t="s">
+    <row r="10" spans="1:25" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="11"/>
+      <c r="B10" s="11"/>
+      <c r="C10" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="D10" s="14" t="s">
+      <c r="D10" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="E10" s="17">
+      <c r="E10" s="14">
         <v>44820</v>
       </c>
-      <c r="F10" s="17">
+      <c r="F10" s="14">
         <v>44821</v>
       </c>
-      <c r="G10" s="17"/>
-      <c r="H10" s="17"/>
-      <c r="I10" s="14"/>
+      <c r="G10" s="14">
+        <v>44820</v>
+      </c>
+      <c r="H10" s="14"/>
+      <c r="I10" s="11"/>
       <c r="J10" s="5"/>
       <c r="K10" s="5"/>
       <c r="L10" s="5"/>
@@ -895,28 +899,30 @@
       <c r="X10" s="5"/>
       <c r="Y10" s="5"/>
     </row>
-    <row r="11" spans="1:25" ht="25.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="14">
+    <row r="11" spans="1:25" ht="25.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="11">
         <v>3</v>
       </c>
-      <c r="B11" s="15" t="s">
+      <c r="B11" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="C11" s="15" t="s">
+      <c r="C11" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="D11" s="14" t="s">
+      <c r="D11" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="E11" s="17">
+      <c r="E11" s="14">
         <v>44822</v>
       </c>
-      <c r="F11" s="17">
+      <c r="F11" s="14">
         <v>44825</v>
       </c>
-      <c r="G11" s="17"/>
-      <c r="H11" s="17"/>
-      <c r="I11" s="14"/>
+      <c r="G11" s="14">
+        <v>44822</v>
+      </c>
+      <c r="H11" s="14"/>
+      <c r="I11" s="11"/>
       <c r="J11" s="5"/>
       <c r="K11" s="5"/>
       <c r="L11" s="5"/>
@@ -934,28 +940,28 @@
       <c r="X11" s="5"/>
       <c r="Y11" s="5"/>
     </row>
-    <row r="12" spans="1:25" ht="45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="14">
+    <row r="12" spans="1:25" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="11">
         <v>4</v>
       </c>
-      <c r="B12" s="15" t="s">
+      <c r="B12" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="C12" s="16" t="s">
+      <c r="C12" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="D12" s="14" t="s">
+      <c r="D12" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="E12" s="17">
+      <c r="E12" s="14">
         <v>44826</v>
       </c>
-      <c r="F12" s="17">
+      <c r="F12" s="14">
         <v>44835</v>
       </c>
-      <c r="G12" s="17"/>
-      <c r="H12" s="17"/>
-      <c r="I12" s="14"/>
+      <c r="G12" s="14"/>
+      <c r="H12" s="14"/>
+      <c r="I12" s="11"/>
       <c r="J12" s="5"/>
       <c r="K12" s="5"/>
       <c r="L12" s="5"/>
@@ -973,28 +979,28 @@
       <c r="X12" s="5"/>
       <c r="Y12" s="5"/>
     </row>
-    <row r="13" spans="1:25" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="14">
+    <row r="13" spans="1:25" ht="20.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="11">
         <v>5</v>
       </c>
-      <c r="B13" s="15" t="s">
+      <c r="B13" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="C13" s="15" t="s">
+      <c r="C13" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="D13" s="14" t="s">
+      <c r="D13" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="E13" s="17">
+      <c r="E13" s="14">
         <v>44836</v>
       </c>
-      <c r="F13" s="17">
+      <c r="F13" s="14">
         <v>44838</v>
       </c>
-      <c r="G13" s="17"/>
-      <c r="H13" s="17"/>
-      <c r="I13" s="14"/>
+      <c r="G13" s="14"/>
+      <c r="H13" s="14"/>
+      <c r="I13" s="11"/>
       <c r="J13" s="5"/>
       <c r="K13" s="5"/>
       <c r="L13" s="5"/>
@@ -1012,24 +1018,24 @@
       <c r="X13" s="5"/>
       <c r="Y13" s="5"/>
     </row>
-    <row r="14" spans="1:25" ht="62.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="14"/>
-      <c r="B14" s="14"/>
-      <c r="C14" s="16" t="s">
+    <row r="14" spans="1:25" ht="62.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="11"/>
+      <c r="B14" s="11"/>
+      <c r="C14" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="D14" s="14" t="s">
+      <c r="D14" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="E14" s="17">
+      <c r="E14" s="14">
         <v>44838</v>
       </c>
-      <c r="F14" s="17">
+      <c r="F14" s="14">
         <v>44842</v>
       </c>
-      <c r="G14" s="17"/>
-      <c r="H14" s="17"/>
-      <c r="I14" s="14"/>
+      <c r="G14" s="14"/>
+      <c r="H14" s="14"/>
+      <c r="I14" s="11"/>
       <c r="J14" s="5"/>
       <c r="K14" s="5"/>
       <c r="L14" s="5"/>
@@ -1047,28 +1053,28 @@
       <c r="X14" s="5"/>
       <c r="Y14" s="5"/>
     </row>
-    <row r="15" spans="1:25" ht="41.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="14">
+    <row r="15" spans="1:25" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="11">
         <v>6</v>
       </c>
-      <c r="B15" s="15" t="s">
+      <c r="B15" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="C15" s="16" t="s">
+      <c r="C15" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="D15" s="14" t="s">
+      <c r="D15" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="E15" s="17">
+      <c r="E15" s="14">
         <v>44843</v>
       </c>
-      <c r="F15" s="17">
+      <c r="F15" s="14">
         <v>44846</v>
       </c>
-      <c r="G15" s="17"/>
-      <c r="H15" s="17"/>
-      <c r="I15" s="14"/>
+      <c r="G15" s="14"/>
+      <c r="H15" s="14"/>
+      <c r="I15" s="11"/>
       <c r="J15" s="5"/>
       <c r="K15" s="5"/>
       <c r="L15" s="5"/>
@@ -1086,24 +1092,24 @@
       <c r="X15" s="5"/>
       <c r="Y15" s="5"/>
     </row>
-    <row r="16" spans="1:25" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="14"/>
-      <c r="B16" s="14"/>
-      <c r="C16" s="15" t="s">
+    <row r="16" spans="1:25" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="11"/>
+      <c r="B16" s="11"/>
+      <c r="C16" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="D16" s="14" t="s">
+      <c r="D16" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="E16" s="17">
+      <c r="E16" s="14">
         <v>44847</v>
       </c>
-      <c r="F16" s="17">
+      <c r="F16" s="14">
         <v>44849</v>
       </c>
-      <c r="G16" s="17"/>
-      <c r="H16" s="17"/>
-      <c r="I16" s="14"/>
+      <c r="G16" s="14"/>
+      <c r="H16" s="14"/>
+      <c r="I16" s="11"/>
       <c r="J16" s="5"/>
       <c r="K16" s="5"/>
       <c r="L16" s="5"/>
@@ -1121,24 +1127,24 @@
       <c r="X16" s="5"/>
       <c r="Y16" s="5"/>
     </row>
-    <row r="17" spans="1:25" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="14"/>
-      <c r="B17" s="14"/>
-      <c r="C17" s="15" t="s">
+    <row r="17" spans="1:25" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="11"/>
+      <c r="B17" s="11"/>
+      <c r="C17" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="D17" s="14" t="s">
+      <c r="D17" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="E17" s="17">
+      <c r="E17" s="14">
         <v>44850</v>
       </c>
-      <c r="F17" s="17">
+      <c r="F17" s="14">
         <v>44852</v>
       </c>
-      <c r="G17" s="17"/>
-      <c r="H17" s="17"/>
-      <c r="I17" s="14"/>
+      <c r="G17" s="14"/>
+      <c r="H17" s="14"/>
+      <c r="I17" s="11"/>
       <c r="J17" s="5"/>
       <c r="K17" s="5"/>
       <c r="L17" s="5"/>
@@ -1156,24 +1162,24 @@
       <c r="X17" s="5"/>
       <c r="Y17" s="5"/>
     </row>
-    <row r="18" spans="1:25" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="14"/>
-      <c r="B18" s="14"/>
-      <c r="C18" s="15" t="s">
+    <row r="18" spans="1:25" ht="23.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="11"/>
+      <c r="B18" s="11"/>
+      <c r="C18" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="D18" s="14" t="s">
+      <c r="D18" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="E18" s="17">
+      <c r="E18" s="14">
         <v>44853</v>
       </c>
-      <c r="F18" s="17">
+      <c r="F18" s="14">
         <v>44855</v>
       </c>
-      <c r="G18" s="17"/>
-      <c r="H18" s="17"/>
-      <c r="I18" s="14"/>
+      <c r="G18" s="14"/>
+      <c r="H18" s="14"/>
+      <c r="I18" s="11"/>
       <c r="J18" s="5"/>
       <c r="K18" s="5"/>
       <c r="L18" s="5"/>
@@ -1191,24 +1197,24 @@
       <c r="X18" s="5"/>
       <c r="Y18" s="5"/>
     </row>
-    <row r="19" spans="1:25" ht="21.6" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A19" s="14"/>
-      <c r="B19" s="14"/>
-      <c r="C19" s="18" t="s">
+    <row r="19" spans="1:25" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="11"/>
+      <c r="B19" s="11"/>
+      <c r="C19" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="D19" s="14" t="s">
+      <c r="D19" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="E19" s="17">
+      <c r="E19" s="14">
         <v>44856</v>
       </c>
-      <c r="F19" s="17">
+      <c r="F19" s="14">
         <v>44858</v>
       </c>
-      <c r="G19" s="17"/>
-      <c r="H19" s="17"/>
-      <c r="I19" s="14"/>
+      <c r="G19" s="14"/>
+      <c r="H19" s="14"/>
+      <c r="I19" s="11"/>
       <c r="J19" s="5"/>
       <c r="K19" s="5"/>
       <c r="L19" s="5"/>
@@ -1226,24 +1232,24 @@
       <c r="X19" s="5"/>
       <c r="Y19" s="5"/>
     </row>
-    <row r="20" spans="1:25" ht="22.8" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A20" s="14"/>
-      <c r="B20" s="14"/>
-      <c r="C20" s="18" t="s">
+    <row r="20" spans="1:25" ht="22.9" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="11"/>
+      <c r="B20" s="11"/>
+      <c r="C20" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="D20" s="14" t="s">
+      <c r="D20" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="E20" s="17">
+      <c r="E20" s="14">
         <v>44859</v>
       </c>
-      <c r="F20" s="17">
+      <c r="F20" s="14">
         <v>44861</v>
       </c>
-      <c r="G20" s="17"/>
-      <c r="H20" s="17"/>
-      <c r="I20" s="14"/>
+      <c r="G20" s="14"/>
+      <c r="H20" s="14"/>
+      <c r="I20" s="11"/>
       <c r="J20" s="5"/>
       <c r="K20" s="5"/>
       <c r="L20" s="5"/>
@@ -1261,24 +1267,24 @@
       <c r="X20" s="5"/>
       <c r="Y20" s="5"/>
     </row>
-    <row r="21" spans="1:25" ht="22.2" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A21" s="14"/>
-      <c r="B21" s="14"/>
-      <c r="C21" s="18" t="s">
+    <row r="21" spans="1:25" ht="22.15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="11"/>
+      <c r="B21" s="11"/>
+      <c r="C21" s="15" t="s">
         <v>40</v>
       </c>
-      <c r="D21" s="14" t="s">
+      <c r="D21" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="E21" s="17">
+      <c r="E21" s="14">
         <v>44862</v>
       </c>
-      <c r="F21" s="17">
+      <c r="F21" s="14">
         <v>44863</v>
       </c>
-      <c r="G21" s="17"/>
-      <c r="H21" s="17"/>
-      <c r="I21" s="14"/>
+      <c r="G21" s="14"/>
+      <c r="H21" s="14"/>
+      <c r="I21" s="11"/>
       <c r="J21" s="5"/>
       <c r="K21" s="5"/>
       <c r="L21" s="5"/>
@@ -1296,24 +1302,24 @@
       <c r="X21" s="5"/>
       <c r="Y21" s="5"/>
     </row>
-    <row r="22" spans="1:25" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A22" s="14"/>
-      <c r="B22" s="14"/>
-      <c r="C22" s="18" t="s">
+    <row r="22" spans="1:25" ht="20.45" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="11"/>
+      <c r="B22" s="11"/>
+      <c r="C22" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="D22" s="14" t="s">
+      <c r="D22" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="E22" s="17">
+      <c r="E22" s="14">
         <v>44864</v>
       </c>
-      <c r="F22" s="17">
+      <c r="F22" s="14">
         <v>44866</v>
       </c>
-      <c r="G22" s="17"/>
-      <c r="H22" s="17"/>
-      <c r="I22" s="14"/>
+      <c r="G22" s="14"/>
+      <c r="H22" s="14"/>
+      <c r="I22" s="11"/>
       <c r="J22" s="5"/>
       <c r="K22" s="5"/>
       <c r="L22" s="5"/>
@@ -1331,24 +1337,24 @@
       <c r="X22" s="5"/>
       <c r="Y22" s="5"/>
     </row>
-    <row r="23" spans="1:25" s="10" customFormat="1" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A23" s="14"/>
-      <c r="B23" s="14"/>
-      <c r="C23" s="18" t="s">
+    <row r="23" spans="1:25" s="10" customFormat="1" ht="20.45" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="11"/>
+      <c r="B23" s="11"/>
+      <c r="C23" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="D23" s="14" t="s">
+      <c r="D23" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="E23" s="17">
+      <c r="E23" s="14">
         <v>44867</v>
       </c>
-      <c r="F23" s="17">
+      <c r="F23" s="14">
         <v>44869</v>
       </c>
-      <c r="G23" s="17"/>
-      <c r="H23" s="17"/>
-      <c r="I23" s="14"/>
+      <c r="G23" s="14"/>
+      <c r="H23" s="14"/>
+      <c r="I23" s="11"/>
       <c r="J23" s="5"/>
       <c r="K23" s="5"/>
       <c r="L23" s="5"/>
@@ -1366,24 +1372,24 @@
       <c r="X23" s="5"/>
       <c r="Y23" s="5"/>
     </row>
-    <row r="24" spans="1:25" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="14"/>
-      <c r="B24" s="14"/>
-      <c r="C24" s="15" t="s">
+    <row r="24" spans="1:25" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="11"/>
+      <c r="B24" s="11"/>
+      <c r="C24" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="D24" s="14" t="s">
+      <c r="D24" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="E24" s="17">
+      <c r="E24" s="14">
         <v>44870</v>
       </c>
-      <c r="F24" s="17">
+      <c r="F24" s="14">
         <v>44873</v>
       </c>
-      <c r="G24" s="17"/>
-      <c r="H24" s="17"/>
-      <c r="I24" s="14"/>
+      <c r="G24" s="14"/>
+      <c r="H24" s="14"/>
+      <c r="I24" s="11"/>
       <c r="J24" s="5"/>
       <c r="K24" s="5"/>
       <c r="L24" s="5"/>
@@ -1401,24 +1407,24 @@
       <c r="X24" s="5"/>
       <c r="Y24" s="5"/>
     </row>
-    <row r="25" spans="1:25" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="14"/>
-      <c r="B25" s="14"/>
-      <c r="C25" s="15" t="s">
+    <row r="25" spans="1:25" ht="24.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="11"/>
+      <c r="B25" s="11"/>
+      <c r="C25" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="D25" s="14" t="s">
+      <c r="D25" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="E25" s="17">
+      <c r="E25" s="14">
         <v>44875</v>
       </c>
-      <c r="F25" s="17">
+      <c r="F25" s="14">
         <v>44880</v>
       </c>
-      <c r="G25" s="17"/>
-      <c r="H25" s="17"/>
-      <c r="I25" s="14"/>
+      <c r="G25" s="14"/>
+      <c r="H25" s="14"/>
+      <c r="I25" s="11"/>
       <c r="J25" s="5"/>
       <c r="K25" s="5"/>
       <c r="L25" s="5"/>
@@ -1436,26 +1442,26 @@
       <c r="X25" s="5"/>
       <c r="Y25" s="5"/>
     </row>
-    <row r="26" spans="1:25" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="14">
+    <row r="26" spans="1:25" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="11">
         <v>7</v>
       </c>
-      <c r="B26" s="15" t="s">
+      <c r="B26" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="C26" s="15"/>
-      <c r="D26" s="14" t="s">
+      <c r="C26" s="12"/>
+      <c r="D26" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="E26" s="17">
+      <c r="E26" s="14">
         <v>44881</v>
       </c>
-      <c r="F26" s="17">
+      <c r="F26" s="14">
         <v>44883</v>
       </c>
-      <c r="G26" s="17"/>
-      <c r="H26" s="17"/>
-      <c r="I26" s="14"/>
+      <c r="G26" s="14"/>
+      <c r="H26" s="14"/>
+      <c r="I26" s="11"/>
       <c r="J26" s="5"/>
       <c r="K26" s="5"/>
       <c r="L26" s="5"/>
@@ -1473,28 +1479,28 @@
       <c r="X26" s="5"/>
       <c r="Y26" s="5"/>
     </row>
-    <row r="27" spans="1:25" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="14">
+    <row r="27" spans="1:25" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="11">
         <v>8</v>
       </c>
-      <c r="B27" s="15" t="s">
+      <c r="B27" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="C27" s="15" t="s">
+      <c r="C27" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="D27" s="14" t="s">
+      <c r="D27" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="E27" s="17">
+      <c r="E27" s="14">
         <v>44884</v>
       </c>
-      <c r="F27" s="17">
+      <c r="F27" s="14">
         <v>44889</v>
       </c>
-      <c r="G27" s="17"/>
-      <c r="H27" s="17"/>
-      <c r="I27" s="14"/>
+      <c r="G27" s="14"/>
+      <c r="H27" s="14"/>
+      <c r="I27" s="11"/>
       <c r="J27" s="5"/>
       <c r="K27" s="5"/>
       <c r="L27" s="5"/>
@@ -1512,26 +1518,26 @@
       <c r="X27" s="5"/>
       <c r="Y27" s="5"/>
     </row>
-    <row r="28" spans="1:25" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="14">
+    <row r="28" spans="1:25" ht="26.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="11">
         <v>9</v>
       </c>
-      <c r="B28" s="15" t="s">
+      <c r="B28" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="C28" s="15"/>
-      <c r="D28" s="14" t="s">
+      <c r="C28" s="12"/>
+      <c r="D28" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="E28" s="17">
+      <c r="E28" s="14">
         <v>44890</v>
       </c>
-      <c r="F28" s="17">
+      <c r="F28" s="14">
         <v>44894</v>
       </c>
-      <c r="G28" s="17"/>
-      <c r="H28" s="17"/>
-      <c r="I28" s="14"/>
+      <c r="G28" s="14"/>
+      <c r="H28" s="14"/>
+      <c r="I28" s="11"/>
       <c r="J28" s="5"/>
       <c r="K28" s="5"/>
       <c r="L28" s="5"/>
@@ -1549,7 +1555,7 @@
       <c r="X28" s="5"/>
       <c r="Y28" s="5"/>
     </row>
-    <row r="29" spans="1:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="6"/>
       <c r="B29" s="6"/>
       <c r="C29" s="7"/>
@@ -1576,7 +1582,7 @@
       <c r="X29" s="5"/>
       <c r="Y29" s="5"/>
     </row>
-    <row r="30" spans="1:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="6"/>
       <c r="B30" s="6"/>
       <c r="C30" s="7"/>
@@ -1603,7 +1609,7 @@
       <c r="X30" s="5"/>
       <c r="Y30" s="5"/>
     </row>
-    <row r="31" spans="1:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="6"/>
       <c r="B31" s="6"/>
       <c r="C31" s="7"/>
@@ -1630,7 +1636,7 @@
       <c r="X31" s="5"/>
       <c r="Y31" s="5"/>
     </row>
-    <row r="32" spans="1:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="6"/>
       <c r="B32" s="9"/>
       <c r="C32" s="7"/>
@@ -1657,7 +1663,7 @@
       <c r="X32" s="5"/>
       <c r="Y32" s="5"/>
     </row>
-    <row r="33" spans="1:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="6"/>
       <c r="B33" s="6"/>
       <c r="C33" s="7"/>
@@ -1684,7 +1690,7 @@
       <c r="X33" s="5"/>
       <c r="Y33" s="5"/>
     </row>
-    <row r="34" spans="1:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="6"/>
       <c r="B34" s="6"/>
       <c r="C34" s="7"/>
@@ -1711,2911 +1717,2911 @@
       <c r="X34" s="5"/>
       <c r="Y34" s="5"/>
     </row>
-    <row r="35" spans="1:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C35" s="4"/>
     </row>
-    <row r="36" spans="1:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C36" s="4"/>
     </row>
-    <row r="37" spans="1:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C37" s="4"/>
     </row>
-    <row r="38" spans="1:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C38" s="4"/>
     </row>
-    <row r="39" spans="1:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C39" s="4"/>
     </row>
-    <row r="40" spans="1:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C40" s="4"/>
     </row>
-    <row r="41" spans="1:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C41" s="4"/>
     </row>
-    <row r="42" spans="1:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C42" s="4"/>
     </row>
-    <row r="43" spans="1:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C43" s="4"/>
     </row>
-    <row r="44" spans="1:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C44" s="4"/>
     </row>
-    <row r="45" spans="1:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C45" s="4"/>
     </row>
-    <row r="46" spans="1:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C46" s="4"/>
     </row>
-    <row r="47" spans="1:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C47" s="4"/>
     </row>
-    <row r="48" spans="1:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C48" s="4"/>
     </row>
-    <row r="49" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C49" s="4"/>
     </row>
-    <row r="50" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C50" s="4"/>
     </row>
-    <row r="51" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C51" s="4"/>
     </row>
-    <row r="52" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C52" s="4"/>
     </row>
-    <row r="53" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C53" s="4"/>
     </row>
-    <row r="54" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C54" s="4"/>
     </row>
-    <row r="55" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C55" s="4"/>
     </row>
-    <row r="56" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C56" s="4"/>
     </row>
-    <row r="57" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C57" s="4"/>
     </row>
-    <row r="58" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C58" s="4"/>
     </row>
-    <row r="59" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C59" s="4"/>
     </row>
-    <row r="60" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C60" s="4"/>
     </row>
-    <row r="61" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C61" s="4"/>
     </row>
-    <row r="62" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C62" s="4"/>
     </row>
-    <row r="63" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C63" s="4"/>
     </row>
-    <row r="64" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C64" s="4"/>
     </row>
-    <row r="65" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C65" s="4"/>
     </row>
-    <row r="66" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C66" s="4"/>
     </row>
-    <row r="67" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="67" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C67" s="4"/>
     </row>
-    <row r="68" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="68" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C68" s="4"/>
     </row>
-    <row r="69" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="69" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C69" s="4"/>
     </row>
-    <row r="70" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="70" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C70" s="4"/>
     </row>
-    <row r="71" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="71" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C71" s="4"/>
     </row>
-    <row r="72" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="72" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C72" s="4"/>
     </row>
-    <row r="73" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="73" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C73" s="4"/>
     </row>
-    <row r="74" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="74" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C74" s="4"/>
     </row>
-    <row r="75" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="75" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C75" s="4"/>
     </row>
-    <row r="76" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="76" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C76" s="4"/>
     </row>
-    <row r="77" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="77" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C77" s="4"/>
     </row>
-    <row r="78" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="78" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C78" s="4"/>
     </row>
-    <row r="79" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="79" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C79" s="4"/>
     </row>
-    <row r="80" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="80" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C80" s="4"/>
     </row>
-    <row r="81" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="81" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C81" s="4"/>
     </row>
-    <row r="82" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="82" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C82" s="4"/>
     </row>
-    <row r="83" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="83" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C83" s="4"/>
     </row>
-    <row r="84" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="84" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C84" s="4"/>
     </row>
-    <row r="85" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="85" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C85" s="4"/>
     </row>
-    <row r="86" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="86" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C86" s="4"/>
     </row>
-    <row r="87" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="87" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C87" s="4"/>
     </row>
-    <row r="88" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="88" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C88" s="4"/>
     </row>
-    <row r="89" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="89" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C89" s="4"/>
     </row>
-    <row r="90" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="90" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C90" s="4"/>
     </row>
-    <row r="91" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="91" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C91" s="4"/>
     </row>
-    <row r="92" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="92" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C92" s="4"/>
     </row>
-    <row r="93" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="93" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C93" s="4"/>
     </row>
-    <row r="94" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="94" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C94" s="4"/>
     </row>
-    <row r="95" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="95" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C95" s="4"/>
     </row>
-    <row r="96" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="96" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C96" s="4"/>
     </row>
-    <row r="97" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="97" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C97" s="4"/>
     </row>
-    <row r="98" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="98" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C98" s="4"/>
     </row>
-    <row r="99" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="99" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C99" s="4"/>
     </row>
-    <row r="100" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="100" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C100" s="4"/>
     </row>
-    <row r="101" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="101" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C101" s="4"/>
     </row>
-    <row r="102" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="102" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C102" s="4"/>
     </row>
-    <row r="103" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="103" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C103" s="4"/>
     </row>
-    <row r="104" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="104" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C104" s="4"/>
     </row>
-    <row r="105" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="105" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C105" s="4"/>
     </row>
-    <row r="106" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="106" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C106" s="4"/>
     </row>
-    <row r="107" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="107" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C107" s="4"/>
     </row>
-    <row r="108" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="108" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C108" s="4"/>
     </row>
-    <row r="109" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="109" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C109" s="4"/>
     </row>
-    <row r="110" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="110" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C110" s="4"/>
     </row>
-    <row r="111" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="111" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C111" s="4"/>
     </row>
-    <row r="112" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="112" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C112" s="4"/>
     </row>
-    <row r="113" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="113" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C113" s="4"/>
     </row>
-    <row r="114" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="114" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C114" s="4"/>
     </row>
-    <row r="115" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="115" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C115" s="4"/>
     </row>
-    <row r="116" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="116" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C116" s="4"/>
     </row>
-    <row r="117" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="117" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C117" s="4"/>
     </row>
-    <row r="118" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="118" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C118" s="4"/>
     </row>
-    <row r="119" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="119" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C119" s="4"/>
     </row>
-    <row r="120" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="120" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C120" s="4"/>
     </row>
-    <row r="121" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="121" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C121" s="4"/>
     </row>
-    <row r="122" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="122" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C122" s="4"/>
     </row>
-    <row r="123" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="123" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C123" s="4"/>
     </row>
-    <row r="124" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="124" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C124" s="4"/>
     </row>
-    <row r="125" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="125" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C125" s="4"/>
     </row>
-    <row r="126" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="126" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C126" s="4"/>
     </row>
-    <row r="127" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="127" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C127" s="4"/>
     </row>
-    <row r="128" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="128" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C128" s="4"/>
     </row>
-    <row r="129" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="129" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C129" s="4"/>
     </row>
-    <row r="130" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="130" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C130" s="4"/>
     </row>
-    <row r="131" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="131" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C131" s="4"/>
     </row>
-    <row r="132" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="132" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C132" s="4"/>
     </row>
-    <row r="133" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="133" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C133" s="4"/>
     </row>
-    <row r="134" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="134" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C134" s="4"/>
     </row>
-    <row r="135" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="135" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C135" s="4"/>
     </row>
-    <row r="136" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="136" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C136" s="4"/>
     </row>
-    <row r="137" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="137" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C137" s="4"/>
     </row>
-    <row r="138" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="138" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C138" s="4"/>
     </row>
-    <row r="139" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="139" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C139" s="4"/>
     </row>
-    <row r="140" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="140" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C140" s="4"/>
     </row>
-    <row r="141" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="141" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C141" s="4"/>
     </row>
-    <row r="142" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="142" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C142" s="4"/>
     </row>
-    <row r="143" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="143" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C143" s="4"/>
     </row>
-    <row r="144" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="144" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C144" s="4"/>
     </row>
-    <row r="145" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="145" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C145" s="4"/>
     </row>
-    <row r="146" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="146" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C146" s="4"/>
     </row>
-    <row r="147" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="147" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C147" s="4"/>
     </row>
-    <row r="148" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="148" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C148" s="4"/>
     </row>
-    <row r="149" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="149" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C149" s="4"/>
     </row>
-    <row r="150" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="150" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C150" s="4"/>
     </row>
-    <row r="151" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="151" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C151" s="4"/>
     </row>
-    <row r="152" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="152" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C152" s="4"/>
     </row>
-    <row r="153" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="153" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C153" s="4"/>
     </row>
-    <row r="154" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="154" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C154" s="4"/>
     </row>
-    <row r="155" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="155" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C155" s="4"/>
     </row>
-    <row r="156" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="156" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C156" s="4"/>
     </row>
-    <row r="157" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="157" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C157" s="4"/>
     </row>
-    <row r="158" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="158" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C158" s="4"/>
     </row>
-    <row r="159" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="159" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C159" s="4"/>
     </row>
-    <row r="160" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="160" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C160" s="4"/>
     </row>
-    <row r="161" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="161" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C161" s="4"/>
     </row>
-    <row r="162" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="162" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C162" s="4"/>
     </row>
-    <row r="163" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="163" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C163" s="4"/>
     </row>
-    <row r="164" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="164" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C164" s="4"/>
     </row>
-    <row r="165" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="165" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C165" s="4"/>
     </row>
-    <row r="166" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="166" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C166" s="4"/>
     </row>
-    <row r="167" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="167" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C167" s="4"/>
     </row>
-    <row r="168" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="168" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C168" s="4"/>
     </row>
-    <row r="169" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="169" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C169" s="4"/>
     </row>
-    <row r="170" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="170" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C170" s="4"/>
     </row>
-    <row r="171" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="171" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C171" s="4"/>
     </row>
-    <row r="172" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="172" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C172" s="4"/>
     </row>
-    <row r="173" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="173" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C173" s="4"/>
     </row>
-    <row r="174" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="174" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C174" s="4"/>
     </row>
-    <row r="175" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="175" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C175" s="4"/>
     </row>
-    <row r="176" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="176" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C176" s="4"/>
     </row>
-    <row r="177" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="177" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C177" s="4"/>
     </row>
-    <row r="178" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="178" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C178" s="4"/>
     </row>
-    <row r="179" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="179" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C179" s="4"/>
     </row>
-    <row r="180" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="180" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C180" s="4"/>
     </row>
-    <row r="181" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="181" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C181" s="4"/>
     </row>
-    <row r="182" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="182" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C182" s="4"/>
     </row>
-    <row r="183" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="183" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C183" s="4"/>
     </row>
-    <row r="184" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="184" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C184" s="4"/>
     </row>
-    <row r="185" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="185" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C185" s="4"/>
     </row>
-    <row r="186" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="186" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C186" s="4"/>
     </row>
-    <row r="187" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="187" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C187" s="4"/>
     </row>
-    <row r="188" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="188" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C188" s="4"/>
     </row>
-    <row r="189" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="189" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C189" s="4"/>
     </row>
-    <row r="190" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="190" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C190" s="4"/>
     </row>
-    <row r="191" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="191" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C191" s="4"/>
     </row>
-    <row r="192" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="192" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C192" s="4"/>
     </row>
-    <row r="193" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="193" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C193" s="4"/>
     </row>
-    <row r="194" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="194" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C194" s="4"/>
     </row>
-    <row r="195" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="195" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C195" s="4"/>
     </row>
-    <row r="196" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="196" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C196" s="4"/>
     </row>
-    <row r="197" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="197" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C197" s="4"/>
     </row>
-    <row r="198" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="198" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C198" s="4"/>
     </row>
-    <row r="199" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="199" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C199" s="4"/>
     </row>
-    <row r="200" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="200" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C200" s="4"/>
     </row>
-    <row r="201" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="201" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C201" s="4"/>
     </row>
-    <row r="202" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="202" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C202" s="4"/>
     </row>
-    <row r="203" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="203" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C203" s="4"/>
     </row>
-    <row r="204" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="204" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C204" s="4"/>
     </row>
-    <row r="205" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="205" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C205" s="4"/>
     </row>
-    <row r="206" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="206" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C206" s="4"/>
     </row>
-    <row r="207" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="207" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C207" s="4"/>
     </row>
-    <row r="208" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="208" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C208" s="4"/>
     </row>
-    <row r="209" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="209" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C209" s="4"/>
     </row>
-    <row r="210" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="210" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C210" s="4"/>
     </row>
-    <row r="211" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="211" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C211" s="4"/>
     </row>
-    <row r="212" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="212" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C212" s="4"/>
     </row>
-    <row r="213" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="213" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C213" s="4"/>
     </row>
-    <row r="214" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="214" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C214" s="4"/>
     </row>
-    <row r="215" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="215" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C215" s="4"/>
     </row>
-    <row r="216" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="216" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C216" s="4"/>
     </row>
-    <row r="217" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="217" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C217" s="4"/>
     </row>
-    <row r="218" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="218" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C218" s="4"/>
     </row>
-    <row r="219" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="219" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C219" s="4"/>
     </row>
-    <row r="220" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="220" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C220" s="4"/>
     </row>
-    <row r="221" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="221" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C221" s="4"/>
     </row>
-    <row r="222" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="222" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C222" s="4"/>
     </row>
-    <row r="223" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="223" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C223" s="4"/>
     </row>
-    <row r="224" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="224" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C224" s="4"/>
     </row>
-    <row r="225" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="225" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C225" s="4"/>
     </row>
-    <row r="226" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="226" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C226" s="4"/>
     </row>
-    <row r="227" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="227" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C227" s="4"/>
     </row>
-    <row r="228" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="228" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C228" s="4"/>
     </row>
-    <row r="229" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="229" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C229" s="4"/>
     </row>
-    <row r="230" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="230" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C230" s="4"/>
     </row>
-    <row r="231" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="231" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C231" s="4"/>
     </row>
-    <row r="232" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="232" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C232" s="4"/>
     </row>
-    <row r="233" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="233" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C233" s="4"/>
     </row>
-    <row r="234" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="234" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C234" s="4"/>
     </row>
-    <row r="235" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="235" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C235" s="4"/>
     </row>
-    <row r="236" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="236" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C236" s="4"/>
     </row>
-    <row r="237" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="237" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C237" s="4"/>
     </row>
-    <row r="238" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="238" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C238" s="4"/>
     </row>
-    <row r="239" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="239" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C239" s="4"/>
     </row>
-    <row r="240" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="240" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C240" s="4"/>
     </row>
-    <row r="241" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="241" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C241" s="4"/>
     </row>
-    <row r="242" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="242" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C242" s="4"/>
     </row>
-    <row r="243" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="243" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C243" s="4"/>
     </row>
-    <row r="244" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="244" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C244" s="4"/>
     </row>
-    <row r="245" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="245" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C245" s="4"/>
     </row>
-    <row r="246" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="246" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C246" s="4"/>
     </row>
-    <row r="247" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="247" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C247" s="4"/>
     </row>
-    <row r="248" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="248" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C248" s="4"/>
     </row>
-    <row r="249" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="249" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C249" s="4"/>
     </row>
-    <row r="250" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="250" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C250" s="4"/>
     </row>
-    <row r="251" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="251" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C251" s="4"/>
     </row>
-    <row r="252" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="252" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C252" s="4"/>
     </row>
-    <row r="253" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="253" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C253" s="4"/>
     </row>
-    <row r="254" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="254" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C254" s="4"/>
     </row>
-    <row r="255" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="255" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C255" s="4"/>
     </row>
-    <row r="256" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="256" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C256" s="4"/>
     </row>
-    <row r="257" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="257" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C257" s="4"/>
     </row>
-    <row r="258" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="258" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C258" s="4"/>
     </row>
-    <row r="259" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="259" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C259" s="4"/>
     </row>
-    <row r="260" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="260" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C260" s="4"/>
     </row>
-    <row r="261" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="261" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C261" s="4"/>
     </row>
-    <row r="262" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="262" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C262" s="4"/>
     </row>
-    <row r="263" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="263" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C263" s="4"/>
     </row>
-    <row r="264" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="264" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C264" s="4"/>
     </row>
-    <row r="265" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="265" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C265" s="4"/>
     </row>
-    <row r="266" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="266" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C266" s="4"/>
     </row>
-    <row r="267" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="267" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C267" s="4"/>
     </row>
-    <row r="268" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="268" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C268" s="4"/>
     </row>
-    <row r="269" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="269" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C269" s="4"/>
     </row>
-    <row r="270" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="270" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C270" s="4"/>
     </row>
-    <row r="271" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="271" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C271" s="4"/>
     </row>
-    <row r="272" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="272" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C272" s="4"/>
     </row>
-    <row r="273" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="273" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C273" s="4"/>
     </row>
-    <row r="274" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="274" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C274" s="4"/>
     </row>
-    <row r="275" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="275" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C275" s="4"/>
     </row>
-    <row r="276" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="276" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C276" s="4"/>
     </row>
-    <row r="277" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="277" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C277" s="4"/>
     </row>
-    <row r="278" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="278" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C278" s="4"/>
     </row>
-    <row r="279" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="279" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C279" s="4"/>
     </row>
-    <row r="280" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="280" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C280" s="4"/>
     </row>
-    <row r="281" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="281" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C281" s="4"/>
     </row>
-    <row r="282" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="282" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C282" s="4"/>
     </row>
-    <row r="283" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="283" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C283" s="4"/>
     </row>
-    <row r="284" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="284" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C284" s="4"/>
     </row>
-    <row r="285" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="285" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C285" s="4"/>
     </row>
-    <row r="286" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="286" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C286" s="4"/>
     </row>
-    <row r="287" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="287" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C287" s="4"/>
     </row>
-    <row r="288" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="288" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C288" s="4"/>
     </row>
-    <row r="289" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="289" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C289" s="4"/>
     </row>
-    <row r="290" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="290" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C290" s="4"/>
     </row>
-    <row r="291" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="291" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C291" s="4"/>
     </row>
-    <row r="292" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="292" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C292" s="4"/>
     </row>
-    <row r="293" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="293" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C293" s="4"/>
     </row>
-    <row r="294" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="294" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C294" s="4"/>
     </row>
-    <row r="295" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="295" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C295" s="4"/>
     </row>
-    <row r="296" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="296" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C296" s="4"/>
     </row>
-    <row r="297" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="297" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C297" s="4"/>
     </row>
-    <row r="298" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="298" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C298" s="4"/>
     </row>
-    <row r="299" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="299" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C299" s="4"/>
     </row>
-    <row r="300" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="300" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C300" s="4"/>
     </row>
-    <row r="301" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="301" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C301" s="4"/>
     </row>
-    <row r="302" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="302" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C302" s="4"/>
     </row>
-    <row r="303" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="303" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C303" s="4"/>
     </row>
-    <row r="304" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="304" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C304" s="4"/>
     </row>
-    <row r="305" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="305" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C305" s="4"/>
     </row>
-    <row r="306" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="306" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C306" s="4"/>
     </row>
-    <row r="307" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="307" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C307" s="4"/>
     </row>
-    <row r="308" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="308" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C308" s="4"/>
     </row>
-    <row r="309" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="309" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C309" s="4"/>
     </row>
-    <row r="310" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="310" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C310" s="4"/>
     </row>
-    <row r="311" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="311" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C311" s="4"/>
     </row>
-    <row r="312" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="312" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C312" s="4"/>
     </row>
-    <row r="313" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="313" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C313" s="4"/>
     </row>
-    <row r="314" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="314" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C314" s="4"/>
     </row>
-    <row r="315" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="315" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C315" s="4"/>
     </row>
-    <row r="316" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="316" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C316" s="4"/>
     </row>
-    <row r="317" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="317" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C317" s="4"/>
     </row>
-    <row r="318" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="318" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C318" s="4"/>
     </row>
-    <row r="319" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="319" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C319" s="4"/>
     </row>
-    <row r="320" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="320" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C320" s="4"/>
     </row>
-    <row r="321" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="321" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C321" s="4"/>
     </row>
-    <row r="322" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="322" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C322" s="4"/>
     </row>
-    <row r="323" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="323" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C323" s="4"/>
     </row>
-    <row r="324" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="324" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C324" s="4"/>
     </row>
-    <row r="325" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="325" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C325" s="4"/>
     </row>
-    <row r="326" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="326" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C326" s="4"/>
     </row>
-    <row r="327" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="327" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C327" s="4"/>
     </row>
-    <row r="328" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="328" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C328" s="4"/>
     </row>
-    <row r="329" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="329" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C329" s="4"/>
     </row>
-    <row r="330" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="330" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C330" s="4"/>
     </row>
-    <row r="331" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="331" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C331" s="4"/>
     </row>
-    <row r="332" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="332" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C332" s="4"/>
     </row>
-    <row r="333" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="333" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C333" s="4"/>
     </row>
-    <row r="334" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="334" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C334" s="4"/>
     </row>
-    <row r="335" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="335" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C335" s="4"/>
     </row>
-    <row r="336" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="336" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C336" s="4"/>
     </row>
-    <row r="337" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="337" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C337" s="4"/>
     </row>
-    <row r="338" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="338" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C338" s="4"/>
     </row>
-    <row r="339" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="339" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C339" s="4"/>
     </row>
-    <row r="340" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="340" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C340" s="4"/>
     </row>
-    <row r="341" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="341" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C341" s="4"/>
     </row>
-    <row r="342" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="342" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C342" s="4"/>
     </row>
-    <row r="343" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="343" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C343" s="4"/>
     </row>
-    <row r="344" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="344" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C344" s="4"/>
     </row>
-    <row r="345" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="345" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C345" s="4"/>
     </row>
-    <row r="346" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="346" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C346" s="4"/>
     </row>
-    <row r="347" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="347" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C347" s="4"/>
     </row>
-    <row r="348" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="348" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C348" s="4"/>
     </row>
-    <row r="349" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="349" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C349" s="4"/>
     </row>
-    <row r="350" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="350" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C350" s="4"/>
     </row>
-    <row r="351" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="351" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C351" s="4"/>
     </row>
-    <row r="352" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="352" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C352" s="4"/>
     </row>
-    <row r="353" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="353" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C353" s="4"/>
     </row>
-    <row r="354" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="354" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C354" s="4"/>
     </row>
-    <row r="355" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="355" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C355" s="4"/>
     </row>
-    <row r="356" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="356" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C356" s="4"/>
     </row>
-    <row r="357" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="357" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C357" s="4"/>
     </row>
-    <row r="358" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="358" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C358" s="4"/>
     </row>
-    <row r="359" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="359" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C359" s="4"/>
     </row>
-    <row r="360" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="360" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C360" s="4"/>
     </row>
-    <row r="361" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="361" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C361" s="4"/>
     </row>
-    <row r="362" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="362" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C362" s="4"/>
     </row>
-    <row r="363" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="363" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C363" s="4"/>
     </row>
-    <row r="364" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="364" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C364" s="4"/>
     </row>
-    <row r="365" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="365" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C365" s="4"/>
     </row>
-    <row r="366" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="366" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C366" s="4"/>
     </row>
-    <row r="367" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="367" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C367" s="4"/>
     </row>
-    <row r="368" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="368" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C368" s="4"/>
     </row>
-    <row r="369" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="369" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C369" s="4"/>
     </row>
-    <row r="370" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="370" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C370" s="4"/>
     </row>
-    <row r="371" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="371" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C371" s="4"/>
     </row>
-    <row r="372" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="372" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C372" s="4"/>
     </row>
-    <row r="373" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="373" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C373" s="4"/>
     </row>
-    <row r="374" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="374" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C374" s="4"/>
     </row>
-    <row r="375" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="375" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C375" s="4"/>
     </row>
-    <row r="376" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="376" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C376" s="4"/>
     </row>
-    <row r="377" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="377" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C377" s="4"/>
     </row>
-    <row r="378" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="378" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C378" s="4"/>
     </row>
-    <row r="379" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="379" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C379" s="4"/>
     </row>
-    <row r="380" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="380" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C380" s="4"/>
     </row>
-    <row r="381" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="381" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C381" s="4"/>
     </row>
-    <row r="382" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="382" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C382" s="4"/>
     </row>
-    <row r="383" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="383" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C383" s="4"/>
     </row>
-    <row r="384" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="384" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C384" s="4"/>
     </row>
-    <row r="385" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="385" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C385" s="4"/>
     </row>
-    <row r="386" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="386" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C386" s="4"/>
     </row>
-    <row r="387" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="387" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C387" s="4"/>
     </row>
-    <row r="388" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="388" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C388" s="4"/>
     </row>
-    <row r="389" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="389" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C389" s="4"/>
     </row>
-    <row r="390" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="390" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C390" s="4"/>
     </row>
-    <row r="391" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="391" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C391" s="4"/>
     </row>
-    <row r="392" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="392" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C392" s="4"/>
     </row>
-    <row r="393" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="393" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C393" s="4"/>
     </row>
-    <row r="394" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="394" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C394" s="4"/>
     </row>
-    <row r="395" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="395" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C395" s="4"/>
     </row>
-    <row r="396" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="396" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C396" s="4"/>
     </row>
-    <row r="397" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="397" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C397" s="4"/>
     </row>
-    <row r="398" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="398" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C398" s="4"/>
     </row>
-    <row r="399" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="399" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C399" s="4"/>
     </row>
-    <row r="400" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="400" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C400" s="4"/>
     </row>
-    <row r="401" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="401" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C401" s="4"/>
     </row>
-    <row r="402" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="402" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C402" s="4"/>
     </row>
-    <row r="403" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="403" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C403" s="4"/>
     </row>
-    <row r="404" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="404" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C404" s="4"/>
     </row>
-    <row r="405" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="405" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C405" s="4"/>
     </row>
-    <row r="406" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="406" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C406" s="4"/>
     </row>
-    <row r="407" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="407" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C407" s="4"/>
     </row>
-    <row r="408" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="408" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C408" s="4"/>
     </row>
-    <row r="409" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="409" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C409" s="4"/>
     </row>
-    <row r="410" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="410" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C410" s="4"/>
     </row>
-    <row r="411" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="411" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C411" s="4"/>
     </row>
-    <row r="412" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="412" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C412" s="4"/>
     </row>
-    <row r="413" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="413" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C413" s="4"/>
     </row>
-    <row r="414" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="414" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C414" s="4"/>
     </row>
-    <row r="415" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="415" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C415" s="4"/>
     </row>
-    <row r="416" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="416" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C416" s="4"/>
     </row>
-    <row r="417" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="417" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C417" s="4"/>
     </row>
-    <row r="418" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="418" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C418" s="4"/>
     </row>
-    <row r="419" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="419" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C419" s="4"/>
     </row>
-    <row r="420" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="420" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C420" s="4"/>
     </row>
-    <row r="421" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="421" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C421" s="4"/>
     </row>
-    <row r="422" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="422" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C422" s="4"/>
     </row>
-    <row r="423" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="423" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C423" s="4"/>
     </row>
-    <row r="424" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="424" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C424" s="4"/>
     </row>
-    <row r="425" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="425" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C425" s="4"/>
     </row>
-    <row r="426" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="426" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C426" s="4"/>
     </row>
-    <row r="427" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="427" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C427" s="4"/>
     </row>
-    <row r="428" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="428" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C428" s="4"/>
     </row>
-    <row r="429" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="429" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C429" s="4"/>
     </row>
-    <row r="430" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="430" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C430" s="4"/>
     </row>
-    <row r="431" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="431" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C431" s="4"/>
     </row>
-    <row r="432" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="432" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C432" s="4"/>
     </row>
-    <row r="433" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="433" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C433" s="4"/>
     </row>
-    <row r="434" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="434" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C434" s="4"/>
     </row>
-    <row r="435" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="435" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C435" s="4"/>
     </row>
-    <row r="436" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="436" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C436" s="4"/>
     </row>
-    <row r="437" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="437" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C437" s="4"/>
     </row>
-    <row r="438" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="438" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C438" s="4"/>
     </row>
-    <row r="439" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="439" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C439" s="4"/>
     </row>
-    <row r="440" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="440" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C440" s="4"/>
     </row>
-    <row r="441" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="441" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C441" s="4"/>
     </row>
-    <row r="442" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="442" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C442" s="4"/>
     </row>
-    <row r="443" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="443" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C443" s="4"/>
     </row>
-    <row r="444" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="444" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C444" s="4"/>
     </row>
-    <row r="445" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="445" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C445" s="4"/>
     </row>
-    <row r="446" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="446" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C446" s="4"/>
     </row>
-    <row r="447" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="447" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C447" s="4"/>
     </row>
-    <row r="448" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="448" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C448" s="4"/>
     </row>
-    <row r="449" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="449" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C449" s="4"/>
     </row>
-    <row r="450" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="450" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C450" s="4"/>
     </row>
-    <row r="451" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="451" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C451" s="4"/>
     </row>
-    <row r="452" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="452" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C452" s="4"/>
     </row>
-    <row r="453" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="453" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C453" s="4"/>
     </row>
-    <row r="454" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="454" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C454" s="4"/>
     </row>
-    <row r="455" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="455" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C455" s="4"/>
     </row>
-    <row r="456" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="456" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C456" s="4"/>
     </row>
-    <row r="457" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="457" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C457" s="4"/>
     </row>
-    <row r="458" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="458" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C458" s="4"/>
     </row>
-    <row r="459" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="459" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C459" s="4"/>
     </row>
-    <row r="460" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="460" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C460" s="4"/>
     </row>
-    <row r="461" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="461" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C461" s="4"/>
     </row>
-    <row r="462" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="462" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C462" s="4"/>
     </row>
-    <row r="463" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="463" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C463" s="4"/>
     </row>
-    <row r="464" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="464" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C464" s="4"/>
     </row>
-    <row r="465" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="465" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C465" s="4"/>
     </row>
-    <row r="466" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="466" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C466" s="4"/>
     </row>
-    <row r="467" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="467" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C467" s="4"/>
     </row>
-    <row r="468" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="468" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C468" s="4"/>
     </row>
-    <row r="469" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="469" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C469" s="4"/>
     </row>
-    <row r="470" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="470" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C470" s="4"/>
     </row>
-    <row r="471" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="471" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C471" s="4"/>
     </row>
-    <row r="472" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="472" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C472" s="4"/>
     </row>
-    <row r="473" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="473" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C473" s="4"/>
     </row>
-    <row r="474" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="474" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C474" s="4"/>
     </row>
-    <row r="475" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="475" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C475" s="4"/>
     </row>
-    <row r="476" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="476" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C476" s="4"/>
     </row>
-    <row r="477" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="477" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C477" s="4"/>
     </row>
-    <row r="478" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="478" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C478" s="4"/>
     </row>
-    <row r="479" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="479" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C479" s="4"/>
     </row>
-    <row r="480" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="480" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C480" s="4"/>
     </row>
-    <row r="481" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="481" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C481" s="4"/>
     </row>
-    <row r="482" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="482" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C482" s="4"/>
     </row>
-    <row r="483" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="483" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C483" s="4"/>
     </row>
-    <row r="484" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="484" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C484" s="4"/>
     </row>
-    <row r="485" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="485" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C485" s="4"/>
     </row>
-    <row r="486" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="486" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C486" s="4"/>
     </row>
-    <row r="487" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="487" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C487" s="4"/>
     </row>
-    <row r="488" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="488" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C488" s="4"/>
     </row>
-    <row r="489" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="489" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C489" s="4"/>
     </row>
-    <row r="490" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="490" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C490" s="4"/>
     </row>
-    <row r="491" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="491" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C491" s="4"/>
     </row>
-    <row r="492" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="492" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C492" s="4"/>
     </row>
-    <row r="493" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="493" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C493" s="4"/>
     </row>
-    <row r="494" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="494" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C494" s="4"/>
     </row>
-    <row r="495" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="495" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C495" s="4"/>
     </row>
-    <row r="496" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="496" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C496" s="4"/>
     </row>
-    <row r="497" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="497" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C497" s="4"/>
     </row>
-    <row r="498" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="498" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C498" s="4"/>
     </row>
-    <row r="499" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="499" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C499" s="4"/>
     </row>
-    <row r="500" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="500" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C500" s="4"/>
     </row>
-    <row r="501" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="501" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C501" s="4"/>
     </row>
-    <row r="502" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="502" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C502" s="4"/>
     </row>
-    <row r="503" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="503" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C503" s="4"/>
     </row>
-    <row r="504" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="504" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C504" s="4"/>
     </row>
-    <row r="505" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="505" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C505" s="4"/>
     </row>
-    <row r="506" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="506" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C506" s="4"/>
     </row>
-    <row r="507" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="507" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C507" s="4"/>
     </row>
-    <row r="508" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="508" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C508" s="4"/>
     </row>
-    <row r="509" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="509" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C509" s="4"/>
     </row>
-    <row r="510" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="510" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C510" s="4"/>
     </row>
-    <row r="511" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="511" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C511" s="4"/>
     </row>
-    <row r="512" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="512" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C512" s="4"/>
     </row>
-    <row r="513" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="513" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C513" s="4"/>
     </row>
-    <row r="514" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="514" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C514" s="4"/>
     </row>
-    <row r="515" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="515" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C515" s="4"/>
     </row>
-    <row r="516" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="516" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C516" s="4"/>
     </row>
-    <row r="517" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="517" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C517" s="4"/>
     </row>
-    <row r="518" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="518" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C518" s="4"/>
     </row>
-    <row r="519" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="519" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C519" s="4"/>
     </row>
-    <row r="520" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="520" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C520" s="4"/>
     </row>
-    <row r="521" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="521" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C521" s="4"/>
     </row>
-    <row r="522" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="522" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C522" s="4"/>
     </row>
-    <row r="523" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="523" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C523" s="4"/>
     </row>
-    <row r="524" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="524" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C524" s="4"/>
     </row>
-    <row r="525" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="525" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C525" s="4"/>
     </row>
-    <row r="526" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="526" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C526" s="4"/>
     </row>
-    <row r="527" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="527" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C527" s="4"/>
     </row>
-    <row r="528" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="528" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C528" s="4"/>
     </row>
-    <row r="529" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="529" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C529" s="4"/>
     </row>
-    <row r="530" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="530" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C530" s="4"/>
     </row>
-    <row r="531" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="531" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C531" s="4"/>
     </row>
-    <row r="532" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="532" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C532" s="4"/>
     </row>
-    <row r="533" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="533" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C533" s="4"/>
     </row>
-    <row r="534" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="534" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C534" s="4"/>
     </row>
-    <row r="535" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="535" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C535" s="4"/>
     </row>
-    <row r="536" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="536" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C536" s="4"/>
     </row>
-    <row r="537" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="537" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C537" s="4"/>
     </row>
-    <row r="538" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="538" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C538" s="4"/>
     </row>
-    <row r="539" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="539" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C539" s="4"/>
     </row>
-    <row r="540" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="540" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C540" s="4"/>
     </row>
-    <row r="541" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="541" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C541" s="4"/>
     </row>
-    <row r="542" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="542" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C542" s="4"/>
     </row>
-    <row r="543" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="543" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C543" s="4"/>
     </row>
-    <row r="544" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="544" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C544" s="4"/>
     </row>
-    <row r="545" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="545" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C545" s="4"/>
     </row>
-    <row r="546" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="546" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C546" s="4"/>
     </row>
-    <row r="547" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="547" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C547" s="4"/>
     </row>
-    <row r="548" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="548" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C548" s="4"/>
     </row>
-    <row r="549" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="549" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C549" s="4"/>
     </row>
-    <row r="550" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="550" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C550" s="4"/>
     </row>
-    <row r="551" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="551" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C551" s="4"/>
     </row>
-    <row r="552" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="552" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C552" s="4"/>
     </row>
-    <row r="553" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="553" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C553" s="4"/>
     </row>
-    <row r="554" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="554" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C554" s="4"/>
     </row>
-    <row r="555" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="555" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C555" s="4"/>
     </row>
-    <row r="556" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="556" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C556" s="4"/>
     </row>
-    <row r="557" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="557" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C557" s="4"/>
     </row>
-    <row r="558" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="558" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C558" s="4"/>
     </row>
-    <row r="559" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="559" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C559" s="4"/>
     </row>
-    <row r="560" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="560" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C560" s="4"/>
     </row>
-    <row r="561" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="561" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C561" s="4"/>
     </row>
-    <row r="562" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="562" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C562" s="4"/>
     </row>
-    <row r="563" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="563" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C563" s="4"/>
     </row>
-    <row r="564" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="564" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C564" s="4"/>
     </row>
-    <row r="565" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="565" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C565" s="4"/>
     </row>
-    <row r="566" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="566" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C566" s="4"/>
     </row>
-    <row r="567" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="567" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C567" s="4"/>
     </row>
-    <row r="568" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="568" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C568" s="4"/>
     </row>
-    <row r="569" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="569" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C569" s="4"/>
     </row>
-    <row r="570" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="570" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C570" s="4"/>
     </row>
-    <row r="571" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="571" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C571" s="4"/>
     </row>
-    <row r="572" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="572" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C572" s="4"/>
     </row>
-    <row r="573" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="573" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C573" s="4"/>
     </row>
-    <row r="574" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="574" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C574" s="4"/>
     </row>
-    <row r="575" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="575" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C575" s="4"/>
     </row>
-    <row r="576" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="576" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C576" s="4"/>
     </row>
-    <row r="577" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="577" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C577" s="4"/>
     </row>
-    <row r="578" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="578" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C578" s="4"/>
     </row>
-    <row r="579" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="579" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C579" s="4"/>
     </row>
-    <row r="580" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="580" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C580" s="4"/>
     </row>
-    <row r="581" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="581" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C581" s="4"/>
     </row>
-    <row r="582" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="582" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C582" s="4"/>
     </row>
-    <row r="583" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="583" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C583" s="4"/>
     </row>
-    <row r="584" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="584" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C584" s="4"/>
     </row>
-    <row r="585" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="585" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C585" s="4"/>
     </row>
-    <row r="586" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="586" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C586" s="4"/>
     </row>
-    <row r="587" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="587" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C587" s="4"/>
     </row>
-    <row r="588" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="588" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C588" s="4"/>
     </row>
-    <row r="589" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="589" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C589" s="4"/>
     </row>
-    <row r="590" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="590" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C590" s="4"/>
     </row>
-    <row r="591" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="591" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C591" s="4"/>
     </row>
-    <row r="592" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="592" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C592" s="4"/>
     </row>
-    <row r="593" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="593" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C593" s="4"/>
     </row>
-    <row r="594" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="594" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C594" s="4"/>
     </row>
-    <row r="595" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="595" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C595" s="4"/>
     </row>
-    <row r="596" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="596" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C596" s="4"/>
     </row>
-    <row r="597" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="597" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C597" s="4"/>
     </row>
-    <row r="598" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="598" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C598" s="4"/>
     </row>
-    <row r="599" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="599" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C599" s="4"/>
     </row>
-    <row r="600" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="600" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C600" s="4"/>
     </row>
-    <row r="601" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="601" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C601" s="4"/>
     </row>
-    <row r="602" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="602" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C602" s="4"/>
     </row>
-    <row r="603" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="603" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C603" s="4"/>
     </row>
-    <row r="604" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="604" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C604" s="4"/>
     </row>
-    <row r="605" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="605" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C605" s="4"/>
     </row>
-    <row r="606" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="606" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C606" s="4"/>
     </row>
-    <row r="607" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="607" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C607" s="4"/>
     </row>
-    <row r="608" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="608" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C608" s="4"/>
     </row>
-    <row r="609" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="609" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C609" s="4"/>
     </row>
-    <row r="610" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="610" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C610" s="4"/>
     </row>
-    <row r="611" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="611" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C611" s="4"/>
     </row>
-    <row r="612" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="612" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C612" s="4"/>
     </row>
-    <row r="613" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="613" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C613" s="4"/>
     </row>
-    <row r="614" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="614" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C614" s="4"/>
     </row>
-    <row r="615" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="615" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C615" s="4"/>
     </row>
-    <row r="616" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="616" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C616" s="4"/>
     </row>
-    <row r="617" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="617" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C617" s="4"/>
     </row>
-    <row r="618" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="618" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C618" s="4"/>
     </row>
-    <row r="619" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="619" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C619" s="4"/>
     </row>
-    <row r="620" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="620" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C620" s="4"/>
     </row>
-    <row r="621" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="621" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C621" s="4"/>
     </row>
-    <row r="622" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="622" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C622" s="4"/>
     </row>
-    <row r="623" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="623" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C623" s="4"/>
     </row>
-    <row r="624" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="624" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C624" s="4"/>
     </row>
-    <row r="625" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="625" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C625" s="4"/>
     </row>
-    <row r="626" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="626" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C626" s="4"/>
     </row>
-    <row r="627" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="627" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C627" s="4"/>
     </row>
-    <row r="628" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="628" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C628" s="4"/>
     </row>
-    <row r="629" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="629" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C629" s="4"/>
     </row>
-    <row r="630" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="630" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C630" s="4"/>
     </row>
-    <row r="631" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="631" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C631" s="4"/>
     </row>
-    <row r="632" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="632" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C632" s="4"/>
     </row>
-    <row r="633" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="633" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C633" s="4"/>
     </row>
-    <row r="634" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="634" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C634" s="4"/>
     </row>
-    <row r="635" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="635" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C635" s="4"/>
     </row>
-    <row r="636" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="636" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C636" s="4"/>
     </row>
-    <row r="637" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="637" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C637" s="4"/>
     </row>
-    <row r="638" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="638" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C638" s="4"/>
     </row>
-    <row r="639" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="639" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C639" s="4"/>
     </row>
-    <row r="640" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="640" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C640" s="4"/>
     </row>
-    <row r="641" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="641" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C641" s="4"/>
     </row>
-    <row r="642" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="642" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C642" s="4"/>
     </row>
-    <row r="643" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="643" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C643" s="4"/>
     </row>
-    <row r="644" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="644" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C644" s="4"/>
     </row>
-    <row r="645" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="645" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C645" s="4"/>
     </row>
-    <row r="646" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="646" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C646" s="4"/>
     </row>
-    <row r="647" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="647" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C647" s="4"/>
     </row>
-    <row r="648" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="648" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C648" s="4"/>
     </row>
-    <row r="649" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="649" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C649" s="4"/>
     </row>
-    <row r="650" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="650" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C650" s="4"/>
     </row>
-    <row r="651" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="651" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C651" s="4"/>
     </row>
-    <row r="652" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="652" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C652" s="4"/>
     </row>
-    <row r="653" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="653" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C653" s="4"/>
     </row>
-    <row r="654" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="654" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C654" s="4"/>
     </row>
-    <row r="655" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="655" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C655" s="4"/>
     </row>
-    <row r="656" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="656" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C656" s="4"/>
     </row>
-    <row r="657" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="657" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C657" s="4"/>
     </row>
-    <row r="658" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="658" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C658" s="4"/>
     </row>
-    <row r="659" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="659" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C659" s="4"/>
     </row>
-    <row r="660" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="660" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C660" s="4"/>
     </row>
-    <row r="661" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="661" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C661" s="4"/>
     </row>
-    <row r="662" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="662" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C662" s="4"/>
     </row>
-    <row r="663" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="663" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C663" s="4"/>
     </row>
-    <row r="664" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="664" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C664" s="4"/>
     </row>
-    <row r="665" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="665" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C665" s="4"/>
     </row>
-    <row r="666" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="666" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C666" s="4"/>
     </row>
-    <row r="667" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="667" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C667" s="4"/>
     </row>
-    <row r="668" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="668" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C668" s="4"/>
     </row>
-    <row r="669" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="669" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C669" s="4"/>
     </row>
-    <row r="670" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="670" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C670" s="4"/>
     </row>
-    <row r="671" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="671" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C671" s="4"/>
     </row>
-    <row r="672" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="672" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C672" s="4"/>
     </row>
-    <row r="673" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="673" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C673" s="4"/>
     </row>
-    <row r="674" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="674" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C674" s="4"/>
     </row>
-    <row r="675" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="675" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C675" s="4"/>
     </row>
-    <row r="676" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="676" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C676" s="4"/>
     </row>
-    <row r="677" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="677" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C677" s="4"/>
     </row>
-    <row r="678" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="678" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C678" s="4"/>
     </row>
-    <row r="679" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="679" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C679" s="4"/>
     </row>
-    <row r="680" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="680" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C680" s="4"/>
     </row>
-    <row r="681" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="681" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C681" s="4"/>
     </row>
-    <row r="682" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="682" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C682" s="4"/>
     </row>
-    <row r="683" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="683" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C683" s="4"/>
     </row>
-    <row r="684" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="684" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C684" s="4"/>
     </row>
-    <row r="685" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="685" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C685" s="4"/>
     </row>
-    <row r="686" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="686" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C686" s="4"/>
     </row>
-    <row r="687" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="687" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C687" s="4"/>
     </row>
-    <row r="688" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="688" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C688" s="4"/>
     </row>
-    <row r="689" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="689" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C689" s="4"/>
     </row>
-    <row r="690" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="690" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C690" s="4"/>
     </row>
-    <row r="691" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="691" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C691" s="4"/>
     </row>
-    <row r="692" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="692" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C692" s="4"/>
     </row>
-    <row r="693" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="693" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C693" s="4"/>
     </row>
-    <row r="694" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="694" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C694" s="4"/>
     </row>
-    <row r="695" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="695" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C695" s="4"/>
     </row>
-    <row r="696" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="696" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C696" s="4"/>
     </row>
-    <row r="697" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="697" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C697" s="4"/>
     </row>
-    <row r="698" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="698" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C698" s="4"/>
     </row>
-    <row r="699" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="699" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C699" s="4"/>
     </row>
-    <row r="700" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="700" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C700" s="4"/>
     </row>
-    <row r="701" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="701" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C701" s="4"/>
     </row>
-    <row r="702" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="702" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C702" s="4"/>
     </row>
-    <row r="703" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="703" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C703" s="4"/>
     </row>
-    <row r="704" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="704" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C704" s="4"/>
     </row>
-    <row r="705" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="705" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C705" s="4"/>
     </row>
-    <row r="706" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="706" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C706" s="4"/>
     </row>
-    <row r="707" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="707" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C707" s="4"/>
     </row>
-    <row r="708" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="708" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C708" s="4"/>
     </row>
-    <row r="709" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="709" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C709" s="4"/>
     </row>
-    <row r="710" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="710" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C710" s="4"/>
     </row>
-    <row r="711" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="711" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C711" s="4"/>
     </row>
-    <row r="712" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="712" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C712" s="4"/>
     </row>
-    <row r="713" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="713" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C713" s="4"/>
     </row>
-    <row r="714" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="714" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C714" s="4"/>
     </row>
-    <row r="715" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="715" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C715" s="4"/>
     </row>
-    <row r="716" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="716" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C716" s="4"/>
     </row>
-    <row r="717" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="717" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C717" s="4"/>
     </row>
-    <row r="718" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="718" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C718" s="4"/>
     </row>
-    <row r="719" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="719" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C719" s="4"/>
     </row>
-    <row r="720" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="720" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C720" s="4"/>
     </row>
-    <row r="721" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="721" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C721" s="4"/>
     </row>
-    <row r="722" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="722" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C722" s="4"/>
     </row>
-    <row r="723" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="723" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C723" s="4"/>
     </row>
-    <row r="724" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="724" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C724" s="4"/>
     </row>
-    <row r="725" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="725" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C725" s="4"/>
     </row>
-    <row r="726" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="726" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C726" s="4"/>
     </row>
-    <row r="727" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="727" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C727" s="4"/>
     </row>
-    <row r="728" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="728" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C728" s="4"/>
     </row>
-    <row r="729" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="729" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C729" s="4"/>
     </row>
-    <row r="730" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="730" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C730" s="4"/>
     </row>
-    <row r="731" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="731" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C731" s="4"/>
     </row>
-    <row r="732" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="732" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C732" s="4"/>
     </row>
-    <row r="733" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="733" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C733" s="4"/>
     </row>
-    <row r="734" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="734" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C734" s="4"/>
     </row>
-    <row r="735" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="735" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C735" s="4"/>
     </row>
-    <row r="736" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="736" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C736" s="4"/>
     </row>
-    <row r="737" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="737" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C737" s="4"/>
     </row>
-    <row r="738" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="738" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C738" s="4"/>
     </row>
-    <row r="739" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="739" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C739" s="4"/>
     </row>
-    <row r="740" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="740" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C740" s="4"/>
     </row>
-    <row r="741" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="741" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C741" s="4"/>
     </row>
-    <row r="742" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="742" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C742" s="4"/>
     </row>
-    <row r="743" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="743" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C743" s="4"/>
     </row>
-    <row r="744" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="744" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C744" s="4"/>
     </row>
-    <row r="745" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="745" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C745" s="4"/>
     </row>
-    <row r="746" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="746" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C746" s="4"/>
     </row>
-    <row r="747" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="747" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C747" s="4"/>
     </row>
-    <row r="748" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="748" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C748" s="4"/>
     </row>
-    <row r="749" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="749" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C749" s="4"/>
     </row>
-    <row r="750" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="750" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C750" s="4"/>
     </row>
-    <row r="751" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="751" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C751" s="4"/>
     </row>
-    <row r="752" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="752" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C752" s="4"/>
     </row>
-    <row r="753" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="753" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C753" s="4"/>
     </row>
-    <row r="754" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="754" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C754" s="4"/>
     </row>
-    <row r="755" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="755" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C755" s="4"/>
     </row>
-    <row r="756" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="756" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C756" s="4"/>
     </row>
-    <row r="757" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="757" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C757" s="4"/>
     </row>
-    <row r="758" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="758" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C758" s="4"/>
     </row>
-    <row r="759" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="759" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C759" s="4"/>
     </row>
-    <row r="760" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="760" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C760" s="4"/>
     </row>
-    <row r="761" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="761" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C761" s="4"/>
     </row>
-    <row r="762" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="762" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C762" s="4"/>
     </row>
-    <row r="763" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="763" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C763" s="4"/>
     </row>
-    <row r="764" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="764" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C764" s="4"/>
     </row>
-    <row r="765" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="765" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C765" s="4"/>
     </row>
-    <row r="766" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="766" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C766" s="4"/>
     </row>
-    <row r="767" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="767" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C767" s="4"/>
     </row>
-    <row r="768" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="768" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C768" s="4"/>
     </row>
-    <row r="769" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="769" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C769" s="4"/>
     </row>
-    <row r="770" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="770" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C770" s="4"/>
     </row>
-    <row r="771" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="771" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C771" s="4"/>
     </row>
-    <row r="772" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="772" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C772" s="4"/>
     </row>
-    <row r="773" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="773" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C773" s="4"/>
     </row>
-    <row r="774" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="774" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C774" s="4"/>
     </row>
-    <row r="775" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="775" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C775" s="4"/>
     </row>
-    <row r="776" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="776" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C776" s="4"/>
     </row>
-    <row r="777" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="777" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C777" s="4"/>
     </row>
-    <row r="778" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="778" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C778" s="4"/>
     </row>
-    <row r="779" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="779" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C779" s="4"/>
     </row>
-    <row r="780" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="780" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C780" s="4"/>
     </row>
-    <row r="781" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="781" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C781" s="4"/>
     </row>
-    <row r="782" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="782" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C782" s="4"/>
     </row>
-    <row r="783" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="783" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C783" s="4"/>
     </row>
-    <row r="784" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="784" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C784" s="4"/>
     </row>
-    <row r="785" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="785" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C785" s="4"/>
     </row>
-    <row r="786" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="786" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C786" s="4"/>
     </row>
-    <row r="787" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="787" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C787" s="4"/>
     </row>
-    <row r="788" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="788" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C788" s="4"/>
     </row>
-    <row r="789" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="789" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C789" s="4"/>
     </row>
-    <row r="790" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="790" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C790" s="4"/>
     </row>
-    <row r="791" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="791" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C791" s="4"/>
     </row>
-    <row r="792" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="792" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C792" s="4"/>
     </row>
-    <row r="793" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="793" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C793" s="4"/>
     </row>
-    <row r="794" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="794" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C794" s="4"/>
     </row>
-    <row r="795" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="795" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C795" s="4"/>
     </row>
-    <row r="796" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="796" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C796" s="4"/>
     </row>
-    <row r="797" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="797" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C797" s="4"/>
     </row>
-    <row r="798" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="798" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C798" s="4"/>
     </row>
-    <row r="799" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="799" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C799" s="4"/>
     </row>
-    <row r="800" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="800" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C800" s="4"/>
     </row>
-    <row r="801" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="801" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C801" s="4"/>
     </row>
-    <row r="802" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="802" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C802" s="4"/>
     </row>
-    <row r="803" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="803" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C803" s="4"/>
     </row>
-    <row r="804" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="804" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C804" s="4"/>
     </row>
-    <row r="805" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="805" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C805" s="4"/>
     </row>
-    <row r="806" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="806" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C806" s="4"/>
     </row>
-    <row r="807" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="807" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C807" s="4"/>
     </row>
-    <row r="808" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="808" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C808" s="4"/>
     </row>
-    <row r="809" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="809" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C809" s="4"/>
     </row>
-    <row r="810" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="810" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C810" s="4"/>
     </row>
-    <row r="811" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="811" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C811" s="4"/>
     </row>
-    <row r="812" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="812" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C812" s="4"/>
     </row>
-    <row r="813" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="813" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C813" s="4"/>
     </row>
-    <row r="814" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="814" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C814" s="4"/>
     </row>
-    <row r="815" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="815" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C815" s="4"/>
     </row>
-    <row r="816" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="816" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C816" s="4"/>
     </row>
-    <row r="817" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="817" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C817" s="4"/>
     </row>
-    <row r="818" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="818" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C818" s="4"/>
     </row>
-    <row r="819" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="819" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C819" s="4"/>
     </row>
-    <row r="820" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="820" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C820" s="4"/>
     </row>
-    <row r="821" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="821" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C821" s="4"/>
     </row>
-    <row r="822" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="822" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C822" s="4"/>
     </row>
-    <row r="823" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="823" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C823" s="4"/>
     </row>
-    <row r="824" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="824" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C824" s="4"/>
     </row>
-    <row r="825" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="825" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C825" s="4"/>
     </row>
-    <row r="826" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="826" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C826" s="4"/>
     </row>
-    <row r="827" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="827" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C827" s="4"/>
     </row>
-    <row r="828" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="828" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C828" s="4"/>
     </row>
-    <row r="829" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="829" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C829" s="4"/>
     </row>
-    <row r="830" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="830" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C830" s="4"/>
     </row>
-    <row r="831" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="831" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C831" s="4"/>
     </row>
-    <row r="832" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="832" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C832" s="4"/>
     </row>
-    <row r="833" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="833" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C833" s="4"/>
     </row>
-    <row r="834" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="834" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C834" s="4"/>
     </row>
-    <row r="835" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="835" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C835" s="4"/>
     </row>
-    <row r="836" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="836" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C836" s="4"/>
     </row>
-    <row r="837" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="837" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C837" s="4"/>
     </row>
-    <row r="838" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="838" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C838" s="4"/>
     </row>
-    <row r="839" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="839" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C839" s="4"/>
     </row>
-    <row r="840" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="840" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C840" s="4"/>
     </row>
-    <row r="841" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="841" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C841" s="4"/>
     </row>
-    <row r="842" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="842" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C842" s="4"/>
     </row>
-    <row r="843" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="843" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C843" s="4"/>
     </row>
-    <row r="844" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="844" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C844" s="4"/>
     </row>
-    <row r="845" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="845" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C845" s="4"/>
     </row>
-    <row r="846" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="846" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C846" s="4"/>
     </row>
-    <row r="847" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="847" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C847" s="4"/>
     </row>
-    <row r="848" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="848" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C848" s="4"/>
     </row>
-    <row r="849" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="849" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C849" s="4"/>
     </row>
-    <row r="850" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="850" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C850" s="4"/>
     </row>
-    <row r="851" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="851" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C851" s="4"/>
     </row>
-    <row r="852" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="852" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C852" s="4"/>
     </row>
-    <row r="853" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="853" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C853" s="4"/>
     </row>
-    <row r="854" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="854" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C854" s="4"/>
     </row>
-    <row r="855" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="855" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C855" s="4"/>
     </row>
-    <row r="856" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="856" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C856" s="4"/>
     </row>
-    <row r="857" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="857" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C857" s="4"/>
     </row>
-    <row r="858" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="858" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C858" s="4"/>
     </row>
-    <row r="859" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="859" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C859" s="4"/>
     </row>
-    <row r="860" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="860" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C860" s="4"/>
     </row>
-    <row r="861" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="861" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C861" s="4"/>
     </row>
-    <row r="862" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="862" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C862" s="4"/>
     </row>
-    <row r="863" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="863" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C863" s="4"/>
     </row>
-    <row r="864" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="864" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C864" s="4"/>
     </row>
-    <row r="865" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="865" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C865" s="4"/>
     </row>
-    <row r="866" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="866" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C866" s="4"/>
     </row>
-    <row r="867" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="867" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C867" s="4"/>
     </row>
-    <row r="868" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="868" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C868" s="4"/>
     </row>
-    <row r="869" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="869" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C869" s="4"/>
     </row>
-    <row r="870" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="870" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C870" s="4"/>
     </row>
-    <row r="871" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="871" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C871" s="4"/>
     </row>
-    <row r="872" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="872" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C872" s="4"/>
     </row>
-    <row r="873" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="873" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C873" s="4"/>
     </row>
-    <row r="874" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="874" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C874" s="4"/>
     </row>
-    <row r="875" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="875" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C875" s="4"/>
     </row>
-    <row r="876" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="876" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C876" s="4"/>
     </row>
-    <row r="877" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="877" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C877" s="4"/>
     </row>
-    <row r="878" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="878" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C878" s="4"/>
     </row>
-    <row r="879" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="879" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C879" s="4"/>
     </row>
-    <row r="880" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="880" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C880" s="4"/>
     </row>
-    <row r="881" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="881" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C881" s="4"/>
     </row>
-    <row r="882" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="882" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C882" s="4"/>
     </row>
-    <row r="883" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="883" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C883" s="4"/>
     </row>
-    <row r="884" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="884" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C884" s="4"/>
     </row>
-    <row r="885" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="885" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C885" s="4"/>
     </row>
-    <row r="886" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="886" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C886" s="4"/>
     </row>
-    <row r="887" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="887" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C887" s="4"/>
     </row>
-    <row r="888" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="888" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C888" s="4"/>
     </row>
-    <row r="889" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="889" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C889" s="4"/>
     </row>
-    <row r="890" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="890" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C890" s="4"/>
     </row>
-    <row r="891" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="891" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C891" s="4"/>
     </row>
-    <row r="892" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="892" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C892" s="4"/>
     </row>
-    <row r="893" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="893" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C893" s="4"/>
     </row>
-    <row r="894" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="894" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C894" s="4"/>
     </row>
-    <row r="895" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="895" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C895" s="4"/>
     </row>
-    <row r="896" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="896" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C896" s="4"/>
     </row>
-    <row r="897" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="897" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C897" s="4"/>
     </row>
-    <row r="898" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="898" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C898" s="4"/>
     </row>
-    <row r="899" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="899" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C899" s="4"/>
     </row>
-    <row r="900" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="900" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C900" s="4"/>
     </row>
-    <row r="901" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="901" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C901" s="4"/>
     </row>
-    <row r="902" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="902" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C902" s="4"/>
     </row>
-    <row r="903" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="903" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C903" s="4"/>
     </row>
-    <row r="904" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="904" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C904" s="4"/>
     </row>
-    <row r="905" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="905" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C905" s="4"/>
     </row>
-    <row r="906" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="906" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C906" s="4"/>
     </row>
-    <row r="907" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="907" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C907" s="4"/>
     </row>
-    <row r="908" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="908" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C908" s="4"/>
     </row>
-    <row r="909" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="909" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C909" s="4"/>
     </row>
-    <row r="910" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="910" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C910" s="4"/>
     </row>
-    <row r="911" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="911" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C911" s="4"/>
     </row>
-    <row r="912" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="912" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C912" s="4"/>
     </row>
-    <row r="913" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="913" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C913" s="4"/>
     </row>
-    <row r="914" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="914" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C914" s="4"/>
     </row>
-    <row r="915" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="915" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C915" s="4"/>
     </row>
-    <row r="916" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="916" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C916" s="4"/>
     </row>
-    <row r="917" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="917" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C917" s="4"/>
     </row>
-    <row r="918" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="918" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C918" s="4"/>
     </row>
-    <row r="919" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="919" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C919" s="4"/>
     </row>
-    <row r="920" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="920" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C920" s="4"/>
     </row>
-    <row r="921" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="921" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C921" s="4"/>
     </row>
-    <row r="922" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="922" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C922" s="4"/>
     </row>
-    <row r="923" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="923" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C923" s="4"/>
     </row>
-    <row r="924" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="924" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C924" s="4"/>
     </row>
-    <row r="925" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="925" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C925" s="4"/>
     </row>
-    <row r="926" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="926" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C926" s="4"/>
     </row>
-    <row r="927" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="927" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C927" s="4"/>
     </row>
-    <row r="928" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="928" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C928" s="4"/>
     </row>
-    <row r="929" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="929" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C929" s="4"/>
     </row>
-    <row r="930" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="930" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C930" s="4"/>
     </row>
-    <row r="931" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="931" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C931" s="4"/>
     </row>
-    <row r="932" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="932" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C932" s="4"/>
     </row>
-    <row r="933" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="933" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C933" s="4"/>
     </row>
-    <row r="934" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="934" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C934" s="4"/>
     </row>
-    <row r="935" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="935" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C935" s="4"/>
     </row>
-    <row r="936" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="936" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C936" s="4"/>
     </row>
-    <row r="937" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="937" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C937" s="4"/>
     </row>
-    <row r="938" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="938" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C938" s="4"/>
     </row>
-    <row r="939" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="939" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C939" s="4"/>
     </row>
-    <row r="940" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="940" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C940" s="4"/>
     </row>
-    <row r="941" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="941" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C941" s="4"/>
     </row>
-    <row r="942" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="942" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C942" s="4"/>
     </row>
-    <row r="943" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="943" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C943" s="4"/>
     </row>
-    <row r="944" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="944" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C944" s="4"/>
     </row>
-    <row r="945" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="945" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C945" s="4"/>
     </row>
-    <row r="946" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="946" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C946" s="4"/>
     </row>
-    <row r="947" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="947" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C947" s="4"/>
     </row>
-    <row r="948" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="948" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C948" s="4"/>
     </row>
-    <row r="949" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="949" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C949" s="4"/>
     </row>
-    <row r="950" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="950" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C950" s="4"/>
     </row>
-    <row r="951" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="951" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C951" s="4"/>
     </row>
-    <row r="952" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="952" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C952" s="4"/>
     </row>
-    <row r="953" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="953" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C953" s="4"/>
     </row>
-    <row r="954" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="954" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C954" s="4"/>
     </row>
-    <row r="955" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="955" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C955" s="4"/>
     </row>
-    <row r="956" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="956" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C956" s="4"/>
     </row>
-    <row r="957" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="957" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C957" s="4"/>
     </row>
-    <row r="958" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="958" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C958" s="4"/>
     </row>
-    <row r="959" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="959" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C959" s="4"/>
     </row>
-    <row r="960" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="960" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C960" s="4"/>
     </row>
-    <row r="961" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="961" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C961" s="4"/>
     </row>
-    <row r="962" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="962" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C962" s="4"/>
     </row>
-    <row r="963" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="963" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C963" s="4"/>
     </row>
-    <row r="964" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="964" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C964" s="4"/>
     </row>
-    <row r="965" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="965" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C965" s="4"/>
     </row>
-    <row r="966" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="966" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C966" s="4"/>
     </row>
-    <row r="967" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="967" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C967" s="4"/>
     </row>
-    <row r="968" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="968" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C968" s="4"/>
     </row>
-    <row r="969" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="969" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C969" s="4"/>
     </row>
-    <row r="970" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="970" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C970" s="4"/>
     </row>
-    <row r="971" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="971" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C971" s="4"/>
     </row>
-    <row r="972" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="972" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C972" s="4"/>
     </row>
-    <row r="973" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="973" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C973" s="4"/>
     </row>
-    <row r="974" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="974" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C974" s="4"/>
     </row>
-    <row r="975" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="975" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C975" s="4"/>
     </row>
-    <row r="976" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="976" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C976" s="4"/>
     </row>
-    <row r="977" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="977" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C977" s="4"/>
     </row>
-    <row r="978" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="978" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C978" s="4"/>
     </row>
-    <row r="979" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="979" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C979" s="4"/>
     </row>
-    <row r="980" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="980" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C980" s="4"/>
     </row>
-    <row r="981" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="981" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C981" s="4"/>
     </row>
-    <row r="982" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="982" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C982" s="4"/>
     </row>
-    <row r="983" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="983" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C983" s="4"/>
     </row>
-    <row r="984" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="984" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C984" s="4"/>
     </row>
-    <row r="985" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="985" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C985" s="4"/>
     </row>
-    <row r="986" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="986" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C986" s="4"/>
     </row>
-    <row r="987" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="987" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C987" s="4"/>
     </row>
-    <row r="988" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="988" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C988" s="4"/>
     </row>
-    <row r="989" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="989" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C989" s="4"/>
     </row>
-    <row r="990" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="990" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C990" s="4"/>
     </row>
-    <row r="991" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="991" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C991" s="4"/>
     </row>
-    <row r="992" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="992" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C992" s="4"/>
     </row>
-    <row r="993" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="993" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C993" s="4"/>
     </row>
-    <row r="994" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="994" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C994" s="4"/>
     </row>
-    <row r="995" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="995" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C995" s="4"/>
     </row>
-    <row r="996" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="996" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C996" s="4"/>
     </row>
-    <row r="997" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="997" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C997" s="4"/>
     </row>
-    <row r="998" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="998" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C998" s="4"/>
     </row>
-    <row r="999" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="999" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C999" s="4"/>
     </row>
-    <row r="1000" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1000" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C1000" s="4"/>
     </row>
-    <row r="1001" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1001" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C1001" s="4"/>
     </row>
-    <row r="1002" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1002" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C1002" s="4"/>
     </row>
-    <row r="1003" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1003" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C1003" s="4"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
create online models and prepare for crud(admin)
</commit_message>
<xml_diff>
--- a/PlanExcel/plan.xlsx
+++ b/PlanExcel/plan.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\~project\AndroidKotlin\MUSIC\PlanExcel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7AD5799-44B8-43A3-B718-2893208BBCBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BBB9378-5904-4CEB-A98C-48BA086E0D51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="14880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -114,9 +114,6 @@
 bài hát)</t>
   </si>
   <si>
-    <t>Phân quyền (người quản trị, người dùng)</t>
-  </si>
-  <si>
     <t>Hoàn thiện giao diện cho ứng dụng</t>
   </si>
   <si>
@@ -157,15 +154,19 @@
     <t>Màn hình tìm kiếm bài hát (Module tìm kiếm bài hát)</t>
   </si>
   <si>
-    <t>MUSIC là một phần mềm di động giúp người yêu nhạc thỏa mãn nhu cầu thưởng thức của mình một cách dễ dàng và trọn vẹn nhất bằng cách:
-- Hỗ trợ phát nhạc trực tuyến.
-- Tìm kiếm và phân loại bài hát theo tên, theo album, nghệ sĩ, thể loại,...
-- Lưu danh sách phát tuỳ chỉnh của người dùng.
-- Tạo giao diện trực quan và dễ dàng thao tác.
-- Hỗ trợ nghe nhạc ngoại tuyến với các bài hát có sẵn trên máy.</t>
+    <t>Màn hình đăng nhập, đăng ký (Module đăng nhập, đăng ký)</t>
   </si>
   <si>
-    <t>Màn hình đăng nhập, đăng ký (Module đăng nhập, đăng ký)</t>
+    <t>Phân quyền (người quản trị, người dùng  - Firebase Authentication API)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MUSIC là một phần mềm di động giúp người yêu nhạc thỏa mãn nhu cầu thưởng thức của mình một cách dễ dàng và trọn vẹn nhất bằng cách:
+- Hỗ trợ phát nhạc trực tuyến và ngoại tuyến với các bài hát có sẵn trên máy.
+- Tìm kiếm và phân loại bài hát theo tên, theo album, theo nghệ sĩ, theo thể loại, theo danh sách phát (tuỳ chỉnh hoặc có sẵn).
+- Quản lý bài hát, danh sách phát, nghệ sĩ, album, thể loại, thông tin tài khoản, người dùng.
+- Đăng nhập, đăng ký, đăng xuất, khôi phục mật khẩu.
+- Để lại bình luận cho từng bài hát.
+- Tạo giao diện trực quan và dễ dàng thao tác. </t>
   </si>
 </sst>
 </file>
@@ -561,25 +562,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Y1003"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4:I4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.7109375" customWidth="1"/>
-    <col min="2" max="2" width="46.5703125" customWidth="1"/>
-    <col min="3" max="3" width="79.28515625" customWidth="1"/>
-    <col min="4" max="4" width="26.28515625" customWidth="1"/>
-    <col min="5" max="5" width="27.85546875" customWidth="1"/>
-    <col min="6" max="6" width="28.28515625" customWidth="1"/>
-    <col min="7" max="7" width="26.28515625" customWidth="1"/>
-    <col min="8" max="8" width="27.28515625" customWidth="1"/>
-    <col min="9" max="9" width="11.28515625" customWidth="1"/>
-    <col min="10" max="25" width="8.7109375" customWidth="1"/>
+    <col min="1" max="1" width="8.6640625" customWidth="1"/>
+    <col min="2" max="2" width="46.5546875" customWidth="1"/>
+    <col min="3" max="3" width="87.88671875" customWidth="1"/>
+    <col min="4" max="4" width="26.33203125" customWidth="1"/>
+    <col min="5" max="5" width="27.88671875" customWidth="1"/>
+    <col min="6" max="6" width="28.33203125" customWidth="1"/>
+    <col min="7" max="7" width="26.33203125" customWidth="1"/>
+    <col min="8" max="8" width="27.33203125" customWidth="1"/>
+    <col min="9" max="9" width="11.33203125" customWidth="1"/>
+    <col min="10" max="25" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" ht="33.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:25" ht="33.6" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
@@ -608,7 +609,7 @@
       <c r="X1" s="1"/>
       <c r="Y1" s="1"/>
     </row>
-    <row r="2" spans="1:25" ht="31.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:25" ht="31.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="16" t="s">
         <v>1</v>
       </c>
@@ -637,7 +638,7 @@
       <c r="X2" s="1"/>
       <c r="Y2" s="1"/>
     </row>
-    <row r="3" spans="1:25" ht="25.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:25" ht="19.8" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="16" t="s">
         <v>2</v>
       </c>
@@ -666,13 +667,13 @@
       <c r="X3" s="1"/>
       <c r="Y3" s="1"/>
     </row>
-    <row r="4" spans="1:25" ht="138.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:25" ht="154.19999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2"/>
       <c r="B4" s="2" t="s">
         <v>3</v>
       </c>
       <c r="C4" s="18" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D4" s="19"/>
       <c r="E4" s="19"/>
@@ -697,10 +698,10 @@
       <c r="X4" s="3"/>
       <c r="Y4" s="3"/>
     </row>
-    <row r="5" spans="1:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C5" s="4"/>
     </row>
-    <row r="6" spans="1:25" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:25" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="11" t="s">
         <v>4</v>
       </c>
@@ -745,7 +746,7 @@
       <c r="X6" s="5"/>
       <c r="Y6" s="5"/>
     </row>
-    <row r="7" spans="1:25" ht="45.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:25" ht="45.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="11">
         <v>1</v>
       </c>
@@ -786,7 +787,7 @@
       <c r="X7" s="5"/>
       <c r="Y7" s="5"/>
     </row>
-    <row r="8" spans="1:25" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:25" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="11">
         <v>2</v>
       </c>
@@ -825,7 +826,7 @@
       <c r="X8" s="5"/>
       <c r="Y8" s="5"/>
     </row>
-    <row r="9" spans="1:25" ht="20.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:25" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="11"/>
       <c r="B9" s="11"/>
       <c r="C9" s="12" t="s">
@@ -862,7 +863,7 @@
       <c r="X9" s="5"/>
       <c r="Y9" s="5"/>
     </row>
-    <row r="10" spans="1:25" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:25" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="11"/>
       <c r="B10" s="11"/>
       <c r="C10" s="12" t="s">
@@ -899,7 +900,7 @@
       <c r="X10" s="5"/>
       <c r="Y10" s="5"/>
     </row>
-    <row r="11" spans="1:25" ht="25.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:25" ht="25.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="11">
         <v>3</v>
       </c>
@@ -940,7 +941,7 @@
       <c r="X11" s="5"/>
       <c r="Y11" s="5"/>
     </row>
-    <row r="12" spans="1:25" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:25" ht="45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="11">
         <v>4</v>
       </c>
@@ -979,7 +980,7 @@
       <c r="X12" s="5"/>
       <c r="Y12" s="5"/>
     </row>
-    <row r="13" spans="1:25" ht="20.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:25" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="11">
         <v>5</v>
       </c>
@@ -1018,11 +1019,11 @@
       <c r="X13" s="5"/>
       <c r="Y13" s="5"/>
     </row>
-    <row r="14" spans="1:25" ht="62.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:25" ht="62.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="11"/>
       <c r="B14" s="11"/>
       <c r="C14" s="13" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D14" s="11" t="s">
         <v>15</v>
@@ -1053,7 +1054,7 @@
       <c r="X14" s="5"/>
       <c r="Y14" s="5"/>
     </row>
-    <row r="15" spans="1:25" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:25" ht="41.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="11">
         <v>6</v>
       </c>
@@ -1092,11 +1093,11 @@
       <c r="X15" s="5"/>
       <c r="Y15" s="5"/>
     </row>
-    <row r="16" spans="1:25" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:25" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="11"/>
       <c r="B16" s="11"/>
       <c r="C16" s="12" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D16" s="11" t="s">
         <v>15</v>
@@ -1127,11 +1128,11 @@
       <c r="X16" s="5"/>
       <c r="Y16" s="5"/>
     </row>
-    <row r="17" spans="1:25" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:25" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="11"/>
       <c r="B17" s="11"/>
       <c r="C17" s="12" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D17" s="11" t="s">
         <v>15</v>
@@ -1162,11 +1163,11 @@
       <c r="X17" s="5"/>
       <c r="Y17" s="5"/>
     </row>
-    <row r="18" spans="1:25" ht="23.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:25" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="11"/>
       <c r="B18" s="11"/>
       <c r="C18" s="12" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D18" s="11" t="s">
         <v>15</v>
@@ -1197,11 +1198,11 @@
       <c r="X18" s="5"/>
       <c r="Y18" s="5"/>
     </row>
-    <row r="19" spans="1:25" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:25" ht="21.6" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A19" s="11"/>
       <c r="B19" s="11"/>
       <c r="C19" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D19" s="11" t="s">
         <v>15</v>
@@ -1232,11 +1233,11 @@
       <c r="X19" s="5"/>
       <c r="Y19" s="5"/>
     </row>
-    <row r="20" spans="1:25" ht="22.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:25" ht="22.95" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A20" s="11"/>
       <c r="B20" s="11"/>
       <c r="C20" s="15" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D20" s="11" t="s">
         <v>15</v>
@@ -1267,11 +1268,11 @@
       <c r="X20" s="5"/>
       <c r="Y20" s="5"/>
     </row>
-    <row r="21" spans="1:25" ht="22.15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:25" ht="22.2" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A21" s="11"/>
       <c r="B21" s="11"/>
       <c r="C21" s="15" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D21" s="11" t="s">
         <v>15</v>
@@ -1302,11 +1303,11 @@
       <c r="X21" s="5"/>
       <c r="Y21" s="5"/>
     </row>
-    <row r="22" spans="1:25" ht="20.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:25" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A22" s="11"/>
       <c r="B22" s="11"/>
       <c r="C22" s="15" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D22" s="11" t="s">
         <v>15</v>
@@ -1337,11 +1338,11 @@
       <c r="X22" s="5"/>
       <c r="Y22" s="5"/>
     </row>
-    <row r="23" spans="1:25" s="10" customFormat="1" ht="20.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:25" s="10" customFormat="1" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A23" s="11"/>
       <c r="B23" s="11"/>
       <c r="C23" s="15" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D23" s="11" t="s">
         <v>15</v>
@@ -1372,11 +1373,11 @@
       <c r="X23" s="5"/>
       <c r="Y23" s="5"/>
     </row>
-    <row r="24" spans="1:25" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:25" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="11"/>
       <c r="B24" s="11"/>
       <c r="C24" s="12" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D24" s="11" t="s">
         <v>15</v>
@@ -1407,11 +1408,11 @@
       <c r="X24" s="5"/>
       <c r="Y24" s="5"/>
     </row>
-    <row r="25" spans="1:25" ht="24.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:25" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="11"/>
       <c r="B25" s="11"/>
       <c r="C25" s="12" t="s">
-        <v>28</v>
+        <v>42</v>
       </c>
       <c r="D25" s="11" t="s">
         <v>15</v>
@@ -1442,12 +1443,12 @@
       <c r="X25" s="5"/>
       <c r="Y25" s="5"/>
     </row>
-    <row r="26" spans="1:25" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:25" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="11">
         <v>7</v>
       </c>
       <c r="B26" s="12" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C26" s="12"/>
       <c r="D26" s="11" t="s">
@@ -1479,15 +1480,15 @@
       <c r="X26" s="5"/>
       <c r="Y26" s="5"/>
     </row>
-    <row r="27" spans="1:25" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:25" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="11">
         <v>8</v>
       </c>
       <c r="B27" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="C27" s="12" t="s">
         <v>30</v>
-      </c>
-      <c r="C27" s="12" t="s">
-        <v>31</v>
       </c>
       <c r="D27" s="11" t="s">
         <v>15</v>
@@ -1518,12 +1519,12 @@
       <c r="X27" s="5"/>
       <c r="Y27" s="5"/>
     </row>
-    <row r="28" spans="1:25" ht="26.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:25" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="11">
         <v>9</v>
       </c>
       <c r="B28" s="12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C28" s="12"/>
       <c r="D28" s="11" t="s">
@@ -1555,7 +1556,7 @@
       <c r="X28" s="5"/>
       <c r="Y28" s="5"/>
     </row>
-    <row r="29" spans="1:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="6"/>
       <c r="B29" s="6"/>
       <c r="C29" s="7"/>
@@ -1582,7 +1583,7 @@
       <c r="X29" s="5"/>
       <c r="Y29" s="5"/>
     </row>
-    <row r="30" spans="1:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="6"/>
       <c r="B30" s="6"/>
       <c r="C30" s="7"/>
@@ -1609,7 +1610,7 @@
       <c r="X30" s="5"/>
       <c r="Y30" s="5"/>
     </row>
-    <row r="31" spans="1:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="6"/>
       <c r="B31" s="6"/>
       <c r="C31" s="7"/>
@@ -1636,7 +1637,7 @@
       <c r="X31" s="5"/>
       <c r="Y31" s="5"/>
     </row>
-    <row r="32" spans="1:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="6"/>
       <c r="B32" s="9"/>
       <c r="C32" s="7"/>
@@ -1663,7 +1664,7 @@
       <c r="X32" s="5"/>
       <c r="Y32" s="5"/>
     </row>
-    <row r="33" spans="1:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="6"/>
       <c r="B33" s="6"/>
       <c r="C33" s="7"/>
@@ -1690,7 +1691,7 @@
       <c r="X33" s="5"/>
       <c r="Y33" s="5"/>
     </row>
-    <row r="34" spans="1:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="6"/>
       <c r="B34" s="6"/>
       <c r="C34" s="7"/>
@@ -1717,2911 +1718,2911 @@
       <c r="X34" s="5"/>
       <c r="Y34" s="5"/>
     </row>
-    <row r="35" spans="1:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C35" s="4"/>
     </row>
-    <row r="36" spans="1:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C36" s="4"/>
     </row>
-    <row r="37" spans="1:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C37" s="4"/>
     </row>
-    <row r="38" spans="1:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C38" s="4"/>
     </row>
-    <row r="39" spans="1:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C39" s="4"/>
     </row>
-    <row r="40" spans="1:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C40" s="4"/>
     </row>
-    <row r="41" spans="1:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C41" s="4"/>
     </row>
-    <row r="42" spans="1:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C42" s="4"/>
     </row>
-    <row r="43" spans="1:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C43" s="4"/>
     </row>
-    <row r="44" spans="1:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C44" s="4"/>
     </row>
-    <row r="45" spans="1:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C45" s="4"/>
     </row>
-    <row r="46" spans="1:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C46" s="4"/>
     </row>
-    <row r="47" spans="1:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C47" s="4"/>
     </row>
-    <row r="48" spans="1:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C48" s="4"/>
     </row>
-    <row r="49" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C49" s="4"/>
     </row>
-    <row r="50" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C50" s="4"/>
     </row>
-    <row r="51" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C51" s="4"/>
     </row>
-    <row r="52" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C52" s="4"/>
     </row>
-    <row r="53" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C53" s="4"/>
     </row>
-    <row r="54" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C54" s="4"/>
     </row>
-    <row r="55" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C55" s="4"/>
     </row>
-    <row r="56" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C56" s="4"/>
     </row>
-    <row r="57" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C57" s="4"/>
     </row>
-    <row r="58" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C58" s="4"/>
     </row>
-    <row r="59" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C59" s="4"/>
     </row>
-    <row r="60" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C60" s="4"/>
     </row>
-    <row r="61" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C61" s="4"/>
     </row>
-    <row r="62" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C62" s="4"/>
     </row>
-    <row r="63" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C63" s="4"/>
     </row>
-    <row r="64" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C64" s="4"/>
     </row>
-    <row r="65" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C65" s="4"/>
     </row>
-    <row r="66" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C66" s="4"/>
     </row>
-    <row r="67" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C67" s="4"/>
     </row>
-    <row r="68" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C68" s="4"/>
     </row>
-    <row r="69" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C69" s="4"/>
     </row>
-    <row r="70" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C70" s="4"/>
     </row>
-    <row r="71" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C71" s="4"/>
     </row>
-    <row r="72" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C72" s="4"/>
     </row>
-    <row r="73" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C73" s="4"/>
     </row>
-    <row r="74" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C74" s="4"/>
     </row>
-    <row r="75" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C75" s="4"/>
     </row>
-    <row r="76" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C76" s="4"/>
     </row>
-    <row r="77" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C77" s="4"/>
     </row>
-    <row r="78" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C78" s="4"/>
     </row>
-    <row r="79" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C79" s="4"/>
     </row>
-    <row r="80" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C80" s="4"/>
     </row>
-    <row r="81" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C81" s="4"/>
     </row>
-    <row r="82" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C82" s="4"/>
     </row>
-    <row r="83" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C83" s="4"/>
     </row>
-    <row r="84" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C84" s="4"/>
     </row>
-    <row r="85" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C85" s="4"/>
     </row>
-    <row r="86" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C86" s="4"/>
     </row>
-    <row r="87" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C87" s="4"/>
     </row>
-    <row r="88" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C88" s="4"/>
     </row>
-    <row r="89" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C89" s="4"/>
     </row>
-    <row r="90" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C90" s="4"/>
     </row>
-    <row r="91" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C91" s="4"/>
     </row>
-    <row r="92" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C92" s="4"/>
     </row>
-    <row r="93" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C93" s="4"/>
     </row>
-    <row r="94" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C94" s="4"/>
     </row>
-    <row r="95" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C95" s="4"/>
     </row>
-    <row r="96" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C96" s="4"/>
     </row>
-    <row r="97" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C97" s="4"/>
     </row>
-    <row r="98" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C98" s="4"/>
     </row>
-    <row r="99" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C99" s="4"/>
     </row>
-    <row r="100" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C100" s="4"/>
     </row>
-    <row r="101" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C101" s="4"/>
     </row>
-    <row r="102" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C102" s="4"/>
     </row>
-    <row r="103" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C103" s="4"/>
     </row>
-    <row r="104" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C104" s="4"/>
     </row>
-    <row r="105" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C105" s="4"/>
     </row>
-    <row r="106" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C106" s="4"/>
     </row>
-    <row r="107" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C107" s="4"/>
     </row>
-    <row r="108" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C108" s="4"/>
     </row>
-    <row r="109" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C109" s="4"/>
     </row>
-    <row r="110" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C110" s="4"/>
     </row>
-    <row r="111" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C111" s="4"/>
     </row>
-    <row r="112" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C112" s="4"/>
     </row>
-    <row r="113" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C113" s="4"/>
     </row>
-    <row r="114" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C114" s="4"/>
     </row>
-    <row r="115" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C115" s="4"/>
     </row>
-    <row r="116" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C116" s="4"/>
     </row>
-    <row r="117" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C117" s="4"/>
     </row>
-    <row r="118" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C118" s="4"/>
     </row>
-    <row r="119" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C119" s="4"/>
     </row>
-    <row r="120" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="120" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C120" s="4"/>
     </row>
-    <row r="121" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="121" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C121" s="4"/>
     </row>
-    <row r="122" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="122" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C122" s="4"/>
     </row>
-    <row r="123" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="123" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C123" s="4"/>
     </row>
-    <row r="124" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="124" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C124" s="4"/>
     </row>
-    <row r="125" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="125" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C125" s="4"/>
     </row>
-    <row r="126" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="126" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C126" s="4"/>
     </row>
-    <row r="127" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="127" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C127" s="4"/>
     </row>
-    <row r="128" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="128" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C128" s="4"/>
     </row>
-    <row r="129" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="129" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C129" s="4"/>
     </row>
-    <row r="130" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="130" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C130" s="4"/>
     </row>
-    <row r="131" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="131" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C131" s="4"/>
     </row>
-    <row r="132" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="132" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C132" s="4"/>
     </row>
-    <row r="133" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="133" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C133" s="4"/>
     </row>
-    <row r="134" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="134" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C134" s="4"/>
     </row>
-    <row r="135" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="135" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C135" s="4"/>
     </row>
-    <row r="136" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="136" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C136" s="4"/>
     </row>
-    <row r="137" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="137" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C137" s="4"/>
     </row>
-    <row r="138" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="138" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C138" s="4"/>
     </row>
-    <row r="139" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="139" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C139" s="4"/>
     </row>
-    <row r="140" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="140" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C140" s="4"/>
     </row>
-    <row r="141" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="141" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C141" s="4"/>
     </row>
-    <row r="142" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="142" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C142" s="4"/>
     </row>
-    <row r="143" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="143" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C143" s="4"/>
     </row>
-    <row r="144" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="144" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C144" s="4"/>
     </row>
-    <row r="145" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="145" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C145" s="4"/>
     </row>
-    <row r="146" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="146" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C146" s="4"/>
     </row>
-    <row r="147" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="147" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C147" s="4"/>
     </row>
-    <row r="148" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="148" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C148" s="4"/>
     </row>
-    <row r="149" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="149" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C149" s="4"/>
     </row>
-    <row r="150" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="150" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C150" s="4"/>
     </row>
-    <row r="151" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="151" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C151" s="4"/>
     </row>
-    <row r="152" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="152" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C152" s="4"/>
     </row>
-    <row r="153" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="153" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C153" s="4"/>
     </row>
-    <row r="154" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="154" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C154" s="4"/>
     </row>
-    <row r="155" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="155" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C155" s="4"/>
     </row>
-    <row r="156" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="156" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C156" s="4"/>
     </row>
-    <row r="157" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="157" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C157" s="4"/>
     </row>
-    <row r="158" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="158" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C158" s="4"/>
     </row>
-    <row r="159" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="159" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C159" s="4"/>
     </row>
-    <row r="160" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="160" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C160" s="4"/>
     </row>
-    <row r="161" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="161" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C161" s="4"/>
     </row>
-    <row r="162" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="162" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C162" s="4"/>
     </row>
-    <row r="163" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="163" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C163" s="4"/>
     </row>
-    <row r="164" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="164" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C164" s="4"/>
     </row>
-    <row r="165" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="165" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C165" s="4"/>
     </row>
-    <row r="166" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="166" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C166" s="4"/>
     </row>
-    <row r="167" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="167" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C167" s="4"/>
     </row>
-    <row r="168" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="168" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C168" s="4"/>
     </row>
-    <row r="169" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="169" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C169" s="4"/>
     </row>
-    <row r="170" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="170" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C170" s="4"/>
     </row>
-    <row r="171" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="171" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C171" s="4"/>
     </row>
-    <row r="172" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="172" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C172" s="4"/>
     </row>
-    <row r="173" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="173" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C173" s="4"/>
     </row>
-    <row r="174" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="174" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C174" s="4"/>
     </row>
-    <row r="175" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="175" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C175" s="4"/>
     </row>
-    <row r="176" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="176" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C176" s="4"/>
     </row>
-    <row r="177" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="177" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C177" s="4"/>
     </row>
-    <row r="178" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="178" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C178" s="4"/>
     </row>
-    <row r="179" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="179" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C179" s="4"/>
     </row>
-    <row r="180" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="180" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C180" s="4"/>
     </row>
-    <row r="181" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="181" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C181" s="4"/>
     </row>
-    <row r="182" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="182" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C182" s="4"/>
     </row>
-    <row r="183" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="183" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C183" s="4"/>
     </row>
-    <row r="184" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="184" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C184" s="4"/>
     </row>
-    <row r="185" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="185" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C185" s="4"/>
     </row>
-    <row r="186" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="186" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C186" s="4"/>
     </row>
-    <row r="187" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="187" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C187" s="4"/>
     </row>
-    <row r="188" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="188" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C188" s="4"/>
     </row>
-    <row r="189" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="189" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C189" s="4"/>
     </row>
-    <row r="190" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="190" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C190" s="4"/>
     </row>
-    <row r="191" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="191" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C191" s="4"/>
     </row>
-    <row r="192" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="192" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C192" s="4"/>
     </row>
-    <row r="193" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="193" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C193" s="4"/>
     </row>
-    <row r="194" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="194" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C194" s="4"/>
     </row>
-    <row r="195" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="195" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C195" s="4"/>
     </row>
-    <row r="196" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="196" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C196" s="4"/>
     </row>
-    <row r="197" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="197" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C197" s="4"/>
     </row>
-    <row r="198" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="198" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C198" s="4"/>
     </row>
-    <row r="199" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="199" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C199" s="4"/>
     </row>
-    <row r="200" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="200" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C200" s="4"/>
     </row>
-    <row r="201" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="201" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C201" s="4"/>
     </row>
-    <row r="202" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="202" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C202" s="4"/>
     </row>
-    <row r="203" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="203" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C203" s="4"/>
     </row>
-    <row r="204" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="204" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C204" s="4"/>
     </row>
-    <row r="205" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="205" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C205" s="4"/>
     </row>
-    <row r="206" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="206" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C206" s="4"/>
     </row>
-    <row r="207" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="207" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C207" s="4"/>
     </row>
-    <row r="208" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="208" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C208" s="4"/>
     </row>
-    <row r="209" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="209" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C209" s="4"/>
     </row>
-    <row r="210" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="210" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C210" s="4"/>
     </row>
-    <row r="211" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="211" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C211" s="4"/>
     </row>
-    <row r="212" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="212" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C212" s="4"/>
     </row>
-    <row r="213" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="213" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C213" s="4"/>
     </row>
-    <row r="214" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="214" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C214" s="4"/>
     </row>
-    <row r="215" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="215" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C215" s="4"/>
     </row>
-    <row r="216" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="216" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C216" s="4"/>
     </row>
-    <row r="217" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="217" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C217" s="4"/>
     </row>
-    <row r="218" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="218" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C218" s="4"/>
     </row>
-    <row r="219" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="219" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C219" s="4"/>
     </row>
-    <row r="220" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="220" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C220" s="4"/>
     </row>
-    <row r="221" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="221" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C221" s="4"/>
     </row>
-    <row r="222" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="222" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C222" s="4"/>
     </row>
-    <row r="223" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="223" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C223" s="4"/>
     </row>
-    <row r="224" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="224" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C224" s="4"/>
     </row>
-    <row r="225" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="225" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C225" s="4"/>
     </row>
-    <row r="226" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="226" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C226" s="4"/>
     </row>
-    <row r="227" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="227" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C227" s="4"/>
     </row>
-    <row r="228" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="228" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C228" s="4"/>
     </row>
-    <row r="229" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="229" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C229" s="4"/>
     </row>
-    <row r="230" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="230" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C230" s="4"/>
     </row>
-    <row r="231" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="231" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C231" s="4"/>
     </row>
-    <row r="232" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="232" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C232" s="4"/>
     </row>
-    <row r="233" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="233" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C233" s="4"/>
     </row>
-    <row r="234" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="234" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C234" s="4"/>
     </row>
-    <row r="235" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="235" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C235" s="4"/>
     </row>
-    <row r="236" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="236" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C236" s="4"/>
     </row>
-    <row r="237" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="237" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C237" s="4"/>
     </row>
-    <row r="238" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="238" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C238" s="4"/>
     </row>
-    <row r="239" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="239" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C239" s="4"/>
     </row>
-    <row r="240" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="240" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C240" s="4"/>
     </row>
-    <row r="241" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="241" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C241" s="4"/>
     </row>
-    <row r="242" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="242" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C242" s="4"/>
     </row>
-    <row r="243" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="243" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C243" s="4"/>
     </row>
-    <row r="244" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="244" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C244" s="4"/>
     </row>
-    <row r="245" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="245" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C245" s="4"/>
     </row>
-    <row r="246" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="246" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C246" s="4"/>
     </row>
-    <row r="247" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="247" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C247" s="4"/>
     </row>
-    <row r="248" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="248" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C248" s="4"/>
     </row>
-    <row r="249" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="249" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C249" s="4"/>
     </row>
-    <row r="250" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="250" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C250" s="4"/>
     </row>
-    <row r="251" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="251" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C251" s="4"/>
     </row>
-    <row r="252" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="252" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C252" s="4"/>
     </row>
-    <row r="253" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="253" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C253" s="4"/>
     </row>
-    <row r="254" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="254" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C254" s="4"/>
     </row>
-    <row r="255" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="255" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C255" s="4"/>
     </row>
-    <row r="256" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="256" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C256" s="4"/>
     </row>
-    <row r="257" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="257" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C257" s="4"/>
     </row>
-    <row r="258" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="258" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C258" s="4"/>
     </row>
-    <row r="259" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="259" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C259" s="4"/>
     </row>
-    <row r="260" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="260" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C260" s="4"/>
     </row>
-    <row r="261" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="261" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C261" s="4"/>
     </row>
-    <row r="262" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="262" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C262" s="4"/>
     </row>
-    <row r="263" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="263" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C263" s="4"/>
     </row>
-    <row r="264" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="264" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C264" s="4"/>
     </row>
-    <row r="265" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="265" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C265" s="4"/>
     </row>
-    <row r="266" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="266" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C266" s="4"/>
     </row>
-    <row r="267" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="267" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C267" s="4"/>
     </row>
-    <row r="268" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="268" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C268" s="4"/>
     </row>
-    <row r="269" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="269" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C269" s="4"/>
     </row>
-    <row r="270" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="270" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C270" s="4"/>
     </row>
-    <row r="271" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="271" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C271" s="4"/>
     </row>
-    <row r="272" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="272" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C272" s="4"/>
     </row>
-    <row r="273" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="273" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C273" s="4"/>
     </row>
-    <row r="274" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="274" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C274" s="4"/>
     </row>
-    <row r="275" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="275" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C275" s="4"/>
     </row>
-    <row r="276" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="276" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C276" s="4"/>
     </row>
-    <row r="277" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="277" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C277" s="4"/>
     </row>
-    <row r="278" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="278" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C278" s="4"/>
     </row>
-    <row r="279" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="279" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C279" s="4"/>
     </row>
-    <row r="280" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="280" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C280" s="4"/>
     </row>
-    <row r="281" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="281" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C281" s="4"/>
     </row>
-    <row r="282" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="282" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C282" s="4"/>
     </row>
-    <row r="283" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="283" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C283" s="4"/>
     </row>
-    <row r="284" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="284" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C284" s="4"/>
     </row>
-    <row r="285" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="285" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C285" s="4"/>
     </row>
-    <row r="286" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="286" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C286" s="4"/>
     </row>
-    <row r="287" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="287" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C287" s="4"/>
     </row>
-    <row r="288" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="288" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C288" s="4"/>
     </row>
-    <row r="289" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="289" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C289" s="4"/>
     </row>
-    <row r="290" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="290" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C290" s="4"/>
     </row>
-    <row r="291" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="291" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C291" s="4"/>
     </row>
-    <row r="292" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="292" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C292" s="4"/>
     </row>
-    <row r="293" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="293" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C293" s="4"/>
     </row>
-    <row r="294" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="294" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C294" s="4"/>
     </row>
-    <row r="295" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="295" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C295" s="4"/>
     </row>
-    <row r="296" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="296" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C296" s="4"/>
     </row>
-    <row r="297" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="297" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C297" s="4"/>
     </row>
-    <row r="298" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="298" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C298" s="4"/>
     </row>
-    <row r="299" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="299" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C299" s="4"/>
     </row>
-    <row r="300" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="300" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C300" s="4"/>
     </row>
-    <row r="301" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="301" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C301" s="4"/>
     </row>
-    <row r="302" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="302" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C302" s="4"/>
     </row>
-    <row r="303" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="303" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C303" s="4"/>
     </row>
-    <row r="304" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="304" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C304" s="4"/>
     </row>
-    <row r="305" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="305" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C305" s="4"/>
     </row>
-    <row r="306" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="306" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C306" s="4"/>
     </row>
-    <row r="307" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="307" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C307" s="4"/>
     </row>
-    <row r="308" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="308" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C308" s="4"/>
     </row>
-    <row r="309" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="309" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C309" s="4"/>
     </row>
-    <row r="310" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="310" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C310" s="4"/>
     </row>
-    <row r="311" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="311" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C311" s="4"/>
     </row>
-    <row r="312" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="312" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C312" s="4"/>
     </row>
-    <row r="313" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="313" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C313" s="4"/>
     </row>
-    <row r="314" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="314" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C314" s="4"/>
     </row>
-    <row r="315" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="315" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C315" s="4"/>
     </row>
-    <row r="316" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="316" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C316" s="4"/>
     </row>
-    <row r="317" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="317" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C317" s="4"/>
     </row>
-    <row r="318" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="318" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C318" s="4"/>
     </row>
-    <row r="319" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="319" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C319" s="4"/>
     </row>
-    <row r="320" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="320" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C320" s="4"/>
     </row>
-    <row r="321" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="321" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C321" s="4"/>
     </row>
-    <row r="322" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="322" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C322" s="4"/>
     </row>
-    <row r="323" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="323" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C323" s="4"/>
     </row>
-    <row r="324" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="324" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C324" s="4"/>
     </row>
-    <row r="325" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="325" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C325" s="4"/>
     </row>
-    <row r="326" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="326" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C326" s="4"/>
     </row>
-    <row r="327" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="327" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C327" s="4"/>
     </row>
-    <row r="328" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="328" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C328" s="4"/>
     </row>
-    <row r="329" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="329" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C329" s="4"/>
     </row>
-    <row r="330" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="330" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C330" s="4"/>
     </row>
-    <row r="331" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="331" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C331" s="4"/>
     </row>
-    <row r="332" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="332" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C332" s="4"/>
     </row>
-    <row r="333" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="333" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C333" s="4"/>
     </row>
-    <row r="334" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="334" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C334" s="4"/>
     </row>
-    <row r="335" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="335" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C335" s="4"/>
     </row>
-    <row r="336" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="336" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C336" s="4"/>
     </row>
-    <row r="337" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="337" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C337" s="4"/>
     </row>
-    <row r="338" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="338" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C338" s="4"/>
     </row>
-    <row r="339" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="339" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C339" s="4"/>
     </row>
-    <row r="340" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="340" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C340" s="4"/>
     </row>
-    <row r="341" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="341" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C341" s="4"/>
     </row>
-    <row r="342" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="342" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C342" s="4"/>
     </row>
-    <row r="343" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="343" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C343" s="4"/>
     </row>
-    <row r="344" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="344" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C344" s="4"/>
     </row>
-    <row r="345" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="345" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C345" s="4"/>
     </row>
-    <row r="346" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="346" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C346" s="4"/>
     </row>
-    <row r="347" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="347" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C347" s="4"/>
     </row>
-    <row r="348" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="348" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C348" s="4"/>
     </row>
-    <row r="349" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="349" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C349" s="4"/>
     </row>
-    <row r="350" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="350" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C350" s="4"/>
     </row>
-    <row r="351" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="351" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C351" s="4"/>
     </row>
-    <row r="352" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="352" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C352" s="4"/>
     </row>
-    <row r="353" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="353" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C353" s="4"/>
     </row>
-    <row r="354" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="354" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C354" s="4"/>
     </row>
-    <row r="355" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="355" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C355" s="4"/>
     </row>
-    <row r="356" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="356" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C356" s="4"/>
     </row>
-    <row r="357" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="357" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C357" s="4"/>
     </row>
-    <row r="358" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="358" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C358" s="4"/>
     </row>
-    <row r="359" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="359" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C359" s="4"/>
     </row>
-    <row r="360" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="360" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C360" s="4"/>
     </row>
-    <row r="361" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="361" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C361" s="4"/>
     </row>
-    <row r="362" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="362" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C362" s="4"/>
     </row>
-    <row r="363" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="363" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C363" s="4"/>
     </row>
-    <row r="364" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="364" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C364" s="4"/>
     </row>
-    <row r="365" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="365" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C365" s="4"/>
     </row>
-    <row r="366" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="366" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C366" s="4"/>
     </row>
-    <row r="367" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="367" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C367" s="4"/>
     </row>
-    <row r="368" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="368" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C368" s="4"/>
     </row>
-    <row r="369" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="369" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C369" s="4"/>
     </row>
-    <row r="370" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="370" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C370" s="4"/>
     </row>
-    <row r="371" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="371" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C371" s="4"/>
     </row>
-    <row r="372" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="372" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C372" s="4"/>
     </row>
-    <row r="373" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="373" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C373" s="4"/>
     </row>
-    <row r="374" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="374" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C374" s="4"/>
     </row>
-    <row r="375" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="375" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C375" s="4"/>
     </row>
-    <row r="376" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="376" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C376" s="4"/>
     </row>
-    <row r="377" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="377" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C377" s="4"/>
     </row>
-    <row r="378" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="378" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C378" s="4"/>
     </row>
-    <row r="379" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="379" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C379" s="4"/>
     </row>
-    <row r="380" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="380" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C380" s="4"/>
     </row>
-    <row r="381" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="381" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C381" s="4"/>
     </row>
-    <row r="382" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="382" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C382" s="4"/>
     </row>
-    <row r="383" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="383" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C383" s="4"/>
     </row>
-    <row r="384" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="384" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C384" s="4"/>
     </row>
-    <row r="385" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="385" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C385" s="4"/>
     </row>
-    <row r="386" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="386" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C386" s="4"/>
     </row>
-    <row r="387" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="387" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C387" s="4"/>
     </row>
-    <row r="388" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="388" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C388" s="4"/>
     </row>
-    <row r="389" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="389" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C389" s="4"/>
     </row>
-    <row r="390" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="390" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C390" s="4"/>
     </row>
-    <row r="391" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="391" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C391" s="4"/>
     </row>
-    <row r="392" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="392" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C392" s="4"/>
     </row>
-    <row r="393" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="393" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C393" s="4"/>
     </row>
-    <row r="394" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="394" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C394" s="4"/>
     </row>
-    <row r="395" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="395" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C395" s="4"/>
     </row>
-    <row r="396" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="396" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C396" s="4"/>
     </row>
-    <row r="397" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="397" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C397" s="4"/>
     </row>
-    <row r="398" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="398" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C398" s="4"/>
     </row>
-    <row r="399" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="399" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C399" s="4"/>
     </row>
-    <row r="400" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="400" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C400" s="4"/>
     </row>
-    <row r="401" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="401" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C401" s="4"/>
     </row>
-    <row r="402" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="402" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C402" s="4"/>
     </row>
-    <row r="403" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="403" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C403" s="4"/>
     </row>
-    <row r="404" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="404" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C404" s="4"/>
     </row>
-    <row r="405" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="405" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C405" s="4"/>
     </row>
-    <row r="406" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="406" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C406" s="4"/>
     </row>
-    <row r="407" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="407" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C407" s="4"/>
     </row>
-    <row r="408" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="408" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C408" s="4"/>
     </row>
-    <row r="409" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="409" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C409" s="4"/>
     </row>
-    <row r="410" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="410" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C410" s="4"/>
     </row>
-    <row r="411" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="411" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C411" s="4"/>
     </row>
-    <row r="412" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="412" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C412" s="4"/>
     </row>
-    <row r="413" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="413" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C413" s="4"/>
     </row>
-    <row r="414" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="414" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C414" s="4"/>
     </row>
-    <row r="415" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="415" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C415" s="4"/>
     </row>
-    <row r="416" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="416" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C416" s="4"/>
     </row>
-    <row r="417" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="417" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C417" s="4"/>
     </row>
-    <row r="418" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="418" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C418" s="4"/>
     </row>
-    <row r="419" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="419" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C419" s="4"/>
     </row>
-    <row r="420" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="420" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C420" s="4"/>
     </row>
-    <row r="421" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="421" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C421" s="4"/>
     </row>
-    <row r="422" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="422" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C422" s="4"/>
     </row>
-    <row r="423" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="423" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C423" s="4"/>
     </row>
-    <row r="424" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="424" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C424" s="4"/>
     </row>
-    <row r="425" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="425" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C425" s="4"/>
     </row>
-    <row r="426" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="426" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C426" s="4"/>
     </row>
-    <row r="427" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="427" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C427" s="4"/>
     </row>
-    <row r="428" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="428" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C428" s="4"/>
     </row>
-    <row r="429" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="429" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C429" s="4"/>
     </row>
-    <row r="430" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="430" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C430" s="4"/>
     </row>
-    <row r="431" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="431" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C431" s="4"/>
     </row>
-    <row r="432" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="432" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C432" s="4"/>
     </row>
-    <row r="433" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="433" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C433" s="4"/>
     </row>
-    <row r="434" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="434" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C434" s="4"/>
     </row>
-    <row r="435" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="435" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C435" s="4"/>
     </row>
-    <row r="436" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="436" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C436" s="4"/>
     </row>
-    <row r="437" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="437" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C437" s="4"/>
     </row>
-    <row r="438" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="438" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C438" s="4"/>
     </row>
-    <row r="439" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="439" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C439" s="4"/>
     </row>
-    <row r="440" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="440" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C440" s="4"/>
     </row>
-    <row r="441" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="441" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C441" s="4"/>
     </row>
-    <row r="442" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="442" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C442" s="4"/>
     </row>
-    <row r="443" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="443" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C443" s="4"/>
     </row>
-    <row r="444" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="444" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C444" s="4"/>
     </row>
-    <row r="445" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="445" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C445" s="4"/>
     </row>
-    <row r="446" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="446" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C446" s="4"/>
     </row>
-    <row r="447" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="447" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C447" s="4"/>
     </row>
-    <row r="448" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="448" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C448" s="4"/>
     </row>
-    <row r="449" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="449" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C449" s="4"/>
     </row>
-    <row r="450" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="450" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C450" s="4"/>
     </row>
-    <row r="451" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="451" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C451" s="4"/>
     </row>
-    <row r="452" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="452" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C452" s="4"/>
     </row>
-    <row r="453" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="453" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C453" s="4"/>
     </row>
-    <row r="454" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="454" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C454" s="4"/>
     </row>
-    <row r="455" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="455" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C455" s="4"/>
     </row>
-    <row r="456" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="456" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C456" s="4"/>
     </row>
-    <row r="457" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="457" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C457" s="4"/>
     </row>
-    <row r="458" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="458" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C458" s="4"/>
     </row>
-    <row r="459" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="459" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C459" s="4"/>
     </row>
-    <row r="460" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="460" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C460" s="4"/>
     </row>
-    <row r="461" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="461" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C461" s="4"/>
     </row>
-    <row r="462" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="462" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C462" s="4"/>
     </row>
-    <row r="463" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="463" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C463" s="4"/>
     </row>
-    <row r="464" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="464" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C464" s="4"/>
     </row>
-    <row r="465" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="465" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C465" s="4"/>
     </row>
-    <row r="466" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="466" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C466" s="4"/>
     </row>
-    <row r="467" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="467" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C467" s="4"/>
     </row>
-    <row r="468" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="468" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C468" s="4"/>
     </row>
-    <row r="469" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="469" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C469" s="4"/>
     </row>
-    <row r="470" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="470" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C470" s="4"/>
     </row>
-    <row r="471" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="471" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C471" s="4"/>
     </row>
-    <row r="472" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="472" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C472" s="4"/>
     </row>
-    <row r="473" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="473" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C473" s="4"/>
     </row>
-    <row r="474" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="474" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C474" s="4"/>
     </row>
-    <row r="475" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="475" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C475" s="4"/>
     </row>
-    <row r="476" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="476" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C476" s="4"/>
     </row>
-    <row r="477" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="477" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C477" s="4"/>
     </row>
-    <row r="478" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="478" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C478" s="4"/>
     </row>
-    <row r="479" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="479" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C479" s="4"/>
     </row>
-    <row r="480" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="480" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C480" s="4"/>
     </row>
-    <row r="481" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="481" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C481" s="4"/>
     </row>
-    <row r="482" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="482" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C482" s="4"/>
     </row>
-    <row r="483" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="483" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C483" s="4"/>
     </row>
-    <row r="484" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="484" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C484" s="4"/>
     </row>
-    <row r="485" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="485" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C485" s="4"/>
     </row>
-    <row r="486" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="486" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C486" s="4"/>
     </row>
-    <row r="487" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="487" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C487" s="4"/>
     </row>
-    <row r="488" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="488" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C488" s="4"/>
     </row>
-    <row r="489" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="489" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C489" s="4"/>
     </row>
-    <row r="490" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="490" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C490" s="4"/>
     </row>
-    <row r="491" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="491" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C491" s="4"/>
     </row>
-    <row r="492" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="492" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C492" s="4"/>
     </row>
-    <row r="493" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="493" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C493" s="4"/>
     </row>
-    <row r="494" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="494" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C494" s="4"/>
     </row>
-    <row r="495" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="495" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C495" s="4"/>
     </row>
-    <row r="496" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="496" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C496" s="4"/>
     </row>
-    <row r="497" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="497" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C497" s="4"/>
     </row>
-    <row r="498" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="498" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C498" s="4"/>
     </row>
-    <row r="499" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="499" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C499" s="4"/>
     </row>
-    <row r="500" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="500" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C500" s="4"/>
     </row>
-    <row r="501" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="501" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C501" s="4"/>
     </row>
-    <row r="502" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="502" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C502" s="4"/>
     </row>
-    <row r="503" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="503" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C503" s="4"/>
     </row>
-    <row r="504" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="504" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C504" s="4"/>
     </row>
-    <row r="505" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="505" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C505" s="4"/>
     </row>
-    <row r="506" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="506" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C506" s="4"/>
     </row>
-    <row r="507" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="507" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C507" s="4"/>
     </row>
-    <row r="508" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="508" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C508" s="4"/>
     </row>
-    <row r="509" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="509" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C509" s="4"/>
     </row>
-    <row r="510" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="510" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C510" s="4"/>
     </row>
-    <row r="511" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="511" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C511" s="4"/>
     </row>
-    <row r="512" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="512" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C512" s="4"/>
     </row>
-    <row r="513" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="513" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C513" s="4"/>
     </row>
-    <row r="514" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="514" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C514" s="4"/>
     </row>
-    <row r="515" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="515" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C515" s="4"/>
     </row>
-    <row r="516" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="516" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C516" s="4"/>
     </row>
-    <row r="517" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="517" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C517" s="4"/>
     </row>
-    <row r="518" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="518" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C518" s="4"/>
     </row>
-    <row r="519" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="519" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C519" s="4"/>
     </row>
-    <row r="520" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="520" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C520" s="4"/>
     </row>
-    <row r="521" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="521" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C521" s="4"/>
     </row>
-    <row r="522" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="522" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C522" s="4"/>
     </row>
-    <row r="523" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="523" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C523" s="4"/>
     </row>
-    <row r="524" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="524" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C524" s="4"/>
     </row>
-    <row r="525" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="525" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C525" s="4"/>
     </row>
-    <row r="526" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="526" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C526" s="4"/>
     </row>
-    <row r="527" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="527" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C527" s="4"/>
     </row>
-    <row r="528" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="528" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C528" s="4"/>
     </row>
-    <row r="529" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="529" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C529" s="4"/>
     </row>
-    <row r="530" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="530" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C530" s="4"/>
     </row>
-    <row r="531" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="531" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C531" s="4"/>
     </row>
-    <row r="532" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="532" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C532" s="4"/>
     </row>
-    <row r="533" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="533" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C533" s="4"/>
     </row>
-    <row r="534" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="534" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C534" s="4"/>
     </row>
-    <row r="535" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="535" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C535" s="4"/>
     </row>
-    <row r="536" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="536" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C536" s="4"/>
     </row>
-    <row r="537" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="537" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C537" s="4"/>
     </row>
-    <row r="538" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="538" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C538" s="4"/>
     </row>
-    <row r="539" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="539" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C539" s="4"/>
     </row>
-    <row r="540" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="540" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C540" s="4"/>
     </row>
-    <row r="541" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="541" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C541" s="4"/>
     </row>
-    <row r="542" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="542" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C542" s="4"/>
     </row>
-    <row r="543" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="543" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C543" s="4"/>
     </row>
-    <row r="544" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="544" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C544" s="4"/>
     </row>
-    <row r="545" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="545" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C545" s="4"/>
     </row>
-    <row r="546" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="546" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C546" s="4"/>
     </row>
-    <row r="547" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="547" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C547" s="4"/>
     </row>
-    <row r="548" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="548" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C548" s="4"/>
     </row>
-    <row r="549" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="549" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C549" s="4"/>
     </row>
-    <row r="550" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="550" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C550" s="4"/>
     </row>
-    <row r="551" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="551" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C551" s="4"/>
     </row>
-    <row r="552" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="552" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C552" s="4"/>
     </row>
-    <row r="553" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="553" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C553" s="4"/>
     </row>
-    <row r="554" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="554" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C554" s="4"/>
     </row>
-    <row r="555" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="555" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C555" s="4"/>
     </row>
-    <row r="556" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="556" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C556" s="4"/>
     </row>
-    <row r="557" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="557" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C557" s="4"/>
     </row>
-    <row r="558" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="558" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C558" s="4"/>
     </row>
-    <row r="559" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="559" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C559" s="4"/>
     </row>
-    <row r="560" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="560" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C560" s="4"/>
     </row>
-    <row r="561" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="561" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C561" s="4"/>
     </row>
-    <row r="562" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="562" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C562" s="4"/>
     </row>
-    <row r="563" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="563" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C563" s="4"/>
     </row>
-    <row r="564" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="564" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C564" s="4"/>
     </row>
-    <row r="565" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="565" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C565" s="4"/>
     </row>
-    <row r="566" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="566" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C566" s="4"/>
     </row>
-    <row r="567" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="567" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C567" s="4"/>
     </row>
-    <row r="568" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="568" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C568" s="4"/>
     </row>
-    <row r="569" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="569" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C569" s="4"/>
     </row>
-    <row r="570" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="570" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C570" s="4"/>
     </row>
-    <row r="571" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="571" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C571" s="4"/>
     </row>
-    <row r="572" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="572" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C572" s="4"/>
     </row>
-    <row r="573" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="573" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C573" s="4"/>
     </row>
-    <row r="574" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="574" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C574" s="4"/>
     </row>
-    <row r="575" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="575" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C575" s="4"/>
     </row>
-    <row r="576" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="576" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C576" s="4"/>
     </row>
-    <row r="577" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="577" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C577" s="4"/>
     </row>
-    <row r="578" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="578" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C578" s="4"/>
     </row>
-    <row r="579" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="579" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C579" s="4"/>
     </row>
-    <row r="580" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="580" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C580" s="4"/>
     </row>
-    <row r="581" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="581" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C581" s="4"/>
     </row>
-    <row r="582" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="582" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C582" s="4"/>
     </row>
-    <row r="583" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="583" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C583" s="4"/>
     </row>
-    <row r="584" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="584" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C584" s="4"/>
     </row>
-    <row r="585" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="585" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C585" s="4"/>
     </row>
-    <row r="586" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="586" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C586" s="4"/>
     </row>
-    <row r="587" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="587" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C587" s="4"/>
     </row>
-    <row r="588" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="588" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C588" s="4"/>
     </row>
-    <row r="589" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="589" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C589" s="4"/>
     </row>
-    <row r="590" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="590" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C590" s="4"/>
     </row>
-    <row r="591" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="591" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C591" s="4"/>
     </row>
-    <row r="592" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="592" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C592" s="4"/>
     </row>
-    <row r="593" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="593" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C593" s="4"/>
     </row>
-    <row r="594" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="594" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C594" s="4"/>
     </row>
-    <row r="595" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="595" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C595" s="4"/>
     </row>
-    <row r="596" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="596" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C596" s="4"/>
     </row>
-    <row r="597" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="597" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C597" s="4"/>
     </row>
-    <row r="598" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="598" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C598" s="4"/>
     </row>
-    <row r="599" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="599" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C599" s="4"/>
     </row>
-    <row r="600" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="600" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C600" s="4"/>
     </row>
-    <row r="601" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="601" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C601" s="4"/>
     </row>
-    <row r="602" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="602" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C602" s="4"/>
     </row>
-    <row r="603" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="603" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C603" s="4"/>
     </row>
-    <row r="604" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="604" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C604" s="4"/>
     </row>
-    <row r="605" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="605" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C605" s="4"/>
     </row>
-    <row r="606" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="606" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C606" s="4"/>
     </row>
-    <row r="607" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="607" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C607" s="4"/>
     </row>
-    <row r="608" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="608" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C608" s="4"/>
     </row>
-    <row r="609" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="609" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C609" s="4"/>
     </row>
-    <row r="610" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="610" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C610" s="4"/>
     </row>
-    <row r="611" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="611" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C611" s="4"/>
     </row>
-    <row r="612" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="612" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C612" s="4"/>
     </row>
-    <row r="613" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="613" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C613" s="4"/>
     </row>
-    <row r="614" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="614" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C614" s="4"/>
     </row>
-    <row r="615" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="615" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C615" s="4"/>
     </row>
-    <row r="616" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="616" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C616" s="4"/>
     </row>
-    <row r="617" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="617" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C617" s="4"/>
     </row>
-    <row r="618" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="618" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C618" s="4"/>
     </row>
-    <row r="619" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="619" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C619" s="4"/>
     </row>
-    <row r="620" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="620" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C620" s="4"/>
     </row>
-    <row r="621" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="621" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C621" s="4"/>
     </row>
-    <row r="622" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="622" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C622" s="4"/>
     </row>
-    <row r="623" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="623" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C623" s="4"/>
     </row>
-    <row r="624" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="624" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C624" s="4"/>
     </row>
-    <row r="625" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="625" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C625" s="4"/>
     </row>
-    <row r="626" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="626" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C626" s="4"/>
     </row>
-    <row r="627" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="627" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C627" s="4"/>
     </row>
-    <row r="628" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="628" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C628" s="4"/>
     </row>
-    <row r="629" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="629" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C629" s="4"/>
     </row>
-    <row r="630" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="630" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C630" s="4"/>
     </row>
-    <row r="631" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="631" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C631" s="4"/>
     </row>
-    <row r="632" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="632" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C632" s="4"/>
     </row>
-    <row r="633" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="633" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C633" s="4"/>
     </row>
-    <row r="634" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="634" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C634" s="4"/>
     </row>
-    <row r="635" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="635" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C635" s="4"/>
     </row>
-    <row r="636" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="636" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C636" s="4"/>
     </row>
-    <row r="637" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="637" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C637" s="4"/>
     </row>
-    <row r="638" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="638" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C638" s="4"/>
     </row>
-    <row r="639" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="639" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C639" s="4"/>
     </row>
-    <row r="640" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="640" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C640" s="4"/>
     </row>
-    <row r="641" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="641" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C641" s="4"/>
     </row>
-    <row r="642" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="642" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C642" s="4"/>
     </row>
-    <row r="643" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="643" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C643" s="4"/>
     </row>
-    <row r="644" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="644" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C644" s="4"/>
     </row>
-    <row r="645" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="645" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C645" s="4"/>
     </row>
-    <row r="646" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="646" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C646" s="4"/>
     </row>
-    <row r="647" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="647" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C647" s="4"/>
     </row>
-    <row r="648" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="648" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C648" s="4"/>
     </row>
-    <row r="649" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="649" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C649" s="4"/>
     </row>
-    <row r="650" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="650" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C650" s="4"/>
     </row>
-    <row r="651" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="651" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C651" s="4"/>
     </row>
-    <row r="652" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="652" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C652" s="4"/>
     </row>
-    <row r="653" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="653" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C653" s="4"/>
     </row>
-    <row r="654" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="654" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C654" s="4"/>
     </row>
-    <row r="655" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="655" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C655" s="4"/>
     </row>
-    <row r="656" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="656" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C656" s="4"/>
     </row>
-    <row r="657" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="657" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C657" s="4"/>
     </row>
-    <row r="658" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="658" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C658" s="4"/>
     </row>
-    <row r="659" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="659" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C659" s="4"/>
     </row>
-    <row r="660" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="660" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C660" s="4"/>
     </row>
-    <row r="661" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="661" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C661" s="4"/>
     </row>
-    <row r="662" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="662" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C662" s="4"/>
     </row>
-    <row r="663" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="663" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C663" s="4"/>
     </row>
-    <row r="664" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="664" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C664" s="4"/>
     </row>
-    <row r="665" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="665" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C665" s="4"/>
     </row>
-    <row r="666" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="666" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C666" s="4"/>
     </row>
-    <row r="667" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="667" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C667" s="4"/>
     </row>
-    <row r="668" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="668" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C668" s="4"/>
     </row>
-    <row r="669" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="669" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C669" s="4"/>
     </row>
-    <row r="670" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="670" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C670" s="4"/>
     </row>
-    <row r="671" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="671" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C671" s="4"/>
     </row>
-    <row r="672" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="672" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C672" s="4"/>
     </row>
-    <row r="673" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="673" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C673" s="4"/>
     </row>
-    <row r="674" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="674" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C674" s="4"/>
     </row>
-    <row r="675" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="675" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C675" s="4"/>
     </row>
-    <row r="676" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="676" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C676" s="4"/>
     </row>
-    <row r="677" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="677" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C677" s="4"/>
     </row>
-    <row r="678" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="678" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C678" s="4"/>
     </row>
-    <row r="679" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="679" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C679" s="4"/>
     </row>
-    <row r="680" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="680" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C680" s="4"/>
     </row>
-    <row r="681" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="681" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C681" s="4"/>
     </row>
-    <row r="682" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="682" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C682" s="4"/>
     </row>
-    <row r="683" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="683" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C683" s="4"/>
     </row>
-    <row r="684" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="684" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C684" s="4"/>
     </row>
-    <row r="685" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="685" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C685" s="4"/>
     </row>
-    <row r="686" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="686" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C686" s="4"/>
     </row>
-    <row r="687" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="687" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C687" s="4"/>
     </row>
-    <row r="688" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="688" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C688" s="4"/>
     </row>
-    <row r="689" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="689" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C689" s="4"/>
     </row>
-    <row r="690" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="690" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C690" s="4"/>
     </row>
-    <row r="691" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="691" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C691" s="4"/>
     </row>
-    <row r="692" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="692" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C692" s="4"/>
     </row>
-    <row r="693" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="693" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C693" s="4"/>
     </row>
-    <row r="694" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="694" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C694" s="4"/>
     </row>
-    <row r="695" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="695" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C695" s="4"/>
     </row>
-    <row r="696" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="696" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C696" s="4"/>
     </row>
-    <row r="697" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="697" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C697" s="4"/>
     </row>
-    <row r="698" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="698" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C698" s="4"/>
     </row>
-    <row r="699" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="699" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C699" s="4"/>
     </row>
-    <row r="700" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="700" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C700" s="4"/>
     </row>
-    <row r="701" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="701" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C701" s="4"/>
     </row>
-    <row r="702" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="702" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C702" s="4"/>
     </row>
-    <row r="703" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="703" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C703" s="4"/>
     </row>
-    <row r="704" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="704" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C704" s="4"/>
     </row>
-    <row r="705" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="705" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C705" s="4"/>
     </row>
-    <row r="706" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="706" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C706" s="4"/>
     </row>
-    <row r="707" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="707" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C707" s="4"/>
     </row>
-    <row r="708" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="708" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C708" s="4"/>
     </row>
-    <row r="709" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="709" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C709" s="4"/>
     </row>
-    <row r="710" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="710" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C710" s="4"/>
     </row>
-    <row r="711" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="711" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C711" s="4"/>
     </row>
-    <row r="712" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="712" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C712" s="4"/>
     </row>
-    <row r="713" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="713" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C713" s="4"/>
     </row>
-    <row r="714" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="714" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C714" s="4"/>
     </row>
-    <row r="715" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="715" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C715" s="4"/>
     </row>
-    <row r="716" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="716" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C716" s="4"/>
     </row>
-    <row r="717" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="717" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C717" s="4"/>
     </row>
-    <row r="718" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="718" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C718" s="4"/>
     </row>
-    <row r="719" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="719" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C719" s="4"/>
     </row>
-    <row r="720" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="720" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C720" s="4"/>
     </row>
-    <row r="721" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="721" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C721" s="4"/>
     </row>
-    <row r="722" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="722" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C722" s="4"/>
     </row>
-    <row r="723" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="723" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C723" s="4"/>
     </row>
-    <row r="724" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="724" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C724" s="4"/>
     </row>
-    <row r="725" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="725" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C725" s="4"/>
     </row>
-    <row r="726" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="726" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C726" s="4"/>
     </row>
-    <row r="727" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="727" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C727" s="4"/>
     </row>
-    <row r="728" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="728" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C728" s="4"/>
     </row>
-    <row r="729" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="729" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C729" s="4"/>
     </row>
-    <row r="730" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="730" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C730" s="4"/>
     </row>
-    <row r="731" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="731" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C731" s="4"/>
     </row>
-    <row r="732" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="732" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C732" s="4"/>
     </row>
-    <row r="733" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="733" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C733" s="4"/>
     </row>
-    <row r="734" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="734" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C734" s="4"/>
     </row>
-    <row r="735" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="735" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C735" s="4"/>
     </row>
-    <row r="736" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="736" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C736" s="4"/>
     </row>
-    <row r="737" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="737" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C737" s="4"/>
     </row>
-    <row r="738" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="738" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C738" s="4"/>
     </row>
-    <row r="739" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="739" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C739" s="4"/>
     </row>
-    <row r="740" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="740" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C740" s="4"/>
     </row>
-    <row r="741" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="741" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C741" s="4"/>
     </row>
-    <row r="742" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="742" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C742" s="4"/>
     </row>
-    <row r="743" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="743" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C743" s="4"/>
     </row>
-    <row r="744" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="744" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C744" s="4"/>
     </row>
-    <row r="745" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="745" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C745" s="4"/>
     </row>
-    <row r="746" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="746" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C746" s="4"/>
     </row>
-    <row r="747" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="747" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C747" s="4"/>
     </row>
-    <row r="748" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="748" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C748" s="4"/>
     </row>
-    <row r="749" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="749" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C749" s="4"/>
     </row>
-    <row r="750" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="750" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C750" s="4"/>
     </row>
-    <row r="751" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="751" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C751" s="4"/>
     </row>
-    <row r="752" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="752" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C752" s="4"/>
     </row>
-    <row r="753" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="753" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C753" s="4"/>
     </row>
-    <row r="754" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="754" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C754" s="4"/>
     </row>
-    <row r="755" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="755" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C755" s="4"/>
     </row>
-    <row r="756" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="756" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C756" s="4"/>
     </row>
-    <row r="757" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="757" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C757" s="4"/>
     </row>
-    <row r="758" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="758" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C758" s="4"/>
     </row>
-    <row r="759" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="759" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C759" s="4"/>
     </row>
-    <row r="760" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="760" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C760" s="4"/>
     </row>
-    <row r="761" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="761" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C761" s="4"/>
     </row>
-    <row r="762" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="762" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C762" s="4"/>
     </row>
-    <row r="763" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="763" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C763" s="4"/>
     </row>
-    <row r="764" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="764" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C764" s="4"/>
     </row>
-    <row r="765" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="765" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C765" s="4"/>
     </row>
-    <row r="766" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="766" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C766" s="4"/>
     </row>
-    <row r="767" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="767" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C767" s="4"/>
     </row>
-    <row r="768" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="768" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C768" s="4"/>
     </row>
-    <row r="769" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="769" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C769" s="4"/>
     </row>
-    <row r="770" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="770" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C770" s="4"/>
     </row>
-    <row r="771" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="771" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C771" s="4"/>
     </row>
-    <row r="772" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="772" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C772" s="4"/>
     </row>
-    <row r="773" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="773" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C773" s="4"/>
     </row>
-    <row r="774" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="774" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C774" s="4"/>
     </row>
-    <row r="775" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="775" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C775" s="4"/>
     </row>
-    <row r="776" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="776" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C776" s="4"/>
     </row>
-    <row r="777" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="777" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C777" s="4"/>
     </row>
-    <row r="778" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="778" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C778" s="4"/>
     </row>
-    <row r="779" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="779" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C779" s="4"/>
     </row>
-    <row r="780" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="780" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C780" s="4"/>
     </row>
-    <row r="781" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="781" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C781" s="4"/>
     </row>
-    <row r="782" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="782" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C782" s="4"/>
     </row>
-    <row r="783" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="783" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C783" s="4"/>
     </row>
-    <row r="784" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="784" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C784" s="4"/>
     </row>
-    <row r="785" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="785" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C785" s="4"/>
     </row>
-    <row r="786" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="786" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C786" s="4"/>
     </row>
-    <row r="787" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="787" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C787" s="4"/>
     </row>
-    <row r="788" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="788" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C788" s="4"/>
     </row>
-    <row r="789" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="789" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C789" s="4"/>
     </row>
-    <row r="790" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="790" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C790" s="4"/>
     </row>
-    <row r="791" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="791" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C791" s="4"/>
     </row>
-    <row r="792" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="792" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C792" s="4"/>
     </row>
-    <row r="793" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="793" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C793" s="4"/>
     </row>
-    <row r="794" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="794" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C794" s="4"/>
     </row>
-    <row r="795" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="795" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C795" s="4"/>
     </row>
-    <row r="796" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="796" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C796" s="4"/>
     </row>
-    <row r="797" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="797" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C797" s="4"/>
     </row>
-    <row r="798" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="798" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C798" s="4"/>
     </row>
-    <row r="799" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="799" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C799" s="4"/>
     </row>
-    <row r="800" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="800" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C800" s="4"/>
     </row>
-    <row r="801" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="801" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C801" s="4"/>
     </row>
-    <row r="802" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="802" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C802" s="4"/>
     </row>
-    <row r="803" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="803" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C803" s="4"/>
     </row>
-    <row r="804" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="804" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C804" s="4"/>
     </row>
-    <row r="805" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="805" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C805" s="4"/>
     </row>
-    <row r="806" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="806" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C806" s="4"/>
     </row>
-    <row r="807" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="807" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C807" s="4"/>
     </row>
-    <row r="808" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="808" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C808" s="4"/>
     </row>
-    <row r="809" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="809" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C809" s="4"/>
     </row>
-    <row r="810" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="810" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C810" s="4"/>
     </row>
-    <row r="811" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="811" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C811" s="4"/>
     </row>
-    <row r="812" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="812" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C812" s="4"/>
     </row>
-    <row r="813" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="813" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C813" s="4"/>
     </row>
-    <row r="814" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="814" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C814" s="4"/>
     </row>
-    <row r="815" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="815" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C815" s="4"/>
     </row>
-    <row r="816" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="816" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C816" s="4"/>
     </row>
-    <row r="817" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="817" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C817" s="4"/>
     </row>
-    <row r="818" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="818" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C818" s="4"/>
     </row>
-    <row r="819" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="819" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C819" s="4"/>
     </row>
-    <row r="820" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="820" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C820" s="4"/>
     </row>
-    <row r="821" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="821" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C821" s="4"/>
     </row>
-    <row r="822" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="822" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C822" s="4"/>
     </row>
-    <row r="823" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="823" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C823" s="4"/>
     </row>
-    <row r="824" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="824" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C824" s="4"/>
     </row>
-    <row r="825" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="825" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C825" s="4"/>
     </row>
-    <row r="826" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="826" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C826" s="4"/>
     </row>
-    <row r="827" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="827" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C827" s="4"/>
     </row>
-    <row r="828" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="828" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C828" s="4"/>
     </row>
-    <row r="829" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="829" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C829" s="4"/>
     </row>
-    <row r="830" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="830" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C830" s="4"/>
     </row>
-    <row r="831" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="831" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C831" s="4"/>
     </row>
-    <row r="832" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="832" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C832" s="4"/>
     </row>
-    <row r="833" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="833" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C833" s="4"/>
     </row>
-    <row r="834" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="834" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C834" s="4"/>
     </row>
-    <row r="835" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="835" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C835" s="4"/>
     </row>
-    <row r="836" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="836" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C836" s="4"/>
     </row>
-    <row r="837" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="837" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C837" s="4"/>
     </row>
-    <row r="838" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="838" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C838" s="4"/>
     </row>
-    <row r="839" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="839" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C839" s="4"/>
     </row>
-    <row r="840" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="840" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C840" s="4"/>
     </row>
-    <row r="841" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="841" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C841" s="4"/>
     </row>
-    <row r="842" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="842" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C842" s="4"/>
     </row>
-    <row r="843" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="843" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C843" s="4"/>
     </row>
-    <row r="844" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="844" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C844" s="4"/>
     </row>
-    <row r="845" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="845" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C845" s="4"/>
     </row>
-    <row r="846" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="846" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C846" s="4"/>
     </row>
-    <row r="847" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="847" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C847" s="4"/>
     </row>
-    <row r="848" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="848" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C848" s="4"/>
     </row>
-    <row r="849" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="849" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C849" s="4"/>
     </row>
-    <row r="850" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="850" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C850" s="4"/>
     </row>
-    <row r="851" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="851" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C851" s="4"/>
     </row>
-    <row r="852" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="852" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C852" s="4"/>
     </row>
-    <row r="853" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="853" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C853" s="4"/>
     </row>
-    <row r="854" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="854" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C854" s="4"/>
     </row>
-    <row r="855" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="855" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C855" s="4"/>
     </row>
-    <row r="856" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="856" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C856" s="4"/>
     </row>
-    <row r="857" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="857" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C857" s="4"/>
     </row>
-    <row r="858" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="858" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C858" s="4"/>
     </row>
-    <row r="859" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="859" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C859" s="4"/>
     </row>
-    <row r="860" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="860" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C860" s="4"/>
     </row>
-    <row r="861" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="861" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C861" s="4"/>
     </row>
-    <row r="862" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="862" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C862" s="4"/>
     </row>
-    <row r="863" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="863" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C863" s="4"/>
     </row>
-    <row r="864" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="864" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C864" s="4"/>
     </row>
-    <row r="865" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="865" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C865" s="4"/>
     </row>
-    <row r="866" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="866" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C866" s="4"/>
     </row>
-    <row r="867" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="867" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C867" s="4"/>
     </row>
-    <row r="868" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="868" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C868" s="4"/>
     </row>
-    <row r="869" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="869" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C869" s="4"/>
     </row>
-    <row r="870" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="870" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C870" s="4"/>
     </row>
-    <row r="871" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="871" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C871" s="4"/>
     </row>
-    <row r="872" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="872" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C872" s="4"/>
     </row>
-    <row r="873" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="873" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C873" s="4"/>
     </row>
-    <row r="874" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="874" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C874" s="4"/>
     </row>
-    <row r="875" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="875" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C875" s="4"/>
     </row>
-    <row r="876" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="876" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C876" s="4"/>
     </row>
-    <row r="877" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="877" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C877" s="4"/>
     </row>
-    <row r="878" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="878" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C878" s="4"/>
     </row>
-    <row r="879" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="879" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C879" s="4"/>
     </row>
-    <row r="880" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="880" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C880" s="4"/>
     </row>
-    <row r="881" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="881" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C881" s="4"/>
     </row>
-    <row r="882" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="882" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C882" s="4"/>
     </row>
-    <row r="883" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="883" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C883" s="4"/>
     </row>
-    <row r="884" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="884" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C884" s="4"/>
     </row>
-    <row r="885" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="885" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C885" s="4"/>
     </row>
-    <row r="886" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="886" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C886" s="4"/>
     </row>
-    <row r="887" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="887" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C887" s="4"/>
     </row>
-    <row r="888" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="888" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C888" s="4"/>
     </row>
-    <row r="889" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="889" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C889" s="4"/>
     </row>
-    <row r="890" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="890" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C890" s="4"/>
     </row>
-    <row r="891" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="891" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C891" s="4"/>
     </row>
-    <row r="892" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="892" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C892" s="4"/>
     </row>
-    <row r="893" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="893" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C893" s="4"/>
     </row>
-    <row r="894" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="894" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C894" s="4"/>
     </row>
-    <row r="895" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="895" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C895" s="4"/>
     </row>
-    <row r="896" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="896" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C896" s="4"/>
     </row>
-    <row r="897" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="897" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C897" s="4"/>
     </row>
-    <row r="898" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="898" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C898" s="4"/>
     </row>
-    <row r="899" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="899" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C899" s="4"/>
     </row>
-    <row r="900" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="900" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C900" s="4"/>
     </row>
-    <row r="901" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="901" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C901" s="4"/>
     </row>
-    <row r="902" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="902" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C902" s="4"/>
     </row>
-    <row r="903" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="903" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C903" s="4"/>
     </row>
-    <row r="904" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="904" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C904" s="4"/>
     </row>
-    <row r="905" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="905" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C905" s="4"/>
     </row>
-    <row r="906" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="906" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C906" s="4"/>
     </row>
-    <row r="907" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="907" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C907" s="4"/>
     </row>
-    <row r="908" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="908" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C908" s="4"/>
     </row>
-    <row r="909" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="909" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C909" s="4"/>
     </row>
-    <row r="910" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="910" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C910" s="4"/>
     </row>
-    <row r="911" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="911" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C911" s="4"/>
     </row>
-    <row r="912" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="912" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C912" s="4"/>
     </row>
-    <row r="913" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="913" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C913" s="4"/>
     </row>
-    <row r="914" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="914" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C914" s="4"/>
     </row>
-    <row r="915" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="915" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C915" s="4"/>
     </row>
-    <row r="916" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="916" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C916" s="4"/>
     </row>
-    <row r="917" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="917" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C917" s="4"/>
     </row>
-    <row r="918" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="918" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C918" s="4"/>
     </row>
-    <row r="919" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="919" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C919" s="4"/>
     </row>
-    <row r="920" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="920" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C920" s="4"/>
     </row>
-    <row r="921" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="921" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C921" s="4"/>
     </row>
-    <row r="922" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="922" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C922" s="4"/>
     </row>
-    <row r="923" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="923" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C923" s="4"/>
     </row>
-    <row r="924" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="924" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C924" s="4"/>
     </row>
-    <row r="925" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="925" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C925" s="4"/>
     </row>
-    <row r="926" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="926" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C926" s="4"/>
     </row>
-    <row r="927" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="927" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C927" s="4"/>
     </row>
-    <row r="928" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="928" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C928" s="4"/>
     </row>
-    <row r="929" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="929" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C929" s="4"/>
     </row>
-    <row r="930" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="930" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C930" s="4"/>
     </row>
-    <row r="931" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="931" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C931" s="4"/>
     </row>
-    <row r="932" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="932" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C932" s="4"/>
     </row>
-    <row r="933" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="933" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C933" s="4"/>
     </row>
-    <row r="934" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="934" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C934" s="4"/>
     </row>
-    <row r="935" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="935" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C935" s="4"/>
     </row>
-    <row r="936" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="936" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C936" s="4"/>
     </row>
-    <row r="937" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="937" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C937" s="4"/>
     </row>
-    <row r="938" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="938" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C938" s="4"/>
     </row>
-    <row r="939" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="939" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C939" s="4"/>
     </row>
-    <row r="940" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="940" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C940" s="4"/>
     </row>
-    <row r="941" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="941" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C941" s="4"/>
     </row>
-    <row r="942" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="942" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C942" s="4"/>
     </row>
-    <row r="943" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="943" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C943" s="4"/>
     </row>
-    <row r="944" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="944" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C944" s="4"/>
     </row>
-    <row r="945" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="945" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C945" s="4"/>
     </row>
-    <row r="946" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="946" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C946" s="4"/>
     </row>
-    <row r="947" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="947" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C947" s="4"/>
     </row>
-    <row r="948" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="948" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C948" s="4"/>
     </row>
-    <row r="949" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="949" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C949" s="4"/>
     </row>
-    <row r="950" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="950" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C950" s="4"/>
     </row>
-    <row r="951" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="951" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C951" s="4"/>
     </row>
-    <row r="952" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="952" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C952" s="4"/>
     </row>
-    <row r="953" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="953" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C953" s="4"/>
     </row>
-    <row r="954" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="954" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C954" s="4"/>
     </row>
-    <row r="955" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="955" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C955" s="4"/>
     </row>
-    <row r="956" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="956" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C956" s="4"/>
     </row>
-    <row r="957" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="957" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C957" s="4"/>
     </row>
-    <row r="958" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="958" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C958" s="4"/>
     </row>
-    <row r="959" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="959" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C959" s="4"/>
     </row>
-    <row r="960" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="960" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C960" s="4"/>
     </row>
-    <row r="961" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="961" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C961" s="4"/>
     </row>
-    <row r="962" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="962" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C962" s="4"/>
     </row>
-    <row r="963" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="963" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C963" s="4"/>
     </row>
-    <row r="964" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="964" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C964" s="4"/>
     </row>
-    <row r="965" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="965" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C965" s="4"/>
     </row>
-    <row r="966" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="966" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C966" s="4"/>
     </row>
-    <row r="967" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="967" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C967" s="4"/>
     </row>
-    <row r="968" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="968" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C968" s="4"/>
     </row>
-    <row r="969" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="969" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C969" s="4"/>
     </row>
-    <row r="970" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="970" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C970" s="4"/>
     </row>
-    <row r="971" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="971" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C971" s="4"/>
     </row>
-    <row r="972" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="972" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C972" s="4"/>
     </row>
-    <row r="973" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="973" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C973" s="4"/>
     </row>
-    <row r="974" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="974" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C974" s="4"/>
     </row>
-    <row r="975" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="975" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C975" s="4"/>
     </row>
-    <row r="976" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="976" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C976" s="4"/>
     </row>
-    <row r="977" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="977" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C977" s="4"/>
     </row>
-    <row r="978" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="978" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C978" s="4"/>
     </row>
-    <row r="979" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="979" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C979" s="4"/>
     </row>
-    <row r="980" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="980" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C980" s="4"/>
     </row>
-    <row r="981" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="981" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C981" s="4"/>
     </row>
-    <row r="982" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="982" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C982" s="4"/>
     </row>
-    <row r="983" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="983" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C983" s="4"/>
     </row>
-    <row r="984" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="984" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C984" s="4"/>
     </row>
-    <row r="985" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="985" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C985" s="4"/>
     </row>
-    <row r="986" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="986" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C986" s="4"/>
     </row>
-    <row r="987" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="987" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C987" s="4"/>
     </row>
-    <row r="988" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="988" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C988" s="4"/>
     </row>
-    <row r="989" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="989" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C989" s="4"/>
     </row>
-    <row r="990" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="990" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C990" s="4"/>
     </row>
-    <row r="991" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="991" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C991" s="4"/>
     </row>
-    <row r="992" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="992" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C992" s="4"/>
     </row>
-    <row r="993" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="993" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C993" s="4"/>
     </row>
-    <row r="994" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="994" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C994" s="4"/>
     </row>
-    <row r="995" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="995" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C995" s="4"/>
     </row>
-    <row r="996" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="996" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C996" s="4"/>
     </row>
-    <row r="997" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="997" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C997" s="4"/>
     </row>
-    <row r="998" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="998" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C998" s="4"/>
     </row>
-    <row r="999" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="999" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C999" s="4"/>
     </row>
-    <row r="1000" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1000" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C1000" s="4"/>
     </row>
-    <row r="1001" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1001" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C1001" s="4"/>
     </row>
-    <row r="1002" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1002" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C1002" s="4"/>
     </row>
-    <row r="1003" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1003" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C1003" s="4"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add data to db online
</commit_message>
<xml_diff>
--- a/PlanExcel/plan.xlsx
+++ b/PlanExcel/plan.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\~project\AndroidKotlin\MUSIC\PlanExcel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D678ADB-6811-4CFC-B416-05BB864914F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2B45912-B7AC-4314-8ECB-BF8C7156BA03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="15000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -562,25 +562,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Y1003"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.7109375" customWidth="1"/>
-    <col min="2" max="2" width="46.5703125" customWidth="1"/>
-    <col min="3" max="3" width="87.85546875" customWidth="1"/>
-    <col min="4" max="4" width="26.28515625" customWidth="1"/>
-    <col min="5" max="5" width="27.85546875" customWidth="1"/>
-    <col min="6" max="6" width="28.28515625" customWidth="1"/>
-    <col min="7" max="7" width="26.28515625" customWidth="1"/>
-    <col min="8" max="8" width="27.28515625" customWidth="1"/>
-    <col min="9" max="9" width="11.28515625" customWidth="1"/>
-    <col min="10" max="25" width="8.7109375" customWidth="1"/>
+    <col min="1" max="1" width="8.6640625" customWidth="1"/>
+    <col min="2" max="2" width="46.5546875" customWidth="1"/>
+    <col min="3" max="3" width="87.88671875" customWidth="1"/>
+    <col min="4" max="4" width="26.33203125" customWidth="1"/>
+    <col min="5" max="5" width="27.88671875" customWidth="1"/>
+    <col min="6" max="6" width="28.33203125" customWidth="1"/>
+    <col min="7" max="7" width="26.33203125" customWidth="1"/>
+    <col min="8" max="8" width="27.33203125" customWidth="1"/>
+    <col min="9" max="9" width="11.33203125" customWidth="1"/>
+    <col min="10" max="25" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" ht="33.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:25" ht="33.6" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
@@ -609,7 +609,7 @@
       <c r="X1" s="1"/>
       <c r="Y1" s="1"/>
     </row>
-    <row r="2" spans="1:25" ht="31.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:25" ht="31.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="16" t="s">
         <v>1</v>
       </c>
@@ -638,7 +638,7 @@
       <c r="X2" s="1"/>
       <c r="Y2" s="1"/>
     </row>
-    <row r="3" spans="1:25" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:25" ht="19.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="16" t="s">
         <v>2</v>
       </c>
@@ -667,7 +667,7 @@
       <c r="X3" s="1"/>
       <c r="Y3" s="1"/>
     </row>
-    <row r="4" spans="1:25" ht="154.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:25" ht="154.19999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2"/>
       <c r="B4" s="2" t="s">
         <v>3</v>
@@ -698,10 +698,10 @@
       <c r="X4" s="3"/>
       <c r="Y4" s="3"/>
     </row>
-    <row r="5" spans="1:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C5" s="4"/>
     </row>
-    <row r="6" spans="1:25" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:25" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="11" t="s">
         <v>4</v>
       </c>
@@ -746,7 +746,7 @@
       <c r="X6" s="5"/>
       <c r="Y6" s="5"/>
     </row>
-    <row r="7" spans="1:25" ht="45.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:25" ht="45.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="11">
         <v>1</v>
       </c>
@@ -789,7 +789,7 @@
       <c r="X7" s="5"/>
       <c r="Y7" s="5"/>
     </row>
-    <row r="8" spans="1:25" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:25" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="11">
         <v>2</v>
       </c>
@@ -832,7 +832,7 @@
       <c r="X8" s="5"/>
       <c r="Y8" s="5"/>
     </row>
-    <row r="9" spans="1:25" ht="20.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:25" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="11"/>
       <c r="B9" s="11"/>
       <c r="C9" s="12" t="s">
@@ -871,7 +871,7 @@
       <c r="X9" s="5"/>
       <c r="Y9" s="5"/>
     </row>
-    <row r="10" spans="1:25" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:25" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="11"/>
       <c r="B10" s="11"/>
       <c r="C10" s="12" t="s">
@@ -910,7 +910,7 @@
       <c r="X10" s="5"/>
       <c r="Y10" s="5"/>
     </row>
-    <row r="11" spans="1:25" ht="25.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:25" ht="25.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="11">
         <v>3</v>
       </c>
@@ -953,7 +953,7 @@
       <c r="X11" s="5"/>
       <c r="Y11" s="5"/>
     </row>
-    <row r="12" spans="1:25" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:25" ht="45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="11">
         <v>4</v>
       </c>
@@ -996,7 +996,7 @@
       <c r="X12" s="5"/>
       <c r="Y12" s="5"/>
     </row>
-    <row r="13" spans="1:25" ht="20.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:25" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="11">
         <v>5</v>
       </c>
@@ -1015,8 +1015,12 @@
       <c r="F13" s="14">
         <v>44838</v>
       </c>
-      <c r="G13" s="14"/>
-      <c r="H13" s="14"/>
+      <c r="G13" s="14">
+        <v>44836</v>
+      </c>
+      <c r="H13" s="14">
+        <v>44838</v>
+      </c>
       <c r="I13" s="11"/>
       <c r="J13" s="5"/>
       <c r="K13" s="5"/>
@@ -1035,7 +1039,7 @@
       <c r="X13" s="5"/>
       <c r="Y13" s="5"/>
     </row>
-    <row r="14" spans="1:25" ht="62.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:25" ht="62.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="11"/>
       <c r="B14" s="11"/>
       <c r="C14" s="13" t="s">
@@ -1070,7 +1074,7 @@
       <c r="X14" s="5"/>
       <c r="Y14" s="5"/>
     </row>
-    <row r="15" spans="1:25" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:25" ht="41.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="11">
         <v>6</v>
       </c>
@@ -1109,7 +1113,7 @@
       <c r="X15" s="5"/>
       <c r="Y15" s="5"/>
     </row>
-    <row r="16" spans="1:25" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:25" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="11"/>
       <c r="B16" s="11"/>
       <c r="C16" s="12" t="s">
@@ -1144,7 +1148,7 @@
       <c r="X16" s="5"/>
       <c r="Y16" s="5"/>
     </row>
-    <row r="17" spans="1:25" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:25" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="11"/>
       <c r="B17" s="11"/>
       <c r="C17" s="12" t="s">
@@ -1179,7 +1183,7 @@
       <c r="X17" s="5"/>
       <c r="Y17" s="5"/>
     </row>
-    <row r="18" spans="1:25" ht="23.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:25" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="11"/>
       <c r="B18" s="11"/>
       <c r="C18" s="12" t="s">
@@ -1214,7 +1218,7 @@
       <c r="X18" s="5"/>
       <c r="Y18" s="5"/>
     </row>
-    <row r="19" spans="1:25" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:25" ht="21.6" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A19" s="11"/>
       <c r="B19" s="11"/>
       <c r="C19" s="15" t="s">
@@ -1249,7 +1253,7 @@
       <c r="X19" s="5"/>
       <c r="Y19" s="5"/>
     </row>
-    <row r="20" spans="1:25" ht="22.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:25" ht="22.95" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A20" s="11"/>
       <c r="B20" s="11"/>
       <c r="C20" s="15" t="s">
@@ -1284,7 +1288,7 @@
       <c r="X20" s="5"/>
       <c r="Y20" s="5"/>
     </row>
-    <row r="21" spans="1:25" ht="22.15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:25" ht="22.2" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A21" s="11"/>
       <c r="B21" s="11"/>
       <c r="C21" s="15" t="s">
@@ -1319,7 +1323,7 @@
       <c r="X21" s="5"/>
       <c r="Y21" s="5"/>
     </row>
-    <row r="22" spans="1:25" ht="20.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:25" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A22" s="11"/>
       <c r="B22" s="11"/>
       <c r="C22" s="15" t="s">
@@ -1354,7 +1358,7 @@
       <c r="X22" s="5"/>
       <c r="Y22" s="5"/>
     </row>
-    <row r="23" spans="1:25" s="10" customFormat="1" ht="20.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:25" s="10" customFormat="1" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A23" s="11"/>
       <c r="B23" s="11"/>
       <c r="C23" s="15" t="s">
@@ -1389,7 +1393,7 @@
       <c r="X23" s="5"/>
       <c r="Y23" s="5"/>
     </row>
-    <row r="24" spans="1:25" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:25" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="11"/>
       <c r="B24" s="11"/>
       <c r="C24" s="12" t="s">
@@ -1424,7 +1428,7 @@
       <c r="X24" s="5"/>
       <c r="Y24" s="5"/>
     </row>
-    <row r="25" spans="1:25" ht="24.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:25" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="11"/>
       <c r="B25" s="11"/>
       <c r="C25" s="12" t="s">
@@ -1459,7 +1463,7 @@
       <c r="X25" s="5"/>
       <c r="Y25" s="5"/>
     </row>
-    <row r="26" spans="1:25" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:25" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="11">
         <v>7</v>
       </c>
@@ -1496,7 +1500,7 @@
       <c r="X26" s="5"/>
       <c r="Y26" s="5"/>
     </row>
-    <row r="27" spans="1:25" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:25" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="11">
         <v>8</v>
       </c>
@@ -1535,7 +1539,7 @@
       <c r="X27" s="5"/>
       <c r="Y27" s="5"/>
     </row>
-    <row r="28" spans="1:25" ht="26.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:25" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="11">
         <v>9</v>
       </c>
@@ -1572,7 +1576,7 @@
       <c r="X28" s="5"/>
       <c r="Y28" s="5"/>
     </row>
-    <row r="29" spans="1:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="6"/>
       <c r="B29" s="6"/>
       <c r="C29" s="7"/>
@@ -1599,7 +1603,7 @@
       <c r="X29" s="5"/>
       <c r="Y29" s="5"/>
     </row>
-    <row r="30" spans="1:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="6"/>
       <c r="B30" s="6"/>
       <c r="C30" s="7"/>
@@ -1626,7 +1630,7 @@
       <c r="X30" s="5"/>
       <c r="Y30" s="5"/>
     </row>
-    <row r="31" spans="1:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="6"/>
       <c r="B31" s="6"/>
       <c r="C31" s="7"/>
@@ -1653,7 +1657,7 @@
       <c r="X31" s="5"/>
       <c r="Y31" s="5"/>
     </row>
-    <row r="32" spans="1:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="6"/>
       <c r="B32" s="9"/>
       <c r="C32" s="7"/>
@@ -1680,7 +1684,7 @@
       <c r="X32" s="5"/>
       <c r="Y32" s="5"/>
     </row>
-    <row r="33" spans="1:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="6"/>
       <c r="B33" s="6"/>
       <c r="C33" s="7"/>
@@ -1707,7 +1711,7 @@
       <c r="X33" s="5"/>
       <c r="Y33" s="5"/>
     </row>
-    <row r="34" spans="1:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="6"/>
       <c r="B34" s="6"/>
       <c r="C34" s="7"/>
@@ -1734,2911 +1738,2911 @@
       <c r="X34" s="5"/>
       <c r="Y34" s="5"/>
     </row>
-    <row r="35" spans="1:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C35" s="4"/>
     </row>
-    <row r="36" spans="1:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C36" s="4"/>
     </row>
-    <row r="37" spans="1:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C37" s="4"/>
     </row>
-    <row r="38" spans="1:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C38" s="4"/>
     </row>
-    <row r="39" spans="1:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C39" s="4"/>
     </row>
-    <row r="40" spans="1:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C40" s="4"/>
     </row>
-    <row r="41" spans="1:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C41" s="4"/>
     </row>
-    <row r="42" spans="1:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C42" s="4"/>
     </row>
-    <row r="43" spans="1:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C43" s="4"/>
     </row>
-    <row r="44" spans="1:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C44" s="4"/>
     </row>
-    <row r="45" spans="1:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C45" s="4"/>
     </row>
-    <row r="46" spans="1:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C46" s="4"/>
     </row>
-    <row r="47" spans="1:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C47" s="4"/>
     </row>
-    <row r="48" spans="1:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C48" s="4"/>
     </row>
-    <row r="49" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C49" s="4"/>
     </row>
-    <row r="50" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C50" s="4"/>
     </row>
-    <row r="51" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C51" s="4"/>
     </row>
-    <row r="52" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C52" s="4"/>
     </row>
-    <row r="53" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C53" s="4"/>
     </row>
-    <row r="54" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C54" s="4"/>
     </row>
-    <row r="55" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C55" s="4"/>
     </row>
-    <row r="56" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C56" s="4"/>
     </row>
-    <row r="57" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C57" s="4"/>
     </row>
-    <row r="58" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C58" s="4"/>
     </row>
-    <row r="59" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C59" s="4"/>
     </row>
-    <row r="60" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C60" s="4"/>
     </row>
-    <row r="61" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C61" s="4"/>
     </row>
-    <row r="62" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C62" s="4"/>
     </row>
-    <row r="63" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C63" s="4"/>
     </row>
-    <row r="64" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C64" s="4"/>
     </row>
-    <row r="65" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C65" s="4"/>
     </row>
-    <row r="66" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C66" s="4"/>
     </row>
-    <row r="67" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C67" s="4"/>
     </row>
-    <row r="68" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C68" s="4"/>
     </row>
-    <row r="69" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C69" s="4"/>
     </row>
-    <row r="70" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C70" s="4"/>
     </row>
-    <row r="71" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C71" s="4"/>
     </row>
-    <row r="72" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C72" s="4"/>
     </row>
-    <row r="73" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C73" s="4"/>
     </row>
-    <row r="74" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C74" s="4"/>
     </row>
-    <row r="75" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C75" s="4"/>
     </row>
-    <row r="76" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C76" s="4"/>
     </row>
-    <row r="77" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C77" s="4"/>
     </row>
-    <row r="78" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C78" s="4"/>
     </row>
-    <row r="79" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C79" s="4"/>
     </row>
-    <row r="80" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C80" s="4"/>
     </row>
-    <row r="81" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C81" s="4"/>
     </row>
-    <row r="82" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C82" s="4"/>
     </row>
-    <row r="83" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C83" s="4"/>
     </row>
-    <row r="84" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C84" s="4"/>
     </row>
-    <row r="85" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C85" s="4"/>
     </row>
-    <row r="86" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C86" s="4"/>
     </row>
-    <row r="87" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C87" s="4"/>
     </row>
-    <row r="88" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C88" s="4"/>
     </row>
-    <row r="89" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C89" s="4"/>
     </row>
-    <row r="90" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C90" s="4"/>
     </row>
-    <row r="91" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C91" s="4"/>
     </row>
-    <row r="92" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C92" s="4"/>
     </row>
-    <row r="93" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C93" s="4"/>
     </row>
-    <row r="94" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C94" s="4"/>
     </row>
-    <row r="95" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C95" s="4"/>
     </row>
-    <row r="96" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C96" s="4"/>
     </row>
-    <row r="97" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C97" s="4"/>
     </row>
-    <row r="98" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C98" s="4"/>
     </row>
-    <row r="99" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C99" s="4"/>
     </row>
-    <row r="100" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C100" s="4"/>
     </row>
-    <row r="101" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C101" s="4"/>
     </row>
-    <row r="102" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C102" s="4"/>
     </row>
-    <row r="103" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C103" s="4"/>
     </row>
-    <row r="104" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C104" s="4"/>
     </row>
-    <row r="105" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C105" s="4"/>
     </row>
-    <row r="106" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C106" s="4"/>
     </row>
-    <row r="107" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C107" s="4"/>
     </row>
-    <row r="108" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C108" s="4"/>
     </row>
-    <row r="109" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C109" s="4"/>
     </row>
-    <row r="110" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C110" s="4"/>
     </row>
-    <row r="111" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C111" s="4"/>
     </row>
-    <row r="112" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C112" s="4"/>
     </row>
-    <row r="113" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C113" s="4"/>
     </row>
-    <row r="114" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C114" s="4"/>
     </row>
-    <row r="115" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C115" s="4"/>
     </row>
-    <row r="116" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C116" s="4"/>
     </row>
-    <row r="117" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C117" s="4"/>
     </row>
-    <row r="118" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C118" s="4"/>
     </row>
-    <row r="119" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C119" s="4"/>
     </row>
-    <row r="120" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="120" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C120" s="4"/>
     </row>
-    <row r="121" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="121" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C121" s="4"/>
     </row>
-    <row r="122" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="122" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C122" s="4"/>
     </row>
-    <row r="123" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="123" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C123" s="4"/>
     </row>
-    <row r="124" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="124" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C124" s="4"/>
     </row>
-    <row r="125" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="125" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C125" s="4"/>
     </row>
-    <row r="126" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="126" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C126" s="4"/>
     </row>
-    <row r="127" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="127" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C127" s="4"/>
     </row>
-    <row r="128" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="128" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C128" s="4"/>
     </row>
-    <row r="129" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="129" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C129" s="4"/>
     </row>
-    <row r="130" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="130" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C130" s="4"/>
     </row>
-    <row r="131" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="131" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C131" s="4"/>
     </row>
-    <row r="132" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="132" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C132" s="4"/>
     </row>
-    <row r="133" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="133" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C133" s="4"/>
     </row>
-    <row r="134" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="134" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C134" s="4"/>
     </row>
-    <row r="135" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="135" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C135" s="4"/>
     </row>
-    <row r="136" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="136" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C136" s="4"/>
     </row>
-    <row r="137" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="137" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C137" s="4"/>
     </row>
-    <row r="138" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="138" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C138" s="4"/>
     </row>
-    <row r="139" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="139" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C139" s="4"/>
     </row>
-    <row r="140" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="140" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C140" s="4"/>
     </row>
-    <row r="141" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="141" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C141" s="4"/>
     </row>
-    <row r="142" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="142" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C142" s="4"/>
     </row>
-    <row r="143" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="143" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C143" s="4"/>
     </row>
-    <row r="144" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="144" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C144" s="4"/>
     </row>
-    <row r="145" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="145" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C145" s="4"/>
     </row>
-    <row r="146" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="146" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C146" s="4"/>
     </row>
-    <row r="147" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="147" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C147" s="4"/>
     </row>
-    <row r="148" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="148" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C148" s="4"/>
     </row>
-    <row r="149" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="149" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C149" s="4"/>
     </row>
-    <row r="150" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="150" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C150" s="4"/>
     </row>
-    <row r="151" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="151" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C151" s="4"/>
     </row>
-    <row r="152" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="152" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C152" s="4"/>
     </row>
-    <row r="153" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="153" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C153" s="4"/>
     </row>
-    <row r="154" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="154" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C154" s="4"/>
     </row>
-    <row r="155" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="155" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C155" s="4"/>
     </row>
-    <row r="156" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="156" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C156" s="4"/>
     </row>
-    <row r="157" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="157" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C157" s="4"/>
     </row>
-    <row r="158" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="158" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C158" s="4"/>
     </row>
-    <row r="159" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="159" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C159" s="4"/>
     </row>
-    <row r="160" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="160" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C160" s="4"/>
     </row>
-    <row r="161" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="161" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C161" s="4"/>
     </row>
-    <row r="162" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="162" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C162" s="4"/>
     </row>
-    <row r="163" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="163" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C163" s="4"/>
     </row>
-    <row r="164" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="164" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C164" s="4"/>
     </row>
-    <row r="165" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="165" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C165" s="4"/>
     </row>
-    <row r="166" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="166" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C166" s="4"/>
     </row>
-    <row r="167" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="167" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C167" s="4"/>
     </row>
-    <row r="168" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="168" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C168" s="4"/>
     </row>
-    <row r="169" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="169" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C169" s="4"/>
     </row>
-    <row r="170" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="170" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C170" s="4"/>
     </row>
-    <row r="171" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="171" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C171" s="4"/>
     </row>
-    <row r="172" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="172" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C172" s="4"/>
     </row>
-    <row r="173" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="173" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C173" s="4"/>
     </row>
-    <row r="174" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="174" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C174" s="4"/>
     </row>
-    <row r="175" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="175" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C175" s="4"/>
     </row>
-    <row r="176" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="176" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C176" s="4"/>
     </row>
-    <row r="177" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="177" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C177" s="4"/>
     </row>
-    <row r="178" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="178" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C178" s="4"/>
     </row>
-    <row r="179" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="179" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C179" s="4"/>
     </row>
-    <row r="180" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="180" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C180" s="4"/>
     </row>
-    <row r="181" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="181" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C181" s="4"/>
     </row>
-    <row r="182" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="182" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C182" s="4"/>
     </row>
-    <row r="183" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="183" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C183" s="4"/>
     </row>
-    <row r="184" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="184" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C184" s="4"/>
     </row>
-    <row r="185" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="185" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C185" s="4"/>
     </row>
-    <row r="186" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="186" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C186" s="4"/>
     </row>
-    <row r="187" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="187" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C187" s="4"/>
     </row>
-    <row r="188" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="188" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C188" s="4"/>
     </row>
-    <row r="189" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="189" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C189" s="4"/>
     </row>
-    <row r="190" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="190" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C190" s="4"/>
     </row>
-    <row r="191" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="191" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C191" s="4"/>
     </row>
-    <row r="192" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="192" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C192" s="4"/>
     </row>
-    <row r="193" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="193" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C193" s="4"/>
     </row>
-    <row r="194" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="194" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C194" s="4"/>
     </row>
-    <row r="195" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="195" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C195" s="4"/>
     </row>
-    <row r="196" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="196" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C196" s="4"/>
     </row>
-    <row r="197" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="197" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C197" s="4"/>
     </row>
-    <row r="198" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="198" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C198" s="4"/>
     </row>
-    <row r="199" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="199" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C199" s="4"/>
     </row>
-    <row r="200" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="200" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C200" s="4"/>
     </row>
-    <row r="201" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="201" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C201" s="4"/>
     </row>
-    <row r="202" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="202" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C202" s="4"/>
     </row>
-    <row r="203" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="203" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C203" s="4"/>
     </row>
-    <row r="204" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="204" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C204" s="4"/>
     </row>
-    <row r="205" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="205" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C205" s="4"/>
     </row>
-    <row r="206" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="206" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C206" s="4"/>
     </row>
-    <row r="207" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="207" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C207" s="4"/>
     </row>
-    <row r="208" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="208" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C208" s="4"/>
     </row>
-    <row r="209" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="209" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C209" s="4"/>
     </row>
-    <row r="210" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="210" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C210" s="4"/>
     </row>
-    <row r="211" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="211" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C211" s="4"/>
     </row>
-    <row r="212" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="212" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C212" s="4"/>
     </row>
-    <row r="213" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="213" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C213" s="4"/>
     </row>
-    <row r="214" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="214" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C214" s="4"/>
     </row>
-    <row r="215" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="215" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C215" s="4"/>
     </row>
-    <row r="216" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="216" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C216" s="4"/>
     </row>
-    <row r="217" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="217" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C217" s="4"/>
     </row>
-    <row r="218" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="218" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C218" s="4"/>
     </row>
-    <row r="219" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="219" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C219" s="4"/>
     </row>
-    <row r="220" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="220" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C220" s="4"/>
     </row>
-    <row r="221" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="221" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C221" s="4"/>
     </row>
-    <row r="222" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="222" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C222" s="4"/>
     </row>
-    <row r="223" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="223" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C223" s="4"/>
     </row>
-    <row r="224" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="224" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C224" s="4"/>
     </row>
-    <row r="225" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="225" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C225" s="4"/>
     </row>
-    <row r="226" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="226" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C226" s="4"/>
     </row>
-    <row r="227" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="227" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C227" s="4"/>
     </row>
-    <row r="228" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="228" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C228" s="4"/>
     </row>
-    <row r="229" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="229" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C229" s="4"/>
     </row>
-    <row r="230" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="230" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C230" s="4"/>
     </row>
-    <row r="231" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="231" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C231" s="4"/>
     </row>
-    <row r="232" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="232" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C232" s="4"/>
     </row>
-    <row r="233" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="233" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C233" s="4"/>
     </row>
-    <row r="234" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="234" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C234" s="4"/>
     </row>
-    <row r="235" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="235" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C235" s="4"/>
     </row>
-    <row r="236" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="236" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C236" s="4"/>
     </row>
-    <row r="237" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="237" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C237" s="4"/>
     </row>
-    <row r="238" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="238" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C238" s="4"/>
     </row>
-    <row r="239" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="239" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C239" s="4"/>
     </row>
-    <row r="240" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="240" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C240" s="4"/>
     </row>
-    <row r="241" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="241" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C241" s="4"/>
     </row>
-    <row r="242" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="242" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C242" s="4"/>
     </row>
-    <row r="243" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="243" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C243" s="4"/>
     </row>
-    <row r="244" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="244" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C244" s="4"/>
     </row>
-    <row r="245" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="245" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C245" s="4"/>
     </row>
-    <row r="246" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="246" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C246" s="4"/>
     </row>
-    <row r="247" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="247" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C247" s="4"/>
     </row>
-    <row r="248" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="248" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C248" s="4"/>
     </row>
-    <row r="249" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="249" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C249" s="4"/>
     </row>
-    <row r="250" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="250" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C250" s="4"/>
     </row>
-    <row r="251" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="251" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C251" s="4"/>
     </row>
-    <row r="252" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="252" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C252" s="4"/>
     </row>
-    <row r="253" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="253" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C253" s="4"/>
     </row>
-    <row r="254" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="254" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C254" s="4"/>
     </row>
-    <row r="255" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="255" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C255" s="4"/>
     </row>
-    <row r="256" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="256" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C256" s="4"/>
     </row>
-    <row r="257" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="257" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C257" s="4"/>
     </row>
-    <row r="258" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="258" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C258" s="4"/>
     </row>
-    <row r="259" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="259" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C259" s="4"/>
     </row>
-    <row r="260" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="260" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C260" s="4"/>
     </row>
-    <row r="261" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="261" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C261" s="4"/>
     </row>
-    <row r="262" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="262" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C262" s="4"/>
     </row>
-    <row r="263" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="263" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C263" s="4"/>
     </row>
-    <row r="264" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="264" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C264" s="4"/>
     </row>
-    <row r="265" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="265" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C265" s="4"/>
     </row>
-    <row r="266" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="266" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C266" s="4"/>
     </row>
-    <row r="267" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="267" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C267" s="4"/>
     </row>
-    <row r="268" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="268" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C268" s="4"/>
     </row>
-    <row r="269" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="269" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C269" s="4"/>
     </row>
-    <row r="270" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="270" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C270" s="4"/>
     </row>
-    <row r="271" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="271" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C271" s="4"/>
     </row>
-    <row r="272" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="272" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C272" s="4"/>
     </row>
-    <row r="273" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="273" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C273" s="4"/>
     </row>
-    <row r="274" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="274" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C274" s="4"/>
     </row>
-    <row r="275" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="275" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C275" s="4"/>
     </row>
-    <row r="276" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="276" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C276" s="4"/>
     </row>
-    <row r="277" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="277" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C277" s="4"/>
     </row>
-    <row r="278" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="278" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C278" s="4"/>
     </row>
-    <row r="279" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="279" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C279" s="4"/>
     </row>
-    <row r="280" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="280" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C280" s="4"/>
     </row>
-    <row r="281" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="281" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C281" s="4"/>
     </row>
-    <row r="282" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="282" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C282" s="4"/>
     </row>
-    <row r="283" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="283" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C283" s="4"/>
     </row>
-    <row r="284" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="284" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C284" s="4"/>
     </row>
-    <row r="285" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="285" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C285" s="4"/>
     </row>
-    <row r="286" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="286" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C286" s="4"/>
     </row>
-    <row r="287" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="287" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C287" s="4"/>
     </row>
-    <row r="288" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="288" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C288" s="4"/>
     </row>
-    <row r="289" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="289" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C289" s="4"/>
     </row>
-    <row r="290" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="290" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C290" s="4"/>
     </row>
-    <row r="291" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="291" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C291" s="4"/>
     </row>
-    <row r="292" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="292" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C292" s="4"/>
     </row>
-    <row r="293" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="293" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C293" s="4"/>
     </row>
-    <row r="294" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="294" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C294" s="4"/>
     </row>
-    <row r="295" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="295" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C295" s="4"/>
     </row>
-    <row r="296" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="296" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C296" s="4"/>
     </row>
-    <row r="297" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="297" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C297" s="4"/>
     </row>
-    <row r="298" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="298" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C298" s="4"/>
     </row>
-    <row r="299" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="299" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C299" s="4"/>
     </row>
-    <row r="300" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="300" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C300" s="4"/>
     </row>
-    <row r="301" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="301" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C301" s="4"/>
     </row>
-    <row r="302" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="302" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C302" s="4"/>
     </row>
-    <row r="303" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="303" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C303" s="4"/>
     </row>
-    <row r="304" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="304" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C304" s="4"/>
     </row>
-    <row r="305" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="305" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C305" s="4"/>
     </row>
-    <row r="306" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="306" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C306" s="4"/>
     </row>
-    <row r="307" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="307" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C307" s="4"/>
     </row>
-    <row r="308" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="308" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C308" s="4"/>
     </row>
-    <row r="309" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="309" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C309" s="4"/>
     </row>
-    <row r="310" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="310" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C310" s="4"/>
     </row>
-    <row r="311" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="311" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C311" s="4"/>
     </row>
-    <row r="312" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="312" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C312" s="4"/>
     </row>
-    <row r="313" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="313" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C313" s="4"/>
     </row>
-    <row r="314" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="314" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C314" s="4"/>
     </row>
-    <row r="315" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="315" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C315" s="4"/>
     </row>
-    <row r="316" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="316" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C316" s="4"/>
     </row>
-    <row r="317" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="317" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C317" s="4"/>
     </row>
-    <row r="318" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="318" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C318" s="4"/>
     </row>
-    <row r="319" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="319" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C319" s="4"/>
     </row>
-    <row r="320" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="320" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C320" s="4"/>
     </row>
-    <row r="321" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="321" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C321" s="4"/>
     </row>
-    <row r="322" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="322" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C322" s="4"/>
     </row>
-    <row r="323" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="323" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C323" s="4"/>
     </row>
-    <row r="324" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="324" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C324" s="4"/>
     </row>
-    <row r="325" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="325" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C325" s="4"/>
     </row>
-    <row r="326" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="326" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C326" s="4"/>
     </row>
-    <row r="327" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="327" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C327" s="4"/>
     </row>
-    <row r="328" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="328" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C328" s="4"/>
     </row>
-    <row r="329" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="329" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C329" s="4"/>
     </row>
-    <row r="330" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="330" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C330" s="4"/>
     </row>
-    <row r="331" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="331" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C331" s="4"/>
     </row>
-    <row r="332" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="332" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C332" s="4"/>
     </row>
-    <row r="333" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="333" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C333" s="4"/>
     </row>
-    <row r="334" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="334" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C334" s="4"/>
     </row>
-    <row r="335" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="335" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C335" s="4"/>
     </row>
-    <row r="336" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="336" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C336" s="4"/>
     </row>
-    <row r="337" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="337" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C337" s="4"/>
     </row>
-    <row r="338" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="338" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C338" s="4"/>
     </row>
-    <row r="339" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="339" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C339" s="4"/>
     </row>
-    <row r="340" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="340" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C340" s="4"/>
     </row>
-    <row r="341" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="341" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C341" s="4"/>
     </row>
-    <row r="342" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="342" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C342" s="4"/>
     </row>
-    <row r="343" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="343" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C343" s="4"/>
     </row>
-    <row r="344" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="344" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C344" s="4"/>
     </row>
-    <row r="345" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="345" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C345" s="4"/>
     </row>
-    <row r="346" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="346" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C346" s="4"/>
     </row>
-    <row r="347" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="347" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C347" s="4"/>
     </row>
-    <row r="348" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="348" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C348" s="4"/>
     </row>
-    <row r="349" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="349" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C349" s="4"/>
     </row>
-    <row r="350" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="350" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C350" s="4"/>
     </row>
-    <row r="351" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="351" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C351" s="4"/>
     </row>
-    <row r="352" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="352" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C352" s="4"/>
     </row>
-    <row r="353" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="353" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C353" s="4"/>
     </row>
-    <row r="354" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="354" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C354" s="4"/>
     </row>
-    <row r="355" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="355" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C355" s="4"/>
     </row>
-    <row r="356" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="356" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C356" s="4"/>
     </row>
-    <row r="357" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="357" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C357" s="4"/>
     </row>
-    <row r="358" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="358" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C358" s="4"/>
     </row>
-    <row r="359" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="359" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C359" s="4"/>
     </row>
-    <row r="360" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="360" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C360" s="4"/>
     </row>
-    <row r="361" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="361" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C361" s="4"/>
     </row>
-    <row r="362" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="362" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C362" s="4"/>
     </row>
-    <row r="363" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="363" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C363" s="4"/>
     </row>
-    <row r="364" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="364" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C364" s="4"/>
     </row>
-    <row r="365" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="365" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C365" s="4"/>
     </row>
-    <row r="366" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="366" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C366" s="4"/>
     </row>
-    <row r="367" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="367" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C367" s="4"/>
     </row>
-    <row r="368" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="368" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C368" s="4"/>
     </row>
-    <row r="369" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="369" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C369" s="4"/>
     </row>
-    <row r="370" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="370" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C370" s="4"/>
     </row>
-    <row r="371" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="371" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C371" s="4"/>
     </row>
-    <row r="372" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="372" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C372" s="4"/>
     </row>
-    <row r="373" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="373" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C373" s="4"/>
     </row>
-    <row r="374" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="374" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C374" s="4"/>
     </row>
-    <row r="375" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="375" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C375" s="4"/>
     </row>
-    <row r="376" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="376" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C376" s="4"/>
     </row>
-    <row r="377" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="377" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C377" s="4"/>
     </row>
-    <row r="378" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="378" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C378" s="4"/>
     </row>
-    <row r="379" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="379" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C379" s="4"/>
     </row>
-    <row r="380" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="380" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C380" s="4"/>
     </row>
-    <row r="381" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="381" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C381" s="4"/>
     </row>
-    <row r="382" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="382" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C382" s="4"/>
     </row>
-    <row r="383" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="383" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C383" s="4"/>
     </row>
-    <row r="384" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="384" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C384" s="4"/>
     </row>
-    <row r="385" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="385" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C385" s="4"/>
     </row>
-    <row r="386" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="386" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C386" s="4"/>
     </row>
-    <row r="387" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="387" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C387" s="4"/>
     </row>
-    <row r="388" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="388" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C388" s="4"/>
     </row>
-    <row r="389" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="389" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C389" s="4"/>
     </row>
-    <row r="390" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="390" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C390" s="4"/>
     </row>
-    <row r="391" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="391" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C391" s="4"/>
     </row>
-    <row r="392" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="392" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C392" s="4"/>
     </row>
-    <row r="393" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="393" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C393" s="4"/>
     </row>
-    <row r="394" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="394" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C394" s="4"/>
     </row>
-    <row r="395" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="395" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C395" s="4"/>
     </row>
-    <row r="396" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="396" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C396" s="4"/>
     </row>
-    <row r="397" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="397" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C397" s="4"/>
     </row>
-    <row r="398" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="398" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C398" s="4"/>
     </row>
-    <row r="399" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="399" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C399" s="4"/>
     </row>
-    <row r="400" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="400" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C400" s="4"/>
     </row>
-    <row r="401" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="401" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C401" s="4"/>
     </row>
-    <row r="402" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="402" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C402" s="4"/>
     </row>
-    <row r="403" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="403" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C403" s="4"/>
     </row>
-    <row r="404" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="404" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C404" s="4"/>
     </row>
-    <row r="405" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="405" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C405" s="4"/>
     </row>
-    <row r="406" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="406" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C406" s="4"/>
     </row>
-    <row r="407" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="407" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C407" s="4"/>
     </row>
-    <row r="408" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="408" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C408" s="4"/>
     </row>
-    <row r="409" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="409" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C409" s="4"/>
     </row>
-    <row r="410" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="410" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C410" s="4"/>
     </row>
-    <row r="411" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="411" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C411" s="4"/>
     </row>
-    <row r="412" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="412" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C412" s="4"/>
     </row>
-    <row r="413" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="413" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C413" s="4"/>
     </row>
-    <row r="414" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="414" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C414" s="4"/>
     </row>
-    <row r="415" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="415" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C415" s="4"/>
     </row>
-    <row r="416" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="416" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C416" s="4"/>
     </row>
-    <row r="417" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="417" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C417" s="4"/>
     </row>
-    <row r="418" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="418" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C418" s="4"/>
     </row>
-    <row r="419" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="419" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C419" s="4"/>
     </row>
-    <row r="420" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="420" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C420" s="4"/>
     </row>
-    <row r="421" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="421" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C421" s="4"/>
     </row>
-    <row r="422" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="422" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C422" s="4"/>
     </row>
-    <row r="423" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="423" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C423" s="4"/>
     </row>
-    <row r="424" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="424" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C424" s="4"/>
     </row>
-    <row r="425" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="425" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C425" s="4"/>
     </row>
-    <row r="426" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="426" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C426" s="4"/>
     </row>
-    <row r="427" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="427" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C427" s="4"/>
     </row>
-    <row r="428" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="428" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C428" s="4"/>
     </row>
-    <row r="429" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="429" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C429" s="4"/>
     </row>
-    <row r="430" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="430" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C430" s="4"/>
     </row>
-    <row r="431" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="431" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C431" s="4"/>
     </row>
-    <row r="432" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="432" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C432" s="4"/>
     </row>
-    <row r="433" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="433" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C433" s="4"/>
     </row>
-    <row r="434" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="434" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C434" s="4"/>
     </row>
-    <row r="435" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="435" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C435" s="4"/>
     </row>
-    <row r="436" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="436" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C436" s="4"/>
     </row>
-    <row r="437" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="437" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C437" s="4"/>
     </row>
-    <row r="438" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="438" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C438" s="4"/>
     </row>
-    <row r="439" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="439" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C439" s="4"/>
     </row>
-    <row r="440" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="440" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C440" s="4"/>
     </row>
-    <row r="441" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="441" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C441" s="4"/>
     </row>
-    <row r="442" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="442" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C442" s="4"/>
     </row>
-    <row r="443" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="443" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C443" s="4"/>
     </row>
-    <row r="444" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="444" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C444" s="4"/>
     </row>
-    <row r="445" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="445" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C445" s="4"/>
     </row>
-    <row r="446" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="446" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C446" s="4"/>
     </row>
-    <row r="447" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="447" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C447" s="4"/>
     </row>
-    <row r="448" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="448" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C448" s="4"/>
     </row>
-    <row r="449" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="449" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C449" s="4"/>
     </row>
-    <row r="450" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="450" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C450" s="4"/>
     </row>
-    <row r="451" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="451" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C451" s="4"/>
     </row>
-    <row r="452" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="452" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C452" s="4"/>
     </row>
-    <row r="453" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="453" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C453" s="4"/>
     </row>
-    <row r="454" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="454" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C454" s="4"/>
     </row>
-    <row r="455" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="455" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C455" s="4"/>
     </row>
-    <row r="456" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="456" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C456" s="4"/>
     </row>
-    <row r="457" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="457" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C457" s="4"/>
     </row>
-    <row r="458" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="458" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C458" s="4"/>
     </row>
-    <row r="459" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="459" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C459" s="4"/>
     </row>
-    <row r="460" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="460" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C460" s="4"/>
     </row>
-    <row r="461" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="461" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C461" s="4"/>
     </row>
-    <row r="462" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="462" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C462" s="4"/>
     </row>
-    <row r="463" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="463" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C463" s="4"/>
     </row>
-    <row r="464" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="464" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C464" s="4"/>
     </row>
-    <row r="465" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="465" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C465" s="4"/>
     </row>
-    <row r="466" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="466" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C466" s="4"/>
     </row>
-    <row r="467" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="467" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C467" s="4"/>
     </row>
-    <row r="468" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="468" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C468" s="4"/>
     </row>
-    <row r="469" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="469" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C469" s="4"/>
     </row>
-    <row r="470" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="470" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C470" s="4"/>
     </row>
-    <row r="471" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="471" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C471" s="4"/>
     </row>
-    <row r="472" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="472" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C472" s="4"/>
     </row>
-    <row r="473" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="473" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C473" s="4"/>
     </row>
-    <row r="474" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="474" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C474" s="4"/>
     </row>
-    <row r="475" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="475" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C475" s="4"/>
     </row>
-    <row r="476" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="476" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C476" s="4"/>
     </row>
-    <row r="477" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="477" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C477" s="4"/>
     </row>
-    <row r="478" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="478" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C478" s="4"/>
     </row>
-    <row r="479" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="479" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C479" s="4"/>
     </row>
-    <row r="480" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="480" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C480" s="4"/>
     </row>
-    <row r="481" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="481" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C481" s="4"/>
     </row>
-    <row r="482" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="482" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C482" s="4"/>
     </row>
-    <row r="483" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="483" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C483" s="4"/>
     </row>
-    <row r="484" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="484" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C484" s="4"/>
     </row>
-    <row r="485" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="485" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C485" s="4"/>
     </row>
-    <row r="486" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="486" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C486" s="4"/>
     </row>
-    <row r="487" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="487" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C487" s="4"/>
     </row>
-    <row r="488" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="488" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C488" s="4"/>
     </row>
-    <row r="489" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="489" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C489" s="4"/>
     </row>
-    <row r="490" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="490" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C490" s="4"/>
     </row>
-    <row r="491" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="491" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C491" s="4"/>
     </row>
-    <row r="492" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="492" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C492" s="4"/>
     </row>
-    <row r="493" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="493" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C493" s="4"/>
     </row>
-    <row r="494" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="494" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C494" s="4"/>
     </row>
-    <row r="495" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="495" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C495" s="4"/>
     </row>
-    <row r="496" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="496" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C496" s="4"/>
     </row>
-    <row r="497" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="497" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C497" s="4"/>
     </row>
-    <row r="498" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="498" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C498" s="4"/>
     </row>
-    <row r="499" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="499" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C499" s="4"/>
     </row>
-    <row r="500" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="500" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C500" s="4"/>
     </row>
-    <row r="501" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="501" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C501" s="4"/>
     </row>
-    <row r="502" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="502" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C502" s="4"/>
     </row>
-    <row r="503" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="503" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C503" s="4"/>
     </row>
-    <row r="504" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="504" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C504" s="4"/>
     </row>
-    <row r="505" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="505" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C505" s="4"/>
     </row>
-    <row r="506" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="506" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C506" s="4"/>
     </row>
-    <row r="507" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="507" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C507" s="4"/>
     </row>
-    <row r="508" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="508" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C508" s="4"/>
     </row>
-    <row r="509" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="509" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C509" s="4"/>
     </row>
-    <row r="510" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="510" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C510" s="4"/>
     </row>
-    <row r="511" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="511" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C511" s="4"/>
     </row>
-    <row r="512" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="512" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C512" s="4"/>
     </row>
-    <row r="513" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="513" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C513" s="4"/>
     </row>
-    <row r="514" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="514" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C514" s="4"/>
     </row>
-    <row r="515" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="515" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C515" s="4"/>
     </row>
-    <row r="516" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="516" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C516" s="4"/>
     </row>
-    <row r="517" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="517" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C517" s="4"/>
     </row>
-    <row r="518" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="518" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C518" s="4"/>
     </row>
-    <row r="519" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="519" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C519" s="4"/>
     </row>
-    <row r="520" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="520" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C520" s="4"/>
     </row>
-    <row r="521" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="521" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C521" s="4"/>
     </row>
-    <row r="522" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="522" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C522" s="4"/>
     </row>
-    <row r="523" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="523" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C523" s="4"/>
     </row>
-    <row r="524" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="524" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C524" s="4"/>
     </row>
-    <row r="525" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="525" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C525" s="4"/>
     </row>
-    <row r="526" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="526" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C526" s="4"/>
     </row>
-    <row r="527" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="527" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C527" s="4"/>
     </row>
-    <row r="528" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="528" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C528" s="4"/>
     </row>
-    <row r="529" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="529" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C529" s="4"/>
     </row>
-    <row r="530" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="530" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C530" s="4"/>
     </row>
-    <row r="531" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="531" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C531" s="4"/>
     </row>
-    <row r="532" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="532" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C532" s="4"/>
     </row>
-    <row r="533" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="533" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C533" s="4"/>
     </row>
-    <row r="534" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="534" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C534" s="4"/>
     </row>
-    <row r="535" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="535" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C535" s="4"/>
     </row>
-    <row r="536" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="536" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C536" s="4"/>
     </row>
-    <row r="537" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="537" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C537" s="4"/>
     </row>
-    <row r="538" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="538" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C538" s="4"/>
     </row>
-    <row r="539" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="539" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C539" s="4"/>
     </row>
-    <row r="540" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="540" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C540" s="4"/>
     </row>
-    <row r="541" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="541" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C541" s="4"/>
     </row>
-    <row r="542" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="542" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C542" s="4"/>
     </row>
-    <row r="543" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="543" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C543" s="4"/>
     </row>
-    <row r="544" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="544" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C544" s="4"/>
     </row>
-    <row r="545" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="545" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C545" s="4"/>
     </row>
-    <row r="546" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="546" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C546" s="4"/>
     </row>
-    <row r="547" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="547" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C547" s="4"/>
     </row>
-    <row r="548" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="548" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C548" s="4"/>
     </row>
-    <row r="549" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="549" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C549" s="4"/>
     </row>
-    <row r="550" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="550" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C550" s="4"/>
     </row>
-    <row r="551" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="551" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C551" s="4"/>
     </row>
-    <row r="552" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="552" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C552" s="4"/>
     </row>
-    <row r="553" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="553" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C553" s="4"/>
     </row>
-    <row r="554" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="554" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C554" s="4"/>
     </row>
-    <row r="555" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="555" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C555" s="4"/>
     </row>
-    <row r="556" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="556" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C556" s="4"/>
     </row>
-    <row r="557" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="557" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C557" s="4"/>
     </row>
-    <row r="558" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="558" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C558" s="4"/>
     </row>
-    <row r="559" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="559" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C559" s="4"/>
     </row>
-    <row r="560" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="560" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C560" s="4"/>
     </row>
-    <row r="561" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="561" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C561" s="4"/>
     </row>
-    <row r="562" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="562" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C562" s="4"/>
     </row>
-    <row r="563" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="563" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C563" s="4"/>
     </row>
-    <row r="564" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="564" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C564" s="4"/>
     </row>
-    <row r="565" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="565" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C565" s="4"/>
     </row>
-    <row r="566" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="566" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C566" s="4"/>
     </row>
-    <row r="567" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="567" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C567" s="4"/>
     </row>
-    <row r="568" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="568" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C568" s="4"/>
     </row>
-    <row r="569" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="569" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C569" s="4"/>
     </row>
-    <row r="570" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="570" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C570" s="4"/>
     </row>
-    <row r="571" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="571" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C571" s="4"/>
     </row>
-    <row r="572" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="572" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C572" s="4"/>
     </row>
-    <row r="573" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="573" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C573" s="4"/>
     </row>
-    <row r="574" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="574" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C574" s="4"/>
     </row>
-    <row r="575" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="575" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C575" s="4"/>
     </row>
-    <row r="576" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="576" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C576" s="4"/>
     </row>
-    <row r="577" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="577" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C577" s="4"/>
     </row>
-    <row r="578" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="578" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C578" s="4"/>
     </row>
-    <row r="579" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="579" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C579" s="4"/>
     </row>
-    <row r="580" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="580" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C580" s="4"/>
     </row>
-    <row r="581" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="581" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C581" s="4"/>
     </row>
-    <row r="582" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="582" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C582" s="4"/>
     </row>
-    <row r="583" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="583" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C583" s="4"/>
     </row>
-    <row r="584" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="584" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C584" s="4"/>
     </row>
-    <row r="585" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="585" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C585" s="4"/>
     </row>
-    <row r="586" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="586" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C586" s="4"/>
     </row>
-    <row r="587" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="587" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C587" s="4"/>
     </row>
-    <row r="588" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="588" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C588" s="4"/>
     </row>
-    <row r="589" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="589" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C589" s="4"/>
     </row>
-    <row r="590" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="590" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C590" s="4"/>
     </row>
-    <row r="591" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="591" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C591" s="4"/>
     </row>
-    <row r="592" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="592" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C592" s="4"/>
     </row>
-    <row r="593" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="593" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C593" s="4"/>
     </row>
-    <row r="594" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="594" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C594" s="4"/>
     </row>
-    <row r="595" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="595" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C595" s="4"/>
     </row>
-    <row r="596" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="596" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C596" s="4"/>
     </row>
-    <row r="597" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="597" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C597" s="4"/>
     </row>
-    <row r="598" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="598" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C598" s="4"/>
     </row>
-    <row r="599" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="599" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C599" s="4"/>
     </row>
-    <row r="600" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="600" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C600" s="4"/>
     </row>
-    <row r="601" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="601" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C601" s="4"/>
     </row>
-    <row r="602" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="602" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C602" s="4"/>
     </row>
-    <row r="603" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="603" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C603" s="4"/>
     </row>
-    <row r="604" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="604" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C604" s="4"/>
     </row>
-    <row r="605" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="605" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C605" s="4"/>
     </row>
-    <row r="606" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="606" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C606" s="4"/>
     </row>
-    <row r="607" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="607" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C607" s="4"/>
     </row>
-    <row r="608" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="608" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C608" s="4"/>
     </row>
-    <row r="609" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="609" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C609" s="4"/>
     </row>
-    <row r="610" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="610" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C610" s="4"/>
     </row>
-    <row r="611" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="611" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C611" s="4"/>
     </row>
-    <row r="612" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="612" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C612" s="4"/>
     </row>
-    <row r="613" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="613" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C613" s="4"/>
     </row>
-    <row r="614" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="614" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C614" s="4"/>
     </row>
-    <row r="615" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="615" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C615" s="4"/>
     </row>
-    <row r="616" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="616" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C616" s="4"/>
     </row>
-    <row r="617" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="617" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C617" s="4"/>
     </row>
-    <row r="618" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="618" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C618" s="4"/>
     </row>
-    <row r="619" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="619" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C619" s="4"/>
     </row>
-    <row r="620" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="620" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C620" s="4"/>
     </row>
-    <row r="621" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="621" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C621" s="4"/>
     </row>
-    <row r="622" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="622" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C622" s="4"/>
     </row>
-    <row r="623" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="623" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C623" s="4"/>
     </row>
-    <row r="624" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="624" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C624" s="4"/>
     </row>
-    <row r="625" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="625" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C625" s="4"/>
     </row>
-    <row r="626" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="626" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C626" s="4"/>
     </row>
-    <row r="627" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="627" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C627" s="4"/>
     </row>
-    <row r="628" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="628" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C628" s="4"/>
     </row>
-    <row r="629" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="629" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C629" s="4"/>
     </row>
-    <row r="630" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="630" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C630" s="4"/>
     </row>
-    <row r="631" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="631" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C631" s="4"/>
     </row>
-    <row r="632" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="632" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C632" s="4"/>
     </row>
-    <row r="633" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="633" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C633" s="4"/>
     </row>
-    <row r="634" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="634" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C634" s="4"/>
     </row>
-    <row r="635" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="635" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C635" s="4"/>
     </row>
-    <row r="636" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="636" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C636" s="4"/>
     </row>
-    <row r="637" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="637" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C637" s="4"/>
     </row>
-    <row r="638" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="638" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C638" s="4"/>
     </row>
-    <row r="639" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="639" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C639" s="4"/>
     </row>
-    <row r="640" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="640" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C640" s="4"/>
     </row>
-    <row r="641" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="641" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C641" s="4"/>
     </row>
-    <row r="642" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="642" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C642" s="4"/>
     </row>
-    <row r="643" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="643" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C643" s="4"/>
     </row>
-    <row r="644" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="644" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C644" s="4"/>
     </row>
-    <row r="645" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="645" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C645" s="4"/>
     </row>
-    <row r="646" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="646" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C646" s="4"/>
     </row>
-    <row r="647" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="647" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C647" s="4"/>
     </row>
-    <row r="648" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="648" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C648" s="4"/>
     </row>
-    <row r="649" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="649" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C649" s="4"/>
     </row>
-    <row r="650" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="650" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C650" s="4"/>
     </row>
-    <row r="651" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="651" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C651" s="4"/>
     </row>
-    <row r="652" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="652" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C652" s="4"/>
     </row>
-    <row r="653" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="653" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C653" s="4"/>
     </row>
-    <row r="654" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="654" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C654" s="4"/>
     </row>
-    <row r="655" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="655" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C655" s="4"/>
     </row>
-    <row r="656" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="656" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C656" s="4"/>
     </row>
-    <row r="657" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="657" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C657" s="4"/>
     </row>
-    <row r="658" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="658" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C658" s="4"/>
     </row>
-    <row r="659" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="659" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C659" s="4"/>
     </row>
-    <row r="660" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="660" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C660" s="4"/>
     </row>
-    <row r="661" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="661" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C661" s="4"/>
     </row>
-    <row r="662" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="662" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C662" s="4"/>
     </row>
-    <row r="663" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="663" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C663" s="4"/>
     </row>
-    <row r="664" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="664" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C664" s="4"/>
     </row>
-    <row r="665" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="665" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C665" s="4"/>
     </row>
-    <row r="666" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="666" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C666" s="4"/>
     </row>
-    <row r="667" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="667" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C667" s="4"/>
     </row>
-    <row r="668" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="668" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C668" s="4"/>
     </row>
-    <row r="669" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="669" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C669" s="4"/>
     </row>
-    <row r="670" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="670" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C670" s="4"/>
     </row>
-    <row r="671" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="671" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C671" s="4"/>
     </row>
-    <row r="672" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="672" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C672" s="4"/>
     </row>
-    <row r="673" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="673" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C673" s="4"/>
     </row>
-    <row r="674" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="674" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C674" s="4"/>
     </row>
-    <row r="675" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="675" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C675" s="4"/>
     </row>
-    <row r="676" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="676" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C676" s="4"/>
     </row>
-    <row r="677" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="677" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C677" s="4"/>
     </row>
-    <row r="678" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="678" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C678" s="4"/>
     </row>
-    <row r="679" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="679" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C679" s="4"/>
     </row>
-    <row r="680" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="680" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C680" s="4"/>
     </row>
-    <row r="681" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="681" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C681" s="4"/>
     </row>
-    <row r="682" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="682" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C682" s="4"/>
     </row>
-    <row r="683" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="683" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C683" s="4"/>
     </row>
-    <row r="684" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="684" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C684" s="4"/>
     </row>
-    <row r="685" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="685" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C685" s="4"/>
     </row>
-    <row r="686" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="686" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C686" s="4"/>
     </row>
-    <row r="687" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="687" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C687" s="4"/>
     </row>
-    <row r="688" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="688" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C688" s="4"/>
     </row>
-    <row r="689" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="689" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C689" s="4"/>
     </row>
-    <row r="690" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="690" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C690" s="4"/>
     </row>
-    <row r="691" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="691" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C691" s="4"/>
     </row>
-    <row r="692" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="692" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C692" s="4"/>
     </row>
-    <row r="693" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="693" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C693" s="4"/>
     </row>
-    <row r="694" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="694" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C694" s="4"/>
     </row>
-    <row r="695" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="695" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C695" s="4"/>
     </row>
-    <row r="696" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="696" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C696" s="4"/>
     </row>
-    <row r="697" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="697" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C697" s="4"/>
     </row>
-    <row r="698" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="698" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C698" s="4"/>
     </row>
-    <row r="699" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="699" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C699" s="4"/>
     </row>
-    <row r="700" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="700" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C700" s="4"/>
     </row>
-    <row r="701" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="701" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C701" s="4"/>
     </row>
-    <row r="702" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="702" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C702" s="4"/>
     </row>
-    <row r="703" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="703" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C703" s="4"/>
     </row>
-    <row r="704" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="704" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C704" s="4"/>
     </row>
-    <row r="705" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="705" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C705" s="4"/>
     </row>
-    <row r="706" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="706" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C706" s="4"/>
     </row>
-    <row r="707" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="707" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C707" s="4"/>
     </row>
-    <row r="708" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="708" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C708" s="4"/>
     </row>
-    <row r="709" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="709" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C709" s="4"/>
     </row>
-    <row r="710" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="710" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C710" s="4"/>
     </row>
-    <row r="711" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="711" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C711" s="4"/>
     </row>
-    <row r="712" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="712" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C712" s="4"/>
     </row>
-    <row r="713" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="713" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C713" s="4"/>
     </row>
-    <row r="714" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="714" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C714" s="4"/>
     </row>
-    <row r="715" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="715" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C715" s="4"/>
     </row>
-    <row r="716" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="716" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C716" s="4"/>
     </row>
-    <row r="717" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="717" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C717" s="4"/>
     </row>
-    <row r="718" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="718" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C718" s="4"/>
     </row>
-    <row r="719" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="719" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C719" s="4"/>
     </row>
-    <row r="720" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="720" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C720" s="4"/>
     </row>
-    <row r="721" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="721" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C721" s="4"/>
     </row>
-    <row r="722" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="722" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C722" s="4"/>
     </row>
-    <row r="723" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="723" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C723" s="4"/>
     </row>
-    <row r="724" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="724" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C724" s="4"/>
     </row>
-    <row r="725" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="725" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C725" s="4"/>
     </row>
-    <row r="726" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="726" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C726" s="4"/>
     </row>
-    <row r="727" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="727" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C727" s="4"/>
     </row>
-    <row r="728" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="728" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C728" s="4"/>
     </row>
-    <row r="729" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="729" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C729" s="4"/>
     </row>
-    <row r="730" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="730" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C730" s="4"/>
     </row>
-    <row r="731" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="731" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C731" s="4"/>
     </row>
-    <row r="732" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="732" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C732" s="4"/>
     </row>
-    <row r="733" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="733" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C733" s="4"/>
     </row>
-    <row r="734" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="734" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C734" s="4"/>
     </row>
-    <row r="735" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="735" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C735" s="4"/>
     </row>
-    <row r="736" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="736" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C736" s="4"/>
     </row>
-    <row r="737" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="737" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C737" s="4"/>
     </row>
-    <row r="738" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="738" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C738" s="4"/>
     </row>
-    <row r="739" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="739" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C739" s="4"/>
     </row>
-    <row r="740" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="740" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C740" s="4"/>
     </row>
-    <row r="741" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="741" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C741" s="4"/>
     </row>
-    <row r="742" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="742" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C742" s="4"/>
     </row>
-    <row r="743" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="743" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C743" s="4"/>
     </row>
-    <row r="744" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="744" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C744" s="4"/>
     </row>
-    <row r="745" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="745" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C745" s="4"/>
     </row>
-    <row r="746" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="746" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C746" s="4"/>
     </row>
-    <row r="747" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="747" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C747" s="4"/>
     </row>
-    <row r="748" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="748" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C748" s="4"/>
     </row>
-    <row r="749" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="749" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C749" s="4"/>
     </row>
-    <row r="750" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="750" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C750" s="4"/>
     </row>
-    <row r="751" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="751" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C751" s="4"/>
     </row>
-    <row r="752" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="752" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C752" s="4"/>
     </row>
-    <row r="753" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="753" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C753" s="4"/>
     </row>
-    <row r="754" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="754" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C754" s="4"/>
     </row>
-    <row r="755" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="755" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C755" s="4"/>
     </row>
-    <row r="756" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="756" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C756" s="4"/>
     </row>
-    <row r="757" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="757" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C757" s="4"/>
     </row>
-    <row r="758" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="758" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C758" s="4"/>
     </row>
-    <row r="759" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="759" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C759" s="4"/>
     </row>
-    <row r="760" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="760" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C760" s="4"/>
     </row>
-    <row r="761" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="761" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C761" s="4"/>
     </row>
-    <row r="762" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="762" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C762" s="4"/>
     </row>
-    <row r="763" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="763" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C763" s="4"/>
     </row>
-    <row r="764" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="764" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C764" s="4"/>
     </row>
-    <row r="765" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="765" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C765" s="4"/>
     </row>
-    <row r="766" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="766" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C766" s="4"/>
     </row>
-    <row r="767" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="767" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C767" s="4"/>
     </row>
-    <row r="768" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="768" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C768" s="4"/>
     </row>
-    <row r="769" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="769" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C769" s="4"/>
     </row>
-    <row r="770" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="770" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C770" s="4"/>
     </row>
-    <row r="771" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="771" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C771" s="4"/>
     </row>
-    <row r="772" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="772" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C772" s="4"/>
     </row>
-    <row r="773" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="773" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C773" s="4"/>
     </row>
-    <row r="774" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="774" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C774" s="4"/>
     </row>
-    <row r="775" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="775" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C775" s="4"/>
     </row>
-    <row r="776" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="776" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C776" s="4"/>
     </row>
-    <row r="777" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="777" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C777" s="4"/>
     </row>
-    <row r="778" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="778" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C778" s="4"/>
     </row>
-    <row r="779" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="779" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C779" s="4"/>
     </row>
-    <row r="780" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="780" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C780" s="4"/>
     </row>
-    <row r="781" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="781" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C781" s="4"/>
     </row>
-    <row r="782" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="782" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C782" s="4"/>
     </row>
-    <row r="783" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="783" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C783" s="4"/>
     </row>
-    <row r="784" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="784" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C784" s="4"/>
     </row>
-    <row r="785" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="785" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C785" s="4"/>
     </row>
-    <row r="786" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="786" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C786" s="4"/>
     </row>
-    <row r="787" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="787" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C787" s="4"/>
     </row>
-    <row r="788" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="788" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C788" s="4"/>
     </row>
-    <row r="789" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="789" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C789" s="4"/>
     </row>
-    <row r="790" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="790" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C790" s="4"/>
     </row>
-    <row r="791" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="791" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C791" s="4"/>
     </row>
-    <row r="792" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="792" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C792" s="4"/>
     </row>
-    <row r="793" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="793" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C793" s="4"/>
     </row>
-    <row r="794" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="794" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C794" s="4"/>
     </row>
-    <row r="795" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="795" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C795" s="4"/>
     </row>
-    <row r="796" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="796" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C796" s="4"/>
     </row>
-    <row r="797" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="797" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C797" s="4"/>
     </row>
-    <row r="798" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="798" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C798" s="4"/>
     </row>
-    <row r="799" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="799" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C799" s="4"/>
     </row>
-    <row r="800" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="800" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C800" s="4"/>
     </row>
-    <row r="801" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="801" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C801" s="4"/>
     </row>
-    <row r="802" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="802" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C802" s="4"/>
     </row>
-    <row r="803" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="803" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C803" s="4"/>
     </row>
-    <row r="804" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="804" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C804" s="4"/>
     </row>
-    <row r="805" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="805" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C805" s="4"/>
     </row>
-    <row r="806" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="806" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C806" s="4"/>
     </row>
-    <row r="807" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="807" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C807" s="4"/>
     </row>
-    <row r="808" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="808" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C808" s="4"/>
     </row>
-    <row r="809" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="809" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C809" s="4"/>
     </row>
-    <row r="810" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="810" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C810" s="4"/>
     </row>
-    <row r="811" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="811" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C811" s="4"/>
     </row>
-    <row r="812" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="812" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C812" s="4"/>
     </row>
-    <row r="813" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="813" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C813" s="4"/>
     </row>
-    <row r="814" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="814" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C814" s="4"/>
     </row>
-    <row r="815" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="815" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C815" s="4"/>
     </row>
-    <row r="816" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="816" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C816" s="4"/>
     </row>
-    <row r="817" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="817" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C817" s="4"/>
     </row>
-    <row r="818" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="818" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C818" s="4"/>
     </row>
-    <row r="819" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="819" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C819" s="4"/>
     </row>
-    <row r="820" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="820" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C820" s="4"/>
     </row>
-    <row r="821" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="821" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C821" s="4"/>
     </row>
-    <row r="822" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="822" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C822" s="4"/>
     </row>
-    <row r="823" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="823" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C823" s="4"/>
     </row>
-    <row r="824" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="824" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C824" s="4"/>
     </row>
-    <row r="825" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="825" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C825" s="4"/>
     </row>
-    <row r="826" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="826" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C826" s="4"/>
     </row>
-    <row r="827" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="827" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C827" s="4"/>
     </row>
-    <row r="828" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="828" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C828" s="4"/>
     </row>
-    <row r="829" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="829" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C829" s="4"/>
     </row>
-    <row r="830" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="830" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C830" s="4"/>
     </row>
-    <row r="831" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="831" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C831" s="4"/>
     </row>
-    <row r="832" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="832" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C832" s="4"/>
     </row>
-    <row r="833" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="833" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C833" s="4"/>
     </row>
-    <row r="834" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="834" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C834" s="4"/>
     </row>
-    <row r="835" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="835" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C835" s="4"/>
     </row>
-    <row r="836" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="836" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C836" s="4"/>
     </row>
-    <row r="837" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="837" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C837" s="4"/>
     </row>
-    <row r="838" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="838" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C838" s="4"/>
     </row>
-    <row r="839" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="839" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C839" s="4"/>
     </row>
-    <row r="840" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="840" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C840" s="4"/>
     </row>
-    <row r="841" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="841" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C841" s="4"/>
     </row>
-    <row r="842" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="842" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C842" s="4"/>
     </row>
-    <row r="843" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="843" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C843" s="4"/>
     </row>
-    <row r="844" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="844" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C844" s="4"/>
     </row>
-    <row r="845" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="845" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C845" s="4"/>
     </row>
-    <row r="846" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="846" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C846" s="4"/>
     </row>
-    <row r="847" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="847" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C847" s="4"/>
     </row>
-    <row r="848" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="848" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C848" s="4"/>
     </row>
-    <row r="849" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="849" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C849" s="4"/>
     </row>
-    <row r="850" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="850" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C850" s="4"/>
     </row>
-    <row r="851" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="851" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C851" s="4"/>
     </row>
-    <row r="852" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="852" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C852" s="4"/>
     </row>
-    <row r="853" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="853" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C853" s="4"/>
     </row>
-    <row r="854" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="854" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C854" s="4"/>
     </row>
-    <row r="855" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="855" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C855" s="4"/>
     </row>
-    <row r="856" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="856" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C856" s="4"/>
     </row>
-    <row r="857" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="857" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C857" s="4"/>
     </row>
-    <row r="858" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="858" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C858" s="4"/>
     </row>
-    <row r="859" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="859" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C859" s="4"/>
     </row>
-    <row r="860" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="860" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C860" s="4"/>
     </row>
-    <row r="861" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="861" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C861" s="4"/>
     </row>
-    <row r="862" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="862" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C862" s="4"/>
     </row>
-    <row r="863" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="863" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C863" s="4"/>
     </row>
-    <row r="864" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="864" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C864" s="4"/>
     </row>
-    <row r="865" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="865" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C865" s="4"/>
     </row>
-    <row r="866" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="866" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C866" s="4"/>
     </row>
-    <row r="867" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="867" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C867" s="4"/>
     </row>
-    <row r="868" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="868" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C868" s="4"/>
     </row>
-    <row r="869" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="869" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C869" s="4"/>
     </row>
-    <row r="870" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="870" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C870" s="4"/>
     </row>
-    <row r="871" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="871" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C871" s="4"/>
     </row>
-    <row r="872" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="872" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C872" s="4"/>
     </row>
-    <row r="873" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="873" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C873" s="4"/>
     </row>
-    <row r="874" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="874" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C874" s="4"/>
     </row>
-    <row r="875" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="875" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C875" s="4"/>
     </row>
-    <row r="876" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="876" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C876" s="4"/>
     </row>
-    <row r="877" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="877" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C877" s="4"/>
     </row>
-    <row r="878" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="878" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C878" s="4"/>
     </row>
-    <row r="879" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="879" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C879" s="4"/>
     </row>
-    <row r="880" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="880" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C880" s="4"/>
     </row>
-    <row r="881" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="881" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C881" s="4"/>
     </row>
-    <row r="882" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="882" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C882" s="4"/>
     </row>
-    <row r="883" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="883" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C883" s="4"/>
     </row>
-    <row r="884" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="884" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C884" s="4"/>
     </row>
-    <row r="885" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="885" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C885" s="4"/>
     </row>
-    <row r="886" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="886" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C886" s="4"/>
     </row>
-    <row r="887" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="887" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C887" s="4"/>
     </row>
-    <row r="888" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="888" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C888" s="4"/>
     </row>
-    <row r="889" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="889" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C889" s="4"/>
     </row>
-    <row r="890" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="890" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C890" s="4"/>
     </row>
-    <row r="891" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="891" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C891" s="4"/>
     </row>
-    <row r="892" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="892" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C892" s="4"/>
     </row>
-    <row r="893" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="893" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C893" s="4"/>
     </row>
-    <row r="894" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="894" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C894" s="4"/>
     </row>
-    <row r="895" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="895" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C895" s="4"/>
     </row>
-    <row r="896" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="896" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C896" s="4"/>
     </row>
-    <row r="897" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="897" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C897" s="4"/>
     </row>
-    <row r="898" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="898" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C898" s="4"/>
     </row>
-    <row r="899" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="899" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C899" s="4"/>
     </row>
-    <row r="900" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="900" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C900" s="4"/>
     </row>
-    <row r="901" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="901" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C901" s="4"/>
     </row>
-    <row r="902" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="902" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C902" s="4"/>
     </row>
-    <row r="903" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="903" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C903" s="4"/>
     </row>
-    <row r="904" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="904" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C904" s="4"/>
     </row>
-    <row r="905" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="905" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C905" s="4"/>
     </row>
-    <row r="906" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="906" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C906" s="4"/>
     </row>
-    <row r="907" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="907" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C907" s="4"/>
     </row>
-    <row r="908" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="908" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C908" s="4"/>
     </row>
-    <row r="909" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="909" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C909" s="4"/>
     </row>
-    <row r="910" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="910" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C910" s="4"/>
     </row>
-    <row r="911" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="911" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C911" s="4"/>
     </row>
-    <row r="912" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="912" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C912" s="4"/>
     </row>
-    <row r="913" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="913" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C913" s="4"/>
     </row>
-    <row r="914" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="914" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C914" s="4"/>
     </row>
-    <row r="915" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="915" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C915" s="4"/>
     </row>
-    <row r="916" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="916" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C916" s="4"/>
     </row>
-    <row r="917" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="917" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C917" s="4"/>
     </row>
-    <row r="918" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="918" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C918" s="4"/>
     </row>
-    <row r="919" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="919" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C919" s="4"/>
     </row>
-    <row r="920" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="920" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C920" s="4"/>
     </row>
-    <row r="921" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="921" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C921" s="4"/>
     </row>
-    <row r="922" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="922" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C922" s="4"/>
     </row>
-    <row r="923" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="923" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C923" s="4"/>
     </row>
-    <row r="924" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="924" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C924" s="4"/>
     </row>
-    <row r="925" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="925" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C925" s="4"/>
     </row>
-    <row r="926" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="926" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C926" s="4"/>
     </row>
-    <row r="927" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="927" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C927" s="4"/>
     </row>
-    <row r="928" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="928" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C928" s="4"/>
     </row>
-    <row r="929" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="929" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C929" s="4"/>
     </row>
-    <row r="930" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="930" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C930" s="4"/>
     </row>
-    <row r="931" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="931" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C931" s="4"/>
     </row>
-    <row r="932" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="932" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C932" s="4"/>
     </row>
-    <row r="933" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="933" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C933" s="4"/>
     </row>
-    <row r="934" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="934" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C934" s="4"/>
     </row>
-    <row r="935" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="935" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C935" s="4"/>
     </row>
-    <row r="936" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="936" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C936" s="4"/>
     </row>
-    <row r="937" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="937" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C937" s="4"/>
     </row>
-    <row r="938" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="938" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C938" s="4"/>
     </row>
-    <row r="939" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="939" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C939" s="4"/>
     </row>
-    <row r="940" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="940" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C940" s="4"/>
     </row>
-    <row r="941" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="941" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C941" s="4"/>
     </row>
-    <row r="942" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="942" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C942" s="4"/>
     </row>
-    <row r="943" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="943" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C943" s="4"/>
     </row>
-    <row r="944" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="944" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C944" s="4"/>
     </row>
-    <row r="945" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="945" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C945" s="4"/>
     </row>
-    <row r="946" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="946" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C946" s="4"/>
     </row>
-    <row r="947" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="947" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C947" s="4"/>
     </row>
-    <row r="948" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="948" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C948" s="4"/>
     </row>
-    <row r="949" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="949" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C949" s="4"/>
     </row>
-    <row r="950" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="950" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C950" s="4"/>
     </row>
-    <row r="951" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="951" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C951" s="4"/>
     </row>
-    <row r="952" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="952" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C952" s="4"/>
     </row>
-    <row r="953" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="953" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C953" s="4"/>
     </row>
-    <row r="954" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="954" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C954" s="4"/>
     </row>
-    <row r="955" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="955" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C955" s="4"/>
     </row>
-    <row r="956" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="956" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C956" s="4"/>
     </row>
-    <row r="957" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="957" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C957" s="4"/>
     </row>
-    <row r="958" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="958" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C958" s="4"/>
     </row>
-    <row r="959" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="959" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C959" s="4"/>
     </row>
-    <row r="960" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="960" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C960" s="4"/>
     </row>
-    <row r="961" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="961" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C961" s="4"/>
     </row>
-    <row r="962" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="962" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C962" s="4"/>
     </row>
-    <row r="963" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="963" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C963" s="4"/>
     </row>
-    <row r="964" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="964" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C964" s="4"/>
     </row>
-    <row r="965" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="965" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C965" s="4"/>
     </row>
-    <row r="966" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="966" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C966" s="4"/>
     </row>
-    <row r="967" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="967" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C967" s="4"/>
     </row>
-    <row r="968" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="968" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C968" s="4"/>
     </row>
-    <row r="969" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="969" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C969" s="4"/>
     </row>
-    <row r="970" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="970" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C970" s="4"/>
     </row>
-    <row r="971" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="971" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C971" s="4"/>
     </row>
-    <row r="972" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="972" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C972" s="4"/>
     </row>
-    <row r="973" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="973" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C973" s="4"/>
     </row>
-    <row r="974" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="974" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C974" s="4"/>
     </row>
-    <row r="975" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="975" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C975" s="4"/>
     </row>
-    <row r="976" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="976" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C976" s="4"/>
     </row>
-    <row r="977" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="977" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C977" s="4"/>
     </row>
-    <row r="978" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="978" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C978" s="4"/>
     </row>
-    <row r="979" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="979" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C979" s="4"/>
     </row>
-    <row r="980" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="980" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C980" s="4"/>
     </row>
-    <row r="981" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="981" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C981" s="4"/>
     </row>
-    <row r="982" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="982" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C982" s="4"/>
     </row>
-    <row r="983" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="983" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C983" s="4"/>
     </row>
-    <row r="984" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="984" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C984" s="4"/>
     </row>
-    <row r="985" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="985" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C985" s="4"/>
     </row>
-    <row r="986" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="986" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C986" s="4"/>
     </row>
-    <row r="987" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="987" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C987" s="4"/>
     </row>
-    <row r="988" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="988" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C988" s="4"/>
     </row>
-    <row r="989" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="989" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C989" s="4"/>
     </row>
-    <row r="990" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="990" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C990" s="4"/>
     </row>
-    <row r="991" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="991" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C991" s="4"/>
     </row>
-    <row r="992" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="992" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C992" s="4"/>
     </row>
-    <row r="993" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="993" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C993" s="4"/>
     </row>
-    <row r="994" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="994" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C994" s="4"/>
     </row>
-    <row r="995" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="995" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C995" s="4"/>
     </row>
-    <row r="996" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="996" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C996" s="4"/>
     </row>
-    <row r="997" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="997" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C997" s="4"/>
     </row>
-    <row r="998" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="998" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C998" s="4"/>
     </row>
-    <row r="999" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="999" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C999" s="4"/>
     </row>
-    <row r="1000" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1000" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C1000" s="4"/>
     </row>
-    <row r="1001" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1001" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C1001" s="4"/>
     </row>
-    <row r="1002" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1002" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C1002" s="4"/>
     </row>
-    <row r="1003" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1003" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C1003" s="4"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
comment added, load song's image
</commit_message>
<xml_diff>
--- a/PlanExcel/plan.xlsx
+++ b/PlanExcel/plan.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\~project\AndroidKotlin\MUSIC\PlanExcel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2B45912-B7AC-4314-8ECB-BF8C7156BA03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3B836C0-2826-44F0-9BD0-8AB2ED40AB2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -562,8 +562,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Y1003"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1054,7 +1054,9 @@
       <c r="F14" s="14">
         <v>44842</v>
       </c>
-      <c r="G14" s="14"/>
+      <c r="G14" s="14">
+        <v>44838</v>
+      </c>
       <c r="H14" s="14"/>
       <c r="I14" s="11"/>
       <c r="J14" s="5"/>

</xml_diff>

<commit_message>
welcome text based on time in home fragment
</commit_message>
<xml_diff>
--- a/PlanExcel/plan.xlsx
+++ b/PlanExcel/plan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\~project\AndroidKotlin\MUSIC\PlanExcel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3B836C0-2826-44F0-9BD0-8AB2ED40AB2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A783072-4299-4FD0-8FE1-BEFE54456107}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -563,7 +563,7 @@
   <dimension ref="A1:Y1003"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1057,7 +1057,9 @@
       <c r="G14" s="14">
         <v>44838</v>
       </c>
-      <c r="H14" s="14"/>
+      <c r="H14" s="14">
+        <v>44842</v>
+      </c>
       <c r="I14" s="11"/>
       <c r="J14" s="5"/>
       <c r="K14" s="5"/>
@@ -1095,7 +1097,9 @@
       <c r="F15" s="14">
         <v>44846</v>
       </c>
-      <c r="G15" s="14"/>
+      <c r="G15" s="14">
+        <v>44843</v>
+      </c>
       <c r="H15" s="14"/>
       <c r="I15" s="11"/>
       <c r="J15" s="5"/>

</xml_diff>

<commit_message>
improve search in crud fragments
</commit_message>
<xml_diff>
--- a/PlanExcel/plan.xlsx
+++ b/PlanExcel/plan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\~project\AndroidKotlin\MUSIC\PlanExcel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A783072-4299-4FD0-8FE1-BEFE54456107}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F87A713-8BD7-40CD-BC85-497CBF76EAA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -563,7 +563,7 @@
   <dimension ref="A1:Y1003"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1100,7 +1100,9 @@
       <c r="G15" s="14">
         <v>44843</v>
       </c>
-      <c r="H15" s="14"/>
+      <c r="H15" s="14">
+        <v>44846</v>
+      </c>
       <c r="I15" s="11"/>
       <c r="J15" s="5"/>
       <c r="K15" s="5"/>
@@ -1134,7 +1136,9 @@
       <c r="F16" s="14">
         <v>44849</v>
       </c>
-      <c r="G16" s="14"/>
+      <c r="G16" s="14">
+        <v>44847</v>
+      </c>
       <c r="H16" s="14"/>
       <c r="I16" s="11"/>
       <c r="J16" s="5"/>

</xml_diff>

<commit_message>
upgrade download song, improve ui
</commit_message>
<xml_diff>
--- a/PlanExcel/plan.xlsx
+++ b/PlanExcel/plan.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\~project\AndroidKotlin\MUSIC\PlanExcel\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D5FC623-90D0-4C47-8BC0-4D8F3C9A7B0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -171,7 +172,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd/mm"/>
   </numFmts>
@@ -238,8 +239,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+  <cellXfs count="18">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -262,10 +263,6 @@
     <xf numFmtId="164" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -284,13 +281,13 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -322,7 +319,7 @@
     </dxf>
   </dxfs>
   <tableStyles count="1">
-    <tableStyle name="Sheet1-style" pivot="0" count="3">
+    <tableStyle name="Sheet1-style" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
       <tableStyleElement type="headerRow" dxfId="2"/>
       <tableStyleElement type="firstRowStripe" dxfId="1"/>
       <tableStyleElement type="secondRowStripe" dxfId="0"/>
@@ -340,17 +337,17 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table_1" displayName="Table_1" ref="A6:I34" headerRowCount="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table_1" displayName="Table_1" ref="A6:I34" headerRowCount="0">
   <tableColumns count="9">
-    <tableColumn id="1" name="Column1"/>
-    <tableColumn id="2" name="Column2"/>
-    <tableColumn id="3" name="Column3"/>
-    <tableColumn id="4" name="Column4"/>
-    <tableColumn id="6" name="Column6"/>
-    <tableColumn id="7" name="Column7"/>
-    <tableColumn id="8" name="Column8"/>
-    <tableColumn id="9" name="Column9"/>
-    <tableColumn id="10" name="Column10"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Column1"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Column2"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Column3"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Column4"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Column6"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Column7"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Column8"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Column9"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Column10"/>
   </tableColumns>
   <tableStyleInfo name="Sheet1-style" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="0"/>
   <extLst>
@@ -558,11 +555,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Y1003"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -580,17 +577,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:25" ht="33.6" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
-      <c r="E1" s="17"/>
-      <c r="F1" s="17"/>
-      <c r="G1" s="17"/>
-      <c r="H1" s="17"/>
-      <c r="I1" s="17"/>
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
+      <c r="H1" s="15"/>
+      <c r="I1" s="15"/>
       <c r="J1" s="1"/>
       <c r="K1" s="1"/>
       <c r="L1" s="1"/>
@@ -609,17 +606,17 @@
       <c r="Y1" s="1"/>
     </row>
     <row r="2" spans="1:25" ht="31.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="16" t="s">
+      <c r="A2" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="17"/>
-      <c r="C2" s="17"/>
-      <c r="D2" s="17"/>
-      <c r="E2" s="17"/>
-      <c r="F2" s="17"/>
-      <c r="G2" s="17"/>
-      <c r="H2" s="17"/>
-      <c r="I2" s="17"/>
+      <c r="B2" s="15"/>
+      <c r="C2" s="15"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="15"/>
+      <c r="F2" s="15"/>
+      <c r="G2" s="15"/>
+      <c r="H2" s="15"/>
+      <c r="I2" s="15"/>
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
       <c r="L2" s="1"/>
@@ -638,17 +635,17 @@
       <c r="Y2" s="1"/>
     </row>
     <row r="3" spans="1:25" ht="19.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="16" t="s">
+      <c r="A3" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="17"/>
-      <c r="C3" s="17"/>
-      <c r="D3" s="17"/>
-      <c r="E3" s="17"/>
-      <c r="F3" s="17"/>
-      <c r="G3" s="17"/>
-      <c r="H3" s="17"/>
-      <c r="I3" s="17"/>
+      <c r="B3" s="15"/>
+      <c r="C3" s="15"/>
+      <c r="D3" s="15"/>
+      <c r="E3" s="15"/>
+      <c r="F3" s="15"/>
+      <c r="G3" s="15"/>
+      <c r="H3" s="15"/>
+      <c r="I3" s="15"/>
       <c r="J3" s="1"/>
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
@@ -671,15 +668,15 @@
       <c r="B4" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="18" t="s">
+      <c r="C4" s="16" t="s">
         <v>43</v>
       </c>
-      <c r="D4" s="19"/>
-      <c r="E4" s="19"/>
-      <c r="F4" s="19"/>
-      <c r="G4" s="19"/>
-      <c r="H4" s="19"/>
-      <c r="I4" s="19"/>
+      <c r="D4" s="17"/>
+      <c r="E4" s="17"/>
+      <c r="F4" s="17"/>
+      <c r="G4" s="17"/>
+      <c r="H4" s="17"/>
+      <c r="I4" s="17"/>
       <c r="J4" s="3"/>
       <c r="K4" s="3"/>
       <c r="L4" s="3"/>
@@ -701,31 +698,31 @@
       <c r="C5" s="4"/>
     </row>
     <row r="6" spans="1:25" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="11" t="s">
+      <c r="A6" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="11" t="s">
+      <c r="B6" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="11" t="s">
+      <c r="C6" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="D6" s="11" t="s">
+      <c r="D6" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="E6" s="11" t="s">
+      <c r="E6" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="F6" s="11" t="s">
+      <c r="F6" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="G6" s="11" t="s">
+      <c r="G6" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="H6" s="11" t="s">
+      <c r="H6" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="I6" s="11" t="s">
+      <c r="I6" s="9" t="s">
         <v>12</v>
       </c>
       <c r="J6" s="5"/>
@@ -746,31 +743,31 @@
       <c r="Y6" s="5"/>
     </row>
     <row r="7" spans="1:25" ht="45.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="11">
+      <c r="A7" s="9">
         <v>1</v>
       </c>
-      <c r="B7" s="12" t="s">
+      <c r="B7" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="13" t="s">
+      <c r="C7" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="D7" s="11" t="s">
+      <c r="D7" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="E7" s="14">
+      <c r="E7" s="12">
         <v>44809</v>
       </c>
-      <c r="F7" s="14">
+      <c r="F7" s="12">
         <v>44813</v>
       </c>
-      <c r="G7" s="14">
+      <c r="G7" s="12">
         <v>44809</v>
       </c>
-      <c r="H7" s="14">
+      <c r="H7" s="12">
         <v>44813</v>
       </c>
-      <c r="I7" s="11"/>
+      <c r="I7" s="9"/>
       <c r="J7" s="5"/>
       <c r="K7" s="5"/>
       <c r="L7" s="5"/>
@@ -789,31 +786,31 @@
       <c r="Y7" s="5"/>
     </row>
     <row r="8" spans="1:25" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="11">
+      <c r="A8" s="9">
         <v>2</v>
       </c>
-      <c r="B8" s="12" t="s">
+      <c r="B8" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="C8" s="13" t="s">
+      <c r="C8" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="D8" s="11" t="s">
+      <c r="D8" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="E8" s="14">
+      <c r="E8" s="12">
         <v>44814</v>
       </c>
-      <c r="F8" s="14">
+      <c r="F8" s="12">
         <v>44816</v>
       </c>
-      <c r="G8" s="14">
+      <c r="G8" s="12">
         <v>44814</v>
       </c>
-      <c r="H8" s="14">
+      <c r="H8" s="12">
         <v>44816</v>
       </c>
-      <c r="I8" s="11"/>
+      <c r="I8" s="9"/>
       <c r="J8" s="5"/>
       <c r="K8" s="5"/>
       <c r="L8" s="5"/>
@@ -832,27 +829,27 @@
       <c r="Y8" s="5"/>
     </row>
     <row r="9" spans="1:25" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="11"/>
-      <c r="B9" s="11"/>
-      <c r="C9" s="12" t="s">
+      <c r="A9" s="9"/>
+      <c r="B9" s="9"/>
+      <c r="C9" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="D9" s="11" t="s">
+      <c r="D9" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="E9" s="14">
+      <c r="E9" s="12">
         <v>44817</v>
       </c>
-      <c r="F9" s="14">
+      <c r="F9" s="12">
         <v>44819</v>
       </c>
-      <c r="G9" s="14">
+      <c r="G9" s="12">
         <v>44817</v>
       </c>
-      <c r="H9" s="14">
+      <c r="H9" s="12">
         <v>44819</v>
       </c>
-      <c r="I9" s="11"/>
+      <c r="I9" s="9"/>
       <c r="J9" s="5"/>
       <c r="K9" s="5"/>
       <c r="L9" s="5"/>
@@ -871,27 +868,27 @@
       <c r="Y9" s="5"/>
     </row>
     <row r="10" spans="1:25" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="11"/>
-      <c r="B10" s="11"/>
-      <c r="C10" s="12" t="s">
+      <c r="A10" s="9"/>
+      <c r="B10" s="9"/>
+      <c r="C10" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="D10" s="11" t="s">
+      <c r="D10" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="E10" s="14">
+      <c r="E10" s="12">
         <v>44820</v>
       </c>
-      <c r="F10" s="14">
+      <c r="F10" s="12">
         <v>44821</v>
       </c>
-      <c r="G10" s="14">
+      <c r="G10" s="12">
         <v>44820</v>
       </c>
-      <c r="H10" s="14">
+      <c r="H10" s="12">
         <v>44821</v>
       </c>
-      <c r="I10" s="11"/>
+      <c r="I10" s="9"/>
       <c r="J10" s="5"/>
       <c r="K10" s="5"/>
       <c r="L10" s="5"/>
@@ -910,31 +907,31 @@
       <c r="Y10" s="5"/>
     </row>
     <row r="11" spans="1:25" ht="25.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="11">
+      <c r="A11" s="9">
         <v>3</v>
       </c>
-      <c r="B11" s="12" t="s">
+      <c r="B11" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="C11" s="12" t="s">
+      <c r="C11" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="D11" s="11" t="s">
+      <c r="D11" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="E11" s="14">
+      <c r="E11" s="12">
         <v>44822</v>
       </c>
-      <c r="F11" s="14">
+      <c r="F11" s="12">
         <v>44825</v>
       </c>
-      <c r="G11" s="14">
+      <c r="G11" s="12">
         <v>44822</v>
       </c>
-      <c r="H11" s="14">
+      <c r="H11" s="12">
         <v>44825</v>
       </c>
-      <c r="I11" s="11"/>
+      <c r="I11" s="9"/>
       <c r="J11" s="5"/>
       <c r="K11" s="5"/>
       <c r="L11" s="5"/>
@@ -953,31 +950,31 @@
       <c r="Y11" s="5"/>
     </row>
     <row r="12" spans="1:25" ht="45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="11">
+      <c r="A12" s="9">
         <v>4</v>
       </c>
-      <c r="B12" s="12" t="s">
+      <c r="B12" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="C12" s="13" t="s">
+      <c r="C12" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="D12" s="11" t="s">
+      <c r="D12" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="E12" s="14">
+      <c r="E12" s="12">
         <v>44826</v>
       </c>
-      <c r="F12" s="14">
+      <c r="F12" s="12">
         <v>44835</v>
       </c>
-      <c r="G12" s="14">
+      <c r="G12" s="12">
         <v>44826</v>
       </c>
-      <c r="H12" s="14">
+      <c r="H12" s="12">
         <v>44835</v>
       </c>
-      <c r="I12" s="11"/>
+      <c r="I12" s="9"/>
       <c r="J12" s="5"/>
       <c r="K12" s="5"/>
       <c r="L12" s="5"/>
@@ -996,31 +993,31 @@
       <c r="Y12" s="5"/>
     </row>
     <row r="13" spans="1:25" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="11">
+      <c r="A13" s="9">
         <v>5</v>
       </c>
-      <c r="B13" s="12" t="s">
+      <c r="B13" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="C13" s="12" t="s">
+      <c r="C13" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="D13" s="11" t="s">
+      <c r="D13" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="E13" s="14">
+      <c r="E13" s="12">
         <v>44836</v>
       </c>
-      <c r="F13" s="14">
+      <c r="F13" s="12">
         <v>44838</v>
       </c>
-      <c r="G13" s="14">
+      <c r="G13" s="12">
         <v>44836</v>
       </c>
-      <c r="H13" s="14">
+      <c r="H13" s="12">
         <v>44838</v>
       </c>
-      <c r="I13" s="11"/>
+      <c r="I13" s="9"/>
       <c r="J13" s="5"/>
       <c r="K13" s="5"/>
       <c r="L13" s="5"/>
@@ -1039,27 +1036,27 @@
       <c r="Y13" s="5"/>
     </row>
     <row r="14" spans="1:25" ht="62.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="11"/>
-      <c r="B14" s="11"/>
-      <c r="C14" s="13" t="s">
+      <c r="A14" s="9"/>
+      <c r="B14" s="9"/>
+      <c r="C14" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="D14" s="11" t="s">
+      <c r="D14" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="E14" s="14">
+      <c r="E14" s="12">
         <v>44838</v>
       </c>
-      <c r="F14" s="14">
+      <c r="F14" s="12">
         <v>44842</v>
       </c>
-      <c r="G14" s="14">
+      <c r="G14" s="12">
         <v>44838</v>
       </c>
-      <c r="H14" s="14">
+      <c r="H14" s="12">
         <v>44842</v>
       </c>
-      <c r="I14" s="11"/>
+      <c r="I14" s="9"/>
       <c r="J14" s="5"/>
       <c r="K14" s="5"/>
       <c r="L14" s="5"/>
@@ -1078,31 +1075,31 @@
       <c r="Y14" s="5"/>
     </row>
     <row r="15" spans="1:25" ht="41.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="11">
+      <c r="A15" s="9">
         <v>6</v>
       </c>
-      <c r="B15" s="12" t="s">
+      <c r="B15" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="C15" s="13" t="s">
+      <c r="C15" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="D15" s="11" t="s">
+      <c r="D15" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="E15" s="14">
+      <c r="E15" s="12">
         <v>44843</v>
       </c>
-      <c r="F15" s="14">
+      <c r="F15" s="12">
         <v>44846</v>
       </c>
-      <c r="G15" s="14">
+      <c r="G15" s="12">
         <v>44843</v>
       </c>
-      <c r="H15" s="14">
+      <c r="H15" s="12">
         <v>44846</v>
       </c>
-      <c r="I15" s="11"/>
+      <c r="I15" s="9"/>
       <c r="J15" s="5"/>
       <c r="K15" s="5"/>
       <c r="L15" s="5"/>
@@ -1121,27 +1118,27 @@
       <c r="Y15" s="5"/>
     </row>
     <row r="16" spans="1:25" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="11"/>
-      <c r="B16" s="11"/>
-      <c r="C16" s="12" t="s">
+      <c r="A16" s="9"/>
+      <c r="B16" s="9"/>
+      <c r="C16" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="D16" s="11" t="s">
+      <c r="D16" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="E16" s="14">
+      <c r="E16" s="12">
         <v>44847</v>
       </c>
-      <c r="F16" s="14">
+      <c r="F16" s="12">
         <v>44849</v>
       </c>
-      <c r="G16" s="14">
+      <c r="G16" s="12">
         <v>44847</v>
       </c>
-      <c r="H16" s="14">
+      <c r="H16" s="12">
         <v>44849</v>
       </c>
-      <c r="I16" s="11"/>
+      <c r="I16" s="9"/>
       <c r="J16" s="5"/>
       <c r="K16" s="5"/>
       <c r="L16" s="5"/>
@@ -1160,27 +1157,27 @@
       <c r="Y16" s="5"/>
     </row>
     <row r="17" spans="1:25" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="11"/>
-      <c r="B17" s="11"/>
-      <c r="C17" s="12" t="s">
+      <c r="A17" s="9"/>
+      <c r="B17" s="9"/>
+      <c r="C17" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="D17" s="11" t="s">
+      <c r="D17" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="E17" s="14">
+      <c r="E17" s="12">
         <v>44850</v>
       </c>
-      <c r="F17" s="14">
+      <c r="F17" s="12">
         <v>44852</v>
       </c>
-      <c r="G17" s="14">
+      <c r="G17" s="12">
         <v>44850</v>
       </c>
-      <c r="H17" s="14">
+      <c r="H17" s="12">
         <v>44852</v>
       </c>
-      <c r="I17" s="11"/>
+      <c r="I17" s="9"/>
       <c r="J17" s="5"/>
       <c r="K17" s="5"/>
       <c r="L17" s="5"/>
@@ -1199,25 +1196,27 @@
       <c r="Y17" s="5"/>
     </row>
     <row r="18" spans="1:25" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="11"/>
-      <c r="B18" s="11"/>
-      <c r="C18" s="12" t="s">
+      <c r="A18" s="9"/>
+      <c r="B18" s="9"/>
+      <c r="C18" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="D18" s="11" t="s">
+      <c r="D18" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="E18" s="14">
+      <c r="E18" s="12">
         <v>44853</v>
       </c>
-      <c r="F18" s="14">
+      <c r="F18" s="12">
         <v>44855</v>
       </c>
-      <c r="G18" s="14">
+      <c r="G18" s="12">
         <v>44853</v>
       </c>
-      <c r="H18" s="14"/>
-      <c r="I18" s="11"/>
+      <c r="H18" s="12">
+        <v>44855</v>
+      </c>
+      <c r="I18" s="9"/>
       <c r="J18" s="5"/>
       <c r="K18" s="5"/>
       <c r="L18" s="5"/>
@@ -1236,23 +1235,23 @@
       <c r="Y18" s="5"/>
     </row>
     <row r="19" spans="1:25" ht="21.6" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A19" s="11"/>
-      <c r="B19" s="11"/>
-      <c r="C19" s="15" t="s">
+      <c r="A19" s="9"/>
+      <c r="B19" s="9"/>
+      <c r="C19" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="D19" s="11" t="s">
+      <c r="D19" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="E19" s="14">
+      <c r="E19" s="12">
         <v>44856</v>
       </c>
-      <c r="F19" s="14">
+      <c r="F19" s="12">
         <v>44858</v>
       </c>
-      <c r="G19" s="14"/>
-      <c r="H19" s="14"/>
-      <c r="I19" s="11"/>
+      <c r="G19" s="12"/>
+      <c r="H19" s="12"/>
+      <c r="I19" s="9"/>
       <c r="J19" s="5"/>
       <c r="K19" s="5"/>
       <c r="L19" s="5"/>
@@ -1271,23 +1270,23 @@
       <c r="Y19" s="5"/>
     </row>
     <row r="20" spans="1:25" ht="22.95" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A20" s="11"/>
-      <c r="B20" s="11"/>
-      <c r="C20" s="15" t="s">
+      <c r="A20" s="9"/>
+      <c r="B20" s="9"/>
+      <c r="C20" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="D20" s="11" t="s">
+      <c r="D20" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="E20" s="14">
+      <c r="E20" s="12">
         <v>44859</v>
       </c>
-      <c r="F20" s="14">
+      <c r="F20" s="12">
         <v>44861</v>
       </c>
-      <c r="G20" s="14"/>
-      <c r="H20" s="14"/>
-      <c r="I20" s="11"/>
+      <c r="G20" s="12"/>
+      <c r="H20" s="12"/>
+      <c r="I20" s="9"/>
       <c r="J20" s="5"/>
       <c r="K20" s="5"/>
       <c r="L20" s="5"/>
@@ -1306,23 +1305,23 @@
       <c r="Y20" s="5"/>
     </row>
     <row r="21" spans="1:25" ht="22.2" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A21" s="11"/>
-      <c r="B21" s="11"/>
-      <c r="C21" s="15" t="s">
+      <c r="A21" s="9"/>
+      <c r="B21" s="9"/>
+      <c r="C21" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="D21" s="11" t="s">
+      <c r="D21" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="E21" s="14">
+      <c r="E21" s="12">
         <v>44862</v>
       </c>
-      <c r="F21" s="14">
+      <c r="F21" s="12">
         <v>44863</v>
       </c>
-      <c r="G21" s="14"/>
-      <c r="H21" s="14"/>
-      <c r="I21" s="11"/>
+      <c r="G21" s="12"/>
+      <c r="H21" s="12"/>
+      <c r="I21" s="9"/>
       <c r="J21" s="5"/>
       <c r="K21" s="5"/>
       <c r="L21" s="5"/>
@@ -1341,23 +1340,23 @@
       <c r="Y21" s="5"/>
     </row>
     <row r="22" spans="1:25" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A22" s="11"/>
-      <c r="B22" s="11"/>
-      <c r="C22" s="15" t="s">
+      <c r="A22" s="9"/>
+      <c r="B22" s="9"/>
+      <c r="C22" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="D22" s="11" t="s">
+      <c r="D22" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="E22" s="14">
+      <c r="E22" s="12">
         <v>44864</v>
       </c>
-      <c r="F22" s="14">
+      <c r="F22" s="12">
         <v>44866</v>
       </c>
-      <c r="G22" s="14"/>
-      <c r="H22" s="14"/>
-      <c r="I22" s="11"/>
+      <c r="G22" s="12"/>
+      <c r="H22" s="12"/>
+      <c r="I22" s="9"/>
       <c r="J22" s="5"/>
       <c r="K22" s="5"/>
       <c r="L22" s="5"/>
@@ -1375,24 +1374,24 @@
       <c r="X22" s="5"/>
       <c r="Y22" s="5"/>
     </row>
-    <row r="23" spans="1:25" s="10" customFormat="1" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A23" s="11"/>
-      <c r="B23" s="11"/>
-      <c r="C23" s="15" t="s">
+    <row r="23" spans="1:25" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A23" s="9"/>
+      <c r="B23" s="9"/>
+      <c r="C23" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="D23" s="11" t="s">
+      <c r="D23" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="E23" s="14">
+      <c r="E23" s="12">
         <v>44867</v>
       </c>
-      <c r="F23" s="14">
+      <c r="F23" s="12">
         <v>44869</v>
       </c>
-      <c r="G23" s="14"/>
-      <c r="H23" s="14"/>
-      <c r="I23" s="11"/>
+      <c r="G23" s="12"/>
+      <c r="H23" s="12"/>
+      <c r="I23" s="9"/>
       <c r="J23" s="5"/>
       <c r="K23" s="5"/>
       <c r="L23" s="5"/>
@@ -1411,23 +1410,23 @@
       <c r="Y23" s="5"/>
     </row>
     <row r="24" spans="1:25" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="11"/>
-      <c r="B24" s="11"/>
-      <c r="C24" s="12" t="s">
+      <c r="A24" s="9"/>
+      <c r="B24" s="9"/>
+      <c r="C24" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="D24" s="11" t="s">
+      <c r="D24" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="E24" s="14">
+      <c r="E24" s="12">
         <v>44870</v>
       </c>
-      <c r="F24" s="14">
+      <c r="F24" s="12">
         <v>44873</v>
       </c>
-      <c r="G24" s="14"/>
-      <c r="H24" s="14"/>
-      <c r="I24" s="11"/>
+      <c r="G24" s="12"/>
+      <c r="H24" s="12"/>
+      <c r="I24" s="9"/>
       <c r="J24" s="5"/>
       <c r="K24" s="5"/>
       <c r="L24" s="5"/>
@@ -1446,23 +1445,23 @@
       <c r="Y24" s="5"/>
     </row>
     <row r="25" spans="1:25" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="11"/>
-      <c r="B25" s="11"/>
-      <c r="C25" s="12" t="s">
+      <c r="A25" s="9"/>
+      <c r="B25" s="9"/>
+      <c r="C25" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="D25" s="11" t="s">
+      <c r="D25" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="E25" s="14">
+      <c r="E25" s="12">
         <v>44875</v>
       </c>
-      <c r="F25" s="14">
+      <c r="F25" s="12">
         <v>44880</v>
       </c>
-      <c r="G25" s="14"/>
-      <c r="H25" s="14"/>
-      <c r="I25" s="11"/>
+      <c r="G25" s="12"/>
+      <c r="H25" s="12"/>
+      <c r="I25" s="9"/>
       <c r="J25" s="5"/>
       <c r="K25" s="5"/>
       <c r="L25" s="5"/>
@@ -1481,25 +1480,25 @@
       <c r="Y25" s="5"/>
     </row>
     <row r="26" spans="1:25" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="11">
+      <c r="A26" s="9">
         <v>7</v>
       </c>
-      <c r="B26" s="12" t="s">
+      <c r="B26" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="C26" s="12"/>
-      <c r="D26" s="11" t="s">
+      <c r="C26" s="10"/>
+      <c r="D26" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="E26" s="14">
+      <c r="E26" s="12">
         <v>44881</v>
       </c>
-      <c r="F26" s="14">
+      <c r="F26" s="12">
         <v>44883</v>
       </c>
-      <c r="G26" s="14"/>
-      <c r="H26" s="14"/>
-      <c r="I26" s="11"/>
+      <c r="G26" s="12"/>
+      <c r="H26" s="12"/>
+      <c r="I26" s="9"/>
       <c r="J26" s="5"/>
       <c r="K26" s="5"/>
       <c r="L26" s="5"/>
@@ -1518,27 +1517,27 @@
       <c r="Y26" s="5"/>
     </row>
     <row r="27" spans="1:25" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="11">
+      <c r="A27" s="9">
         <v>8</v>
       </c>
-      <c r="B27" s="12" t="s">
+      <c r="B27" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="C27" s="12" t="s">
+      <c r="C27" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="D27" s="11" t="s">
+      <c r="D27" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="E27" s="14">
+      <c r="E27" s="12">
         <v>44884</v>
       </c>
-      <c r="F27" s="14">
+      <c r="F27" s="12">
         <v>44889</v>
       </c>
-      <c r="G27" s="14"/>
-      <c r="H27" s="14"/>
-      <c r="I27" s="11"/>
+      <c r="G27" s="12"/>
+      <c r="H27" s="12"/>
+      <c r="I27" s="9"/>
       <c r="J27" s="5"/>
       <c r="K27" s="5"/>
       <c r="L27" s="5"/>
@@ -1557,25 +1556,25 @@
       <c r="Y27" s="5"/>
     </row>
     <row r="28" spans="1:25" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="11">
+      <c r="A28" s="9">
         <v>9</v>
       </c>
-      <c r="B28" s="12" t="s">
+      <c r="B28" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="C28" s="12"/>
-      <c r="D28" s="11" t="s">
+      <c r="C28" s="10"/>
+      <c r="D28" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="E28" s="14">
+      <c r="E28" s="12">
         <v>44890</v>
       </c>
-      <c r="F28" s="14">
+      <c r="F28" s="12">
         <v>44894</v>
       </c>
-      <c r="G28" s="14"/>
-      <c r="H28" s="14"/>
-      <c r="I28" s="11"/>
+      <c r="G28" s="12"/>
+      <c r="H28" s="12"/>
+      <c r="I28" s="9"/>
       <c r="J28" s="5"/>
       <c r="K28" s="5"/>
       <c r="L28" s="5"/>
@@ -1676,7 +1675,7 @@
     </row>
     <row r="32" spans="1:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="6"/>
-      <c r="B32" s="9"/>
+      <c r="B32" s="6"/>
       <c r="C32" s="7"/>
       <c r="D32" s="6"/>
       <c r="E32" s="8"/>

</xml_diff>

<commit_message>
improve ui, song manager added
</commit_message>
<xml_diff>
--- a/PlanExcel/plan.xlsx
+++ b/PlanExcel/plan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\~project\AndroidKotlin\MUSIC\PlanExcel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D5FC623-90D0-4C47-8BC0-4D8F3C9A7B0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B03E7417-15E9-45FF-AFBB-D3A1A9154B76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -558,8 +558,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Y1003"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1249,7 +1249,9 @@
       <c r="F19" s="12">
         <v>44858</v>
       </c>
-      <c r="G19" s="12"/>
+      <c r="G19" s="12">
+        <v>44856</v>
+      </c>
       <c r="H19" s="12"/>
       <c r="I19" s="9"/>
       <c r="J19" s="5"/>

</xml_diff>

<commit_message>
add view collection and it crud
</commit_message>
<xml_diff>
--- a/PlanExcel/plan.xlsx
+++ b/PlanExcel/plan.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\~project\AndroidKotlin\MUSIC\PlanExcel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B03E7417-15E9-45FF-AFBB-D3A1A9154B76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D46C4B8-14BE-4C49-A9E9-C6BD7A3A3FD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -559,7 +559,7 @@
   <dimension ref="A1:Y1003"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1252,7 +1252,9 @@
       <c r="G19" s="12">
         <v>44856</v>
       </c>
-      <c r="H19" s="12"/>
+      <c r="H19" s="12">
+        <v>44858</v>
+      </c>
       <c r="I19" s="9"/>
       <c r="J19" s="5"/>
       <c r="K19" s="5"/>
@@ -1286,7 +1288,9 @@
       <c r="F20" s="12">
         <v>44861</v>
       </c>
-      <c r="G20" s="12"/>
+      <c r="G20" s="12">
+        <v>44859</v>
+      </c>
       <c r="H20" s="12"/>
       <c r="I20" s="9"/>
       <c r="J20" s="5"/>

</xml_diff>

<commit_message>
update view for clicking in home/search fragment
</commit_message>
<xml_diff>
--- a/PlanExcel/plan.xlsx
+++ b/PlanExcel/plan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\~project\AndroidKotlin\MUSIC\PlanExcel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D46C4B8-14BE-4C49-A9E9-C6BD7A3A3FD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4491D67-0E4E-497E-A6AA-FA9DA809191F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -558,8 +558,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Y1003"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
double back to leave, fix some fragment transaction problems
</commit_message>
<xml_diff>
--- a/PlanExcel/plan.xlsx
+++ b/PlanExcel/plan.xlsx
@@ -557,8 +557,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y1003"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1368,7 +1368,9 @@
       <c r="G22" s="12">
         <v>44864</v>
       </c>
-      <c r="H22" s="12"/>
+      <c r="H22" s="12">
+        <v>44866</v>
+      </c>
       <c r="I22" s="9"/>
       <c r="J22" s="5"/>
       <c r="K22" s="5"/>
@@ -1402,8 +1404,12 @@
       <c r="F23" s="12">
         <v>44869</v>
       </c>
-      <c r="G23" s="12"/>
-      <c r="H23" s="12"/>
+      <c r="G23" s="12">
+        <v>44867</v>
+      </c>
+      <c r="H23" s="12">
+        <v>44869</v>
+      </c>
       <c r="I23" s="9"/>
       <c r="J23" s="5"/>
       <c r="K23" s="5"/>
@@ -1437,7 +1443,9 @@
       <c r="F24" s="12">
         <v>44873</v>
       </c>
-      <c r="G24" s="12"/>
+      <c r="G24" s="12">
+        <v>44870</v>
+      </c>
       <c r="H24" s="12"/>
       <c r="I24" s="9"/>
       <c r="J24" s="5"/>

</xml_diff>

<commit_message>
update trim string for searching
</commit_message>
<xml_diff>
--- a/PlanExcel/plan.xlsx
+++ b/PlanExcel/plan.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
   <si>
     <t>KHOA CÔNG NGHỆ THÔNG TIN</t>
   </si>
@@ -70,9 +70,6 @@
   <si>
     <t>Tìm hiểu các chức năng cần thiết của một
 ứng dụng nghe nhạc trực tuyến</t>
-  </si>
-  <si>
-    <t>x</t>
   </si>
   <si>
     <t>Viết đặc tả thiết kế cho ứng dụng</t>
@@ -167,6 +164,9 @@
 - Để lại bình luận cho từng bài hát.
 - Tạo giao diện trực quan và dễ dàng thao tác. </t>
   </si>
+  <si>
+    <t>Người thực hiện:</t>
+  </si>
 </sst>
 </file>
 
@@ -175,7 +175,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd/mm"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -199,6 +199,7 @@
       <name val="Times New Roman"/>
     </font>
     <font>
+      <b/>
       <sz val="16"/>
       <color theme="1"/>
       <name val="Times New Roman"/>
@@ -206,10 +207,43 @@
     </font>
     <font>
       <b/>
-      <sz val="16"/>
+      <sz val="20"/>
       <color theme="1"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+    </font>
+    <font>
+      <sz val="20"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="20"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="20"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="22"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="22"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -238,7 +272,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -262,31 +296,50 @@
     <xf numFmtId="164" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -336,12 +389,11 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table_1" displayName="Table_1" ref="A6:I34" headerRowCount="0">
-  <tableColumns count="9">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table_1" displayName="Table_1" ref="A8:H36" headerRowCount="0">
+  <tableColumns count="8">
     <tableColumn id="1" name="Column1"/>
     <tableColumn id="2" name="Column2"/>
     <tableColumn id="3" name="Column3"/>
-    <tableColumn id="4" name="Column4"/>
     <tableColumn id="6" name="Column6"/>
     <tableColumn id="7" name="Column7"/>
     <tableColumn id="8" name="Column8"/>
@@ -349,11 +401,6 @@
     <tableColumn id="10" name="Column10"/>
   </tableColumns>
   <tableStyleInfo name="Sheet1-style" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="0"/>
-  <extLst>
-    <ext uri="GoogleSheetsCustomDataVersion1">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" headerRowCount="1"/>
-    </ext>
-  </extLst>
 </table>
 </file>
 
@@ -555,38 +602,37 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Y1003"/>
+  <dimension ref="A1:X1005"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G25" sqref="G25"/>
+    <sheetView tabSelected="1" topLeftCell="B16" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="8.6640625" customWidth="1"/>
-    <col min="2" max="2" width="46.5546875" customWidth="1"/>
-    <col min="3" max="3" width="87.88671875" customWidth="1"/>
-    <col min="4" max="4" width="26.33203125" customWidth="1"/>
-    <col min="5" max="5" width="27.88671875" customWidth="1"/>
-    <col min="6" max="6" width="28.33203125" customWidth="1"/>
-    <col min="7" max="7" width="26.33203125" customWidth="1"/>
-    <col min="8" max="8" width="27.33203125" customWidth="1"/>
-    <col min="9" max="9" width="11.33203125" customWidth="1"/>
-    <col min="10" max="25" width="8.6640625" customWidth="1"/>
+    <col min="2" max="2" width="54" customWidth="1"/>
+    <col min="3" max="3" width="99.44140625" customWidth="1"/>
+    <col min="4" max="4" width="33.88671875" customWidth="1"/>
+    <col min="5" max="5" width="35.21875" customWidth="1"/>
+    <col min="6" max="6" width="32.21875" customWidth="1"/>
+    <col min="7" max="7" width="37.77734375" customWidth="1"/>
+    <col min="8" max="8" width="16.77734375" customWidth="1"/>
+    <col min="9" max="24" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" ht="33.6" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="14" t="s">
+    <row r="1" spans="1:24" ht="33.6" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
-      <c r="G1" s="15"/>
-      <c r="H1" s="15"/>
-      <c r="I1" s="15"/>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
+      <c r="H1" s="22"/>
+      <c r="I1" s="1"/>
       <c r="J1" s="1"/>
       <c r="K1" s="1"/>
       <c r="L1" s="1"/>
@@ -602,20 +648,19 @@
       <c r="V1" s="1"/>
       <c r="W1" s="1"/>
       <c r="X1" s="1"/>
-      <c r="Y1" s="1"/>
-    </row>
-    <row r="2" spans="1:25" ht="31.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="14" t="s">
+    </row>
+    <row r="2" spans="1:24" ht="38.4" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="15"/>
-      <c r="C2" s="15"/>
-      <c r="D2" s="15"/>
-      <c r="E2" s="15"/>
-      <c r="F2" s="15"/>
-      <c r="G2" s="15"/>
-      <c r="H2" s="15"/>
-      <c r="I2" s="15"/>
+      <c r="B2" s="22"/>
+      <c r="C2" s="22"/>
+      <c r="D2" s="22"/>
+      <c r="E2" s="22"/>
+      <c r="F2" s="22"/>
+      <c r="G2" s="22"/>
+      <c r="H2" s="22"/>
+      <c r="I2" s="1"/>
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
       <c r="L2" s="1"/>
@@ -631,20 +676,19 @@
       <c r="V2" s="1"/>
       <c r="W2" s="1"/>
       <c r="X2" s="1"/>
-      <c r="Y2" s="1"/>
-    </row>
-    <row r="3" spans="1:25" ht="19.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="14" t="s">
+    </row>
+    <row r="3" spans="1:24" ht="48" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="15"/>
-      <c r="C3" s="15"/>
-      <c r="D3" s="15"/>
-      <c r="E3" s="15"/>
-      <c r="F3" s="15"/>
-      <c r="G3" s="15"/>
-      <c r="H3" s="15"/>
-      <c r="I3" s="15"/>
+      <c r="B3" s="22"/>
+      <c r="C3" s="22"/>
+      <c r="D3" s="22"/>
+      <c r="E3" s="22"/>
+      <c r="F3" s="22"/>
+      <c r="G3" s="22"/>
+      <c r="H3" s="22"/>
+      <c r="I3" s="1"/>
       <c r="J3" s="1"/>
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
@@ -660,22 +704,21 @@
       <c r="V3" s="1"/>
       <c r="W3" s="1"/>
       <c r="X3" s="1"/>
-      <c r="Y3" s="1"/>
-    </row>
-    <row r="4" spans="1:25" ht="154.19999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="4" spans="1:24" ht="201" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A4" s="2"/>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="16" t="s">
-        <v>43</v>
-      </c>
-      <c r="D4" s="17"/>
-      <c r="E4" s="17"/>
-      <c r="F4" s="17"/>
-      <c r="G4" s="17"/>
-      <c r="H4" s="17"/>
-      <c r="I4" s="17"/>
+      <c r="C4" s="23" t="s">
+        <v>42</v>
+      </c>
+      <c r="D4" s="24"/>
+      <c r="E4" s="24"/>
+      <c r="F4" s="24"/>
+      <c r="G4" s="24"/>
+      <c r="H4" s="24"/>
+      <c r="I4" s="3"/>
       <c r="J4" s="3"/>
       <c r="K4" s="3"/>
       <c r="L4" s="3"/>
@@ -691,125 +734,94 @@
       <c r="V4" s="3"/>
       <c r="W4" s="3"/>
       <c r="X4" s="3"/>
-      <c r="Y4" s="3"/>
-    </row>
-    <row r="5" spans="1:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C5" s="4"/>
-    </row>
-    <row r="6" spans="1:25" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="9" t="s">
+    </row>
+    <row r="5" spans="1:24" s="11" customFormat="1" ht="31.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="9"/>
+      <c r="B5" s="9"/>
+      <c r="C5" s="10"/>
+      <c r="I5" s="3"/>
+      <c r="J5" s="3"/>
+      <c r="K5" s="3"/>
+      <c r="L5" s="3"/>
+      <c r="M5" s="3"/>
+      <c r="N5" s="3"/>
+      <c r="O5" s="3"/>
+      <c r="P5" s="3"/>
+      <c r="Q5" s="3"/>
+      <c r="R5" s="3"/>
+      <c r="S5" s="3"/>
+      <c r="T5" s="3"/>
+      <c r="U5" s="3"/>
+      <c r="V5" s="3"/>
+      <c r="W5" s="3"/>
+      <c r="X5" s="3"/>
+    </row>
+    <row r="6" spans="1:24" s="11" customFormat="1" ht="33.6" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A6" s="12"/>
+      <c r="B6" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="C6" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" s="14"/>
+      <c r="E6" s="14"/>
+      <c r="F6" s="14"/>
+      <c r="G6" s="14"/>
+      <c r="H6" s="14"/>
+      <c r="I6" s="3"/>
+      <c r="J6" s="3"/>
+      <c r="K6" s="3"/>
+      <c r="L6" s="3"/>
+      <c r="M6" s="3"/>
+      <c r="N6" s="3"/>
+      <c r="O6" s="3"/>
+      <c r="P6" s="3"/>
+      <c r="Q6" s="3"/>
+      <c r="R6" s="3"/>
+      <c r="S6" s="3"/>
+      <c r="T6" s="3"/>
+      <c r="U6" s="3"/>
+      <c r="V6" s="3"/>
+      <c r="W6" s="3"/>
+      <c r="X6" s="3"/>
+    </row>
+    <row r="7" spans="1:24" ht="32.4" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A7" s="14"/>
+      <c r="B7" s="14"/>
+      <c r="C7" s="15"/>
+      <c r="D7" s="14"/>
+      <c r="E7" s="14"/>
+      <c r="F7" s="14"/>
+      <c r="G7" s="14"/>
+      <c r="H7" s="14"/>
+    </row>
+    <row r="8" spans="1:24" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="9" t="s">
+      <c r="B8" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="9" t="s">
+      <c r="C8" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="D6" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="E6" s="9" t="s">
+      <c r="D8" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="F6" s="9" t="s">
+      <c r="E8" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="G6" s="9" t="s">
+      <c r="F8" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="H6" s="9" t="s">
+      <c r="G8" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="I6" s="9" t="s">
+      <c r="H8" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="J6" s="5"/>
-      <c r="K6" s="5"/>
-      <c r="L6" s="5"/>
-      <c r="M6" s="5"/>
-      <c r="N6" s="5"/>
-      <c r="O6" s="5"/>
-      <c r="P6" s="5"/>
-      <c r="Q6" s="5"/>
-      <c r="R6" s="5"/>
-      <c r="S6" s="5"/>
-      <c r="T6" s="5"/>
-      <c r="U6" s="5"/>
-      <c r="V6" s="5"/>
-      <c r="W6" s="5"/>
-      <c r="X6" s="5"/>
-      <c r="Y6" s="5"/>
-    </row>
-    <row r="7" spans="1:25" ht="45.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="9">
-        <v>1</v>
-      </c>
-      <c r="B7" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="C7" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="D7" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="E7" s="12">
-        <v>44809</v>
-      </c>
-      <c r="F7" s="12">
-        <v>44813</v>
-      </c>
-      <c r="G7" s="12">
-        <v>44809</v>
-      </c>
-      <c r="H7" s="12">
-        <v>44813</v>
-      </c>
-      <c r="I7" s="9"/>
-      <c r="J7" s="5"/>
-      <c r="K7" s="5"/>
-      <c r="L7" s="5"/>
-      <c r="M7" s="5"/>
-      <c r="N7" s="5"/>
-      <c r="O7" s="5"/>
-      <c r="P7" s="5"/>
-      <c r="Q7" s="5"/>
-      <c r="R7" s="5"/>
-      <c r="S7" s="5"/>
-      <c r="T7" s="5"/>
-      <c r="U7" s="5"/>
-      <c r="V7" s="5"/>
-      <c r="W7" s="5"/>
-      <c r="X7" s="5"/>
-      <c r="Y7" s="5"/>
-    </row>
-    <row r="8" spans="1:25" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="9">
-        <v>2</v>
-      </c>
-      <c r="B8" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="C8" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="D8" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="E8" s="12">
-        <v>44814</v>
-      </c>
-      <c r="F8" s="12">
-        <v>44816</v>
-      </c>
-      <c r="G8" s="12">
-        <v>44814</v>
-      </c>
-      <c r="H8" s="12">
-        <v>44816</v>
-      </c>
-      <c r="I8" s="9"/>
+      <c r="I8" s="5"/>
       <c r="J8" s="5"/>
       <c r="K8" s="5"/>
       <c r="L8" s="5"/>
@@ -825,30 +837,31 @@
       <c r="V8" s="5"/>
       <c r="W8" s="5"/>
       <c r="X8" s="5"/>
-      <c r="Y8" s="5"/>
-    </row>
-    <row r="9" spans="1:25" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="9"/>
-      <c r="B9" s="9"/>
-      <c r="C9" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="D9" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="E9" s="12">
-        <v>44817</v>
-      </c>
-      <c r="F9" s="12">
-        <v>44819</v>
-      </c>
-      <c r="G9" s="12">
-        <v>44817</v>
-      </c>
-      <c r="H9" s="12">
-        <v>44819</v>
-      </c>
-      <c r="I9" s="9"/>
+    </row>
+    <row r="9" spans="1:24" ht="58.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="16">
+        <v>1</v>
+      </c>
+      <c r="B9" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="D9" s="19">
+        <v>44809</v>
+      </c>
+      <c r="E9" s="19">
+        <v>44813</v>
+      </c>
+      <c r="F9" s="19">
+        <v>44809</v>
+      </c>
+      <c r="G9" s="19">
+        <v>44813</v>
+      </c>
+      <c r="H9" s="16"/>
+      <c r="I9" s="5"/>
       <c r="J9" s="5"/>
       <c r="K9" s="5"/>
       <c r="L9" s="5"/>
@@ -864,30 +877,31 @@
       <c r="V9" s="5"/>
       <c r="W9" s="5"/>
       <c r="X9" s="5"/>
-      <c r="Y9" s="5"/>
-    </row>
-    <row r="10" spans="1:25" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="9"/>
-      <c r="B10" s="9"/>
-      <c r="C10" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="D10" s="9" t="s">
+    </row>
+    <row r="10" spans="1:24" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="16">
+        <v>2</v>
+      </c>
+      <c r="B10" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="E10" s="12">
-        <v>44820</v>
-      </c>
-      <c r="F10" s="12">
-        <v>44821</v>
-      </c>
-      <c r="G10" s="12">
-        <v>44820</v>
-      </c>
-      <c r="H10" s="12">
-        <v>44821</v>
-      </c>
-      <c r="I10" s="9"/>
+      <c r="C10" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="D10" s="19">
+        <v>44814</v>
+      </c>
+      <c r="E10" s="19">
+        <v>44816</v>
+      </c>
+      <c r="F10" s="19">
+        <v>44814</v>
+      </c>
+      <c r="G10" s="19">
+        <v>44816</v>
+      </c>
+      <c r="H10" s="16"/>
+      <c r="I10" s="5"/>
       <c r="J10" s="5"/>
       <c r="K10" s="5"/>
       <c r="L10" s="5"/>
@@ -903,34 +917,27 @@
       <c r="V10" s="5"/>
       <c r="W10" s="5"/>
       <c r="X10" s="5"/>
-      <c r="Y10" s="5"/>
-    </row>
-    <row r="11" spans="1:25" ht="25.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="9">
-        <v>3</v>
-      </c>
-      <c r="B11" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="C11" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="D11" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="E11" s="12">
-        <v>44822</v>
-      </c>
-      <c r="F11" s="12">
-        <v>44825</v>
-      </c>
-      <c r="G11" s="12">
-        <v>44822</v>
-      </c>
-      <c r="H11" s="12">
-        <v>44825</v>
-      </c>
-      <c r="I11" s="9"/>
+    </row>
+    <row r="11" spans="1:24" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="16"/>
+      <c r="B11" s="16"/>
+      <c r="C11" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="D11" s="19">
+        <v>44817</v>
+      </c>
+      <c r="E11" s="19">
+        <v>44819</v>
+      </c>
+      <c r="F11" s="19">
+        <v>44817</v>
+      </c>
+      <c r="G11" s="19">
+        <v>44819</v>
+      </c>
+      <c r="H11" s="16"/>
+      <c r="I11" s="5"/>
       <c r="J11" s="5"/>
       <c r="K11" s="5"/>
       <c r="L11" s="5"/>
@@ -946,34 +953,27 @@
       <c r="V11" s="5"/>
       <c r="W11" s="5"/>
       <c r="X11" s="5"/>
-      <c r="Y11" s="5"/>
-    </row>
-    <row r="12" spans="1:25" ht="45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="9">
-        <v>4</v>
-      </c>
-      <c r="B12" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="C12" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="D12" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="E12" s="12">
-        <v>44826</v>
-      </c>
-      <c r="F12" s="12">
-        <v>44835</v>
-      </c>
-      <c r="G12" s="12">
-        <v>44826</v>
-      </c>
-      <c r="H12" s="12">
-        <v>44835</v>
-      </c>
-      <c r="I12" s="9"/>
+    </row>
+    <row r="12" spans="1:24" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="16"/>
+      <c r="B12" s="16"/>
+      <c r="C12" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="D12" s="19">
+        <v>44820</v>
+      </c>
+      <c r="E12" s="19">
+        <v>44821</v>
+      </c>
+      <c r="F12" s="19">
+        <v>44820</v>
+      </c>
+      <c r="G12" s="19">
+        <v>44821</v>
+      </c>
+      <c r="H12" s="16"/>
+      <c r="I12" s="5"/>
       <c r="J12" s="5"/>
       <c r="K12" s="5"/>
       <c r="L12" s="5"/>
@@ -989,34 +989,31 @@
       <c r="V12" s="5"/>
       <c r="W12" s="5"/>
       <c r="X12" s="5"/>
-      <c r="Y12" s="5"/>
-    </row>
-    <row r="13" spans="1:25" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="9">
-        <v>5</v>
-      </c>
-      <c r="B13" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="C13" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="D13" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="E13" s="12">
-        <v>44836</v>
-      </c>
-      <c r="F13" s="12">
-        <v>44838</v>
-      </c>
-      <c r="G13" s="12">
-        <v>44836</v>
-      </c>
-      <c r="H13" s="12">
-        <v>44838</v>
-      </c>
-      <c r="I13" s="9"/>
+    </row>
+    <row r="13" spans="1:24" ht="37.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="16">
+        <v>3</v>
+      </c>
+      <c r="B13" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="C13" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="D13" s="19">
+        <v>44822</v>
+      </c>
+      <c r="E13" s="19">
+        <v>44825</v>
+      </c>
+      <c r="F13" s="19">
+        <v>44822</v>
+      </c>
+      <c r="G13" s="19">
+        <v>44825</v>
+      </c>
+      <c r="H13" s="16"/>
+      <c r="I13" s="5"/>
       <c r="J13" s="5"/>
       <c r="K13" s="5"/>
       <c r="L13" s="5"/>
@@ -1032,30 +1029,31 @@
       <c r="V13" s="5"/>
       <c r="W13" s="5"/>
       <c r="X13" s="5"/>
-      <c r="Y13" s="5"/>
-    </row>
-    <row r="14" spans="1:25" ht="62.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="9"/>
-      <c r="B14" s="9"/>
-      <c r="C14" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="D14" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="E14" s="12">
-        <v>44838</v>
-      </c>
-      <c r="F14" s="12">
-        <v>44842</v>
-      </c>
-      <c r="G14" s="12">
-        <v>44838</v>
-      </c>
-      <c r="H14" s="12">
-        <v>44842</v>
-      </c>
-      <c r="I14" s="9"/>
+    </row>
+    <row r="14" spans="1:24" ht="66" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="16">
+        <v>4</v>
+      </c>
+      <c r="B14" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="C14" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="D14" s="19">
+        <v>44826</v>
+      </c>
+      <c r="E14" s="19">
+        <v>44835</v>
+      </c>
+      <c r="F14" s="19">
+        <v>44826</v>
+      </c>
+      <c r="G14" s="19">
+        <v>44835</v>
+      </c>
+      <c r="H14" s="16"/>
+      <c r="I14" s="5"/>
       <c r="J14" s="5"/>
       <c r="K14" s="5"/>
       <c r="L14" s="5"/>
@@ -1071,34 +1069,31 @@
       <c r="V14" s="5"/>
       <c r="W14" s="5"/>
       <c r="X14" s="5"/>
-      <c r="Y14" s="5"/>
-    </row>
-    <row r="15" spans="1:25" ht="41.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="9">
-        <v>6</v>
-      </c>
-      <c r="B15" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="C15" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="D15" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="E15" s="12">
-        <v>44843</v>
-      </c>
-      <c r="F15" s="12">
-        <v>44846</v>
-      </c>
-      <c r="G15" s="12">
-        <v>44843</v>
-      </c>
-      <c r="H15" s="12">
-        <v>44846</v>
-      </c>
-      <c r="I15" s="9"/>
+    </row>
+    <row r="15" spans="1:24" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="16">
+        <v>5</v>
+      </c>
+      <c r="B15" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="C15" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="D15" s="19">
+        <v>44836</v>
+      </c>
+      <c r="E15" s="19">
+        <v>44838</v>
+      </c>
+      <c r="F15" s="19">
+        <v>44836</v>
+      </c>
+      <c r="G15" s="19">
+        <v>44838</v>
+      </c>
+      <c r="H15" s="16"/>
+      <c r="I15" s="5"/>
       <c r="J15" s="5"/>
       <c r="K15" s="5"/>
       <c r="L15" s="5"/>
@@ -1114,30 +1109,27 @@
       <c r="V15" s="5"/>
       <c r="W15" s="5"/>
       <c r="X15" s="5"/>
-      <c r="Y15" s="5"/>
-    </row>
-    <row r="16" spans="1:25" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="9"/>
-      <c r="B16" s="9"/>
-      <c r="C16" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="D16" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="E16" s="12">
-        <v>44847</v>
-      </c>
-      <c r="F16" s="12">
-        <v>44849</v>
-      </c>
-      <c r="G16" s="12">
-        <v>44847</v>
-      </c>
-      <c r="H16" s="12">
-        <v>44849</v>
-      </c>
-      <c r="I16" s="9"/>
+    </row>
+    <row r="16" spans="1:24" ht="62.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="16"/>
+      <c r="B16" s="16"/>
+      <c r="C16" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="D16" s="19">
+        <v>44838</v>
+      </c>
+      <c r="E16" s="19">
+        <v>44842</v>
+      </c>
+      <c r="F16" s="19">
+        <v>44838</v>
+      </c>
+      <c r="G16" s="19">
+        <v>44842</v>
+      </c>
+      <c r="H16" s="16"/>
+      <c r="I16" s="5"/>
       <c r="J16" s="5"/>
       <c r="K16" s="5"/>
       <c r="L16" s="5"/>
@@ -1153,30 +1145,31 @@
       <c r="V16" s="5"/>
       <c r="W16" s="5"/>
       <c r="X16" s="5"/>
-      <c r="Y16" s="5"/>
-    </row>
-    <row r="17" spans="1:25" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="9"/>
-      <c r="B17" s="9"/>
-      <c r="C17" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="D17" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="E17" s="12">
-        <v>44850</v>
-      </c>
-      <c r="F17" s="12">
-        <v>44852</v>
-      </c>
-      <c r="G17" s="12">
-        <v>44850</v>
-      </c>
-      <c r="H17" s="12">
-        <v>44852</v>
-      </c>
-      <c r="I17" s="9"/>
+    </row>
+    <row r="17" spans="1:24" ht="57" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="16">
+        <v>6</v>
+      </c>
+      <c r="B17" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="C17" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="D17" s="19">
+        <v>44843</v>
+      </c>
+      <c r="E17" s="19">
+        <v>44846</v>
+      </c>
+      <c r="F17" s="19">
+        <v>44843</v>
+      </c>
+      <c r="G17" s="19">
+        <v>44846</v>
+      </c>
+      <c r="H17" s="16"/>
+      <c r="I17" s="5"/>
       <c r="J17" s="5"/>
       <c r="K17" s="5"/>
       <c r="L17" s="5"/>
@@ -1192,30 +1185,27 @@
       <c r="V17" s="5"/>
       <c r="W17" s="5"/>
       <c r="X17" s="5"/>
-      <c r="Y17" s="5"/>
-    </row>
-    <row r="18" spans="1:25" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="9"/>
-      <c r="B18" s="9"/>
-      <c r="C18" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="D18" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="E18" s="12">
-        <v>44853</v>
-      </c>
-      <c r="F18" s="12">
-        <v>44855</v>
-      </c>
-      <c r="G18" s="12">
-        <v>44853</v>
-      </c>
-      <c r="H18" s="12">
-        <v>44855</v>
-      </c>
-      <c r="I18" s="9"/>
+    </row>
+    <row r="18" spans="1:24" ht="31.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="16"/>
+      <c r="B18" s="16"/>
+      <c r="C18" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="D18" s="19">
+        <v>44847</v>
+      </c>
+      <c r="E18" s="19">
+        <v>44849</v>
+      </c>
+      <c r="F18" s="19">
+        <v>44847</v>
+      </c>
+      <c r="G18" s="19">
+        <v>44849</v>
+      </c>
+      <c r="H18" s="16"/>
+      <c r="I18" s="5"/>
       <c r="J18" s="5"/>
       <c r="K18" s="5"/>
       <c r="L18" s="5"/>
@@ -1231,30 +1221,27 @@
       <c r="V18" s="5"/>
       <c r="W18" s="5"/>
       <c r="X18" s="5"/>
-      <c r="Y18" s="5"/>
-    </row>
-    <row r="19" spans="1:25" ht="21.6" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A19" s="9"/>
-      <c r="B19" s="9"/>
-      <c r="C19" s="13" t="s">
-        <v>37</v>
-      </c>
-      <c r="D19" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="E19" s="12">
-        <v>44856</v>
-      </c>
-      <c r="F19" s="12">
-        <v>44858</v>
-      </c>
-      <c r="G19" s="12">
-        <v>44856</v>
-      </c>
-      <c r="H19" s="12">
-        <v>44858</v>
-      </c>
-      <c r="I19" s="9"/>
+    </row>
+    <row r="19" spans="1:24" ht="31.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="16"/>
+      <c r="B19" s="16"/>
+      <c r="C19" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="D19" s="19">
+        <v>44850</v>
+      </c>
+      <c r="E19" s="19">
+        <v>44852</v>
+      </c>
+      <c r="F19" s="19">
+        <v>44850</v>
+      </c>
+      <c r="G19" s="19">
+        <v>44852</v>
+      </c>
+      <c r="H19" s="16"/>
+      <c r="I19" s="5"/>
       <c r="J19" s="5"/>
       <c r="K19" s="5"/>
       <c r="L19" s="5"/>
@@ -1270,30 +1257,27 @@
       <c r="V19" s="5"/>
       <c r="W19" s="5"/>
       <c r="X19" s="5"/>
-      <c r="Y19" s="5"/>
-    </row>
-    <row r="20" spans="1:25" ht="22.95" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A20" s="9"/>
-      <c r="B20" s="9"/>
-      <c r="C20" s="13" t="s">
-        <v>38</v>
-      </c>
-      <c r="D20" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="E20" s="12">
-        <v>44859</v>
-      </c>
-      <c r="F20" s="12">
-        <v>44861</v>
-      </c>
-      <c r="G20" s="12">
-        <v>44859</v>
-      </c>
-      <c r="H20" s="12">
-        <v>44861</v>
-      </c>
-      <c r="I20" s="9"/>
+    </row>
+    <row r="20" spans="1:24" ht="31.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="16"/>
+      <c r="B20" s="16"/>
+      <c r="C20" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="D20" s="19">
+        <v>44853</v>
+      </c>
+      <c r="E20" s="19">
+        <v>44855</v>
+      </c>
+      <c r="F20" s="19">
+        <v>44853</v>
+      </c>
+      <c r="G20" s="19">
+        <v>44855</v>
+      </c>
+      <c r="H20" s="16"/>
+      <c r="I20" s="5"/>
       <c r="J20" s="5"/>
       <c r="K20" s="5"/>
       <c r="L20" s="5"/>
@@ -1309,30 +1293,27 @@
       <c r="V20" s="5"/>
       <c r="W20" s="5"/>
       <c r="X20" s="5"/>
-      <c r="Y20" s="5"/>
-    </row>
-    <row r="21" spans="1:25" ht="22.2" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A21" s="9"/>
-      <c r="B21" s="9"/>
-      <c r="C21" s="13" t="s">
-        <v>39</v>
-      </c>
-      <c r="D21" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="E21" s="12">
-        <v>44862</v>
-      </c>
-      <c r="F21" s="12">
-        <v>44863</v>
-      </c>
-      <c r="G21" s="12">
-        <v>44862</v>
-      </c>
-      <c r="H21" s="12">
-        <v>44863</v>
-      </c>
-      <c r="I21" s="9"/>
+    </row>
+    <row r="21" spans="1:24" ht="28.8" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A21" s="16"/>
+      <c r="B21" s="16"/>
+      <c r="C21" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="D21" s="19">
+        <v>44856</v>
+      </c>
+      <c r="E21" s="19">
+        <v>44858</v>
+      </c>
+      <c r="F21" s="19">
+        <v>44856</v>
+      </c>
+      <c r="G21" s="19">
+        <v>44858</v>
+      </c>
+      <c r="H21" s="16"/>
+      <c r="I21" s="5"/>
       <c r="J21" s="5"/>
       <c r="K21" s="5"/>
       <c r="L21" s="5"/>
@@ -1348,30 +1329,27 @@
       <c r="V21" s="5"/>
       <c r="W21" s="5"/>
       <c r="X21" s="5"/>
-      <c r="Y21" s="5"/>
-    </row>
-    <row r="22" spans="1:25" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A22" s="9"/>
-      <c r="B22" s="9"/>
-      <c r="C22" s="13" t="s">
-        <v>34</v>
-      </c>
-      <c r="D22" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="E22" s="12">
-        <v>44864</v>
-      </c>
-      <c r="F22" s="12">
-        <v>44866</v>
-      </c>
-      <c r="G22" s="12">
-        <v>44864</v>
-      </c>
-      <c r="H22" s="12">
-        <v>44866</v>
-      </c>
-      <c r="I22" s="9"/>
+    </row>
+    <row r="22" spans="1:24" ht="29.4" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A22" s="16"/>
+      <c r="B22" s="16"/>
+      <c r="C22" s="20" t="s">
+        <v>37</v>
+      </c>
+      <c r="D22" s="19">
+        <v>44859</v>
+      </c>
+      <c r="E22" s="19">
+        <v>44861</v>
+      </c>
+      <c r="F22" s="19">
+        <v>44859</v>
+      </c>
+      <c r="G22" s="19">
+        <v>44861</v>
+      </c>
+      <c r="H22" s="16"/>
+      <c r="I22" s="5"/>
       <c r="J22" s="5"/>
       <c r="K22" s="5"/>
       <c r="L22" s="5"/>
@@ -1387,30 +1365,27 @@
       <c r="V22" s="5"/>
       <c r="W22" s="5"/>
       <c r="X22" s="5"/>
-      <c r="Y22" s="5"/>
-    </row>
-    <row r="23" spans="1:25" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A23" s="9"/>
-      <c r="B23" s="9"/>
-      <c r="C23" s="13" t="s">
-        <v>40</v>
-      </c>
-      <c r="D23" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="E23" s="12">
-        <v>44867</v>
-      </c>
-      <c r="F23" s="12">
-        <v>44869</v>
-      </c>
-      <c r="G23" s="12">
-        <v>44867</v>
-      </c>
-      <c r="H23" s="12">
-        <v>44869</v>
-      </c>
-      <c r="I23" s="9"/>
+    </row>
+    <row r="23" spans="1:24" ht="30.6" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A23" s="16"/>
+      <c r="B23" s="16"/>
+      <c r="C23" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="D23" s="19">
+        <v>44862</v>
+      </c>
+      <c r="E23" s="19">
+        <v>44863</v>
+      </c>
+      <c r="F23" s="19">
+        <v>44862</v>
+      </c>
+      <c r="G23" s="19">
+        <v>44863</v>
+      </c>
+      <c r="H23" s="16"/>
+      <c r="I23" s="5"/>
       <c r="J23" s="5"/>
       <c r="K23" s="5"/>
       <c r="L23" s="5"/>
@@ -1426,30 +1401,27 @@
       <c r="V23" s="5"/>
       <c r="W23" s="5"/>
       <c r="X23" s="5"/>
-      <c r="Y23" s="5"/>
-    </row>
-    <row r="24" spans="1:25" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="9"/>
-      <c r="B24" s="9"/>
-      <c r="C24" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="D24" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="E24" s="12">
-        <v>44870</v>
-      </c>
-      <c r="F24" s="12">
-        <v>44873</v>
-      </c>
-      <c r="G24" s="12">
-        <v>44870</v>
-      </c>
-      <c r="H24" s="12">
-        <v>44873</v>
-      </c>
-      <c r="I24" s="9"/>
+    </row>
+    <row r="24" spans="1:24" ht="36" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A24" s="16"/>
+      <c r="B24" s="16"/>
+      <c r="C24" s="20" t="s">
+        <v>33</v>
+      </c>
+      <c r="D24" s="19">
+        <v>44864</v>
+      </c>
+      <c r="E24" s="19">
+        <v>44866</v>
+      </c>
+      <c r="F24" s="19">
+        <v>44864</v>
+      </c>
+      <c r="G24" s="19">
+        <v>44866</v>
+      </c>
+      <c r="H24" s="16"/>
+      <c r="I24" s="5"/>
       <c r="J24" s="5"/>
       <c r="K24" s="5"/>
       <c r="L24" s="5"/>
@@ -1465,28 +1437,27 @@
       <c r="V24" s="5"/>
       <c r="W24" s="5"/>
       <c r="X24" s="5"/>
-      <c r="Y24" s="5"/>
-    </row>
-    <row r="25" spans="1:25" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="9"/>
-      <c r="B25" s="9"/>
-      <c r="C25" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="D25" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="E25" s="12">
-        <v>44875</v>
-      </c>
-      <c r="F25" s="12">
-        <v>44880</v>
-      </c>
-      <c r="G25" s="12">
-        <v>44875</v>
-      </c>
-      <c r="H25" s="12"/>
-      <c r="I25" s="9"/>
+    </row>
+    <row r="25" spans="1:24" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A25" s="16"/>
+      <c r="B25" s="16"/>
+      <c r="C25" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="D25" s="19">
+        <v>44867</v>
+      </c>
+      <c r="E25" s="19">
+        <v>44869</v>
+      </c>
+      <c r="F25" s="19">
+        <v>44867</v>
+      </c>
+      <c r="G25" s="19">
+        <v>44869</v>
+      </c>
+      <c r="H25" s="16"/>
+      <c r="I25" s="5"/>
       <c r="J25" s="5"/>
       <c r="K25" s="5"/>
       <c r="L25" s="5"/>
@@ -1502,28 +1473,27 @@
       <c r="V25" s="5"/>
       <c r="W25" s="5"/>
       <c r="X25" s="5"/>
-      <c r="Y25" s="5"/>
-    </row>
-    <row r="26" spans="1:25" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="9">
-        <v>7</v>
-      </c>
-      <c r="B26" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="C26" s="10"/>
-      <c r="D26" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="E26" s="12">
-        <v>44881</v>
-      </c>
-      <c r="F26" s="12">
-        <v>44883</v>
-      </c>
-      <c r="G26" s="12"/>
-      <c r="H26" s="12"/>
-      <c r="I26" s="9"/>
+    </row>
+    <row r="26" spans="1:24" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="16"/>
+      <c r="B26" s="16"/>
+      <c r="C26" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="D26" s="19">
+        <v>44870</v>
+      </c>
+      <c r="E26" s="19">
+        <v>44873</v>
+      </c>
+      <c r="F26" s="19">
+        <v>44870</v>
+      </c>
+      <c r="G26" s="19">
+        <v>44873</v>
+      </c>
+      <c r="H26" s="16"/>
+      <c r="I26" s="5"/>
       <c r="J26" s="5"/>
       <c r="K26" s="5"/>
       <c r="L26" s="5"/>
@@ -1539,30 +1509,27 @@
       <c r="V26" s="5"/>
       <c r="W26" s="5"/>
       <c r="X26" s="5"/>
-      <c r="Y26" s="5"/>
-    </row>
-    <row r="27" spans="1:25" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="9">
-        <v>8</v>
-      </c>
-      <c r="B27" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="C27" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="D27" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="E27" s="12">
-        <v>44884</v>
-      </c>
-      <c r="F27" s="12">
-        <v>44889</v>
-      </c>
-      <c r="G27" s="12"/>
-      <c r="H27" s="12"/>
-      <c r="I27" s="9"/>
+    </row>
+    <row r="27" spans="1:24" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="16"/>
+      <c r="B27" s="16"/>
+      <c r="C27" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="D27" s="19">
+        <v>44875</v>
+      </c>
+      <c r="E27" s="19">
+        <v>44880</v>
+      </c>
+      <c r="F27" s="19">
+        <v>44875</v>
+      </c>
+      <c r="G27" s="19">
+        <v>44880</v>
+      </c>
+      <c r="H27" s="16"/>
+      <c r="I27" s="5"/>
       <c r="J27" s="5"/>
       <c r="K27" s="5"/>
       <c r="L27" s="5"/>
@@ -1578,28 +1545,25 @@
       <c r="V27" s="5"/>
       <c r="W27" s="5"/>
       <c r="X27" s="5"/>
-      <c r="Y27" s="5"/>
-    </row>
-    <row r="28" spans="1:25" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="9">
-        <v>9</v>
-      </c>
-      <c r="B28" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="C28" s="10"/>
-      <c r="D28" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="E28" s="12">
-        <v>44890</v>
-      </c>
-      <c r="F28" s="12">
-        <v>44894</v>
-      </c>
-      <c r="G28" s="12"/>
-      <c r="H28" s="12"/>
-      <c r="I28" s="9"/>
+    </row>
+    <row r="28" spans="1:24" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="16">
+        <v>7</v>
+      </c>
+      <c r="B28" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="C28" s="17"/>
+      <c r="D28" s="19">
+        <v>44881</v>
+      </c>
+      <c r="E28" s="19">
+        <v>44883</v>
+      </c>
+      <c r="F28" s="19"/>
+      <c r="G28" s="19"/>
+      <c r="H28" s="16"/>
+      <c r="I28" s="5"/>
       <c r="J28" s="5"/>
       <c r="K28" s="5"/>
       <c r="L28" s="5"/>
@@ -1615,18 +1579,27 @@
       <c r="V28" s="5"/>
       <c r="W28" s="5"/>
       <c r="X28" s="5"/>
-      <c r="Y28" s="5"/>
-    </row>
-    <row r="29" spans="1:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="6"/>
-      <c r="B29" s="6"/>
-      <c r="C29" s="7"/>
-      <c r="D29" s="6"/>
-      <c r="E29" s="8"/>
-      <c r="F29" s="8"/>
-      <c r="G29" s="8"/>
-      <c r="H29" s="8"/>
-      <c r="I29" s="6"/>
+    </row>
+    <row r="29" spans="1:24" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="16">
+        <v>8</v>
+      </c>
+      <c r="B29" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="C29" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="D29" s="19">
+        <v>44884</v>
+      </c>
+      <c r="E29" s="19">
+        <v>44889</v>
+      </c>
+      <c r="F29" s="19"/>
+      <c r="G29" s="19"/>
+      <c r="H29" s="16"/>
+      <c r="I29" s="5"/>
       <c r="J29" s="5"/>
       <c r="K29" s="5"/>
       <c r="L29" s="5"/>
@@ -1642,18 +1615,25 @@
       <c r="V29" s="5"/>
       <c r="W29" s="5"/>
       <c r="X29" s="5"/>
-      <c r="Y29" s="5"/>
-    </row>
-    <row r="30" spans="1:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="6"/>
-      <c r="B30" s="6"/>
-      <c r="C30" s="7"/>
-      <c r="D30" s="6"/>
-      <c r="E30" s="8"/>
-      <c r="F30" s="8"/>
-      <c r="G30" s="8"/>
-      <c r="H30" s="8"/>
-      <c r="I30" s="6"/>
+    </row>
+    <row r="30" spans="1:24" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="16">
+        <v>9</v>
+      </c>
+      <c r="B30" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="C30" s="17"/>
+      <c r="D30" s="19">
+        <v>44890</v>
+      </c>
+      <c r="E30" s="19">
+        <v>44894</v>
+      </c>
+      <c r="F30" s="19"/>
+      <c r="G30" s="19"/>
+      <c r="H30" s="16"/>
+      <c r="I30" s="5"/>
       <c r="J30" s="5"/>
       <c r="K30" s="5"/>
       <c r="L30" s="5"/>
@@ -1669,18 +1649,17 @@
       <c r="V30" s="5"/>
       <c r="W30" s="5"/>
       <c r="X30" s="5"/>
-      <c r="Y30" s="5"/>
-    </row>
-    <row r="31" spans="1:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="31" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="6"/>
       <c r="B31" s="6"/>
       <c r="C31" s="7"/>
-      <c r="D31" s="6"/>
+      <c r="D31" s="8"/>
       <c r="E31" s="8"/>
       <c r="F31" s="8"/>
       <c r="G31" s="8"/>
-      <c r="H31" s="8"/>
-      <c r="I31" s="6"/>
+      <c r="H31" s="6"/>
+      <c r="I31" s="5"/>
       <c r="J31" s="5"/>
       <c r="K31" s="5"/>
       <c r="L31" s="5"/>
@@ -1696,18 +1675,17 @@
       <c r="V31" s="5"/>
       <c r="W31" s="5"/>
       <c r="X31" s="5"/>
-      <c r="Y31" s="5"/>
-    </row>
-    <row r="32" spans="1:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="32" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="6"/>
       <c r="B32" s="6"/>
       <c r="C32" s="7"/>
-      <c r="D32" s="6"/>
+      <c r="D32" s="8"/>
       <c r="E32" s="8"/>
       <c r="F32" s="8"/>
       <c r="G32" s="8"/>
-      <c r="H32" s="8"/>
-      <c r="I32" s="6"/>
+      <c r="H32" s="6"/>
+      <c r="I32" s="5"/>
       <c r="J32" s="5"/>
       <c r="K32" s="5"/>
       <c r="L32" s="5"/>
@@ -1723,18 +1701,17 @@
       <c r="V32" s="5"/>
       <c r="W32" s="5"/>
       <c r="X32" s="5"/>
-      <c r="Y32" s="5"/>
-    </row>
-    <row r="33" spans="1:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="33" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="6"/>
       <c r="B33" s="6"/>
       <c r="C33" s="7"/>
-      <c r="D33" s="6"/>
+      <c r="D33" s="8"/>
       <c r="E33" s="8"/>
       <c r="F33" s="8"/>
       <c r="G33" s="8"/>
-      <c r="H33" s="8"/>
-      <c r="I33" s="6"/>
+      <c r="H33" s="6"/>
+      <c r="I33" s="5"/>
       <c r="J33" s="5"/>
       <c r="K33" s="5"/>
       <c r="L33" s="5"/>
@@ -1750,18 +1727,17 @@
       <c r="V33" s="5"/>
       <c r="W33" s="5"/>
       <c r="X33" s="5"/>
-      <c r="Y33" s="5"/>
-    </row>
-    <row r="34" spans="1:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="34" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="6"/>
       <c r="B34" s="6"/>
       <c r="C34" s="7"/>
-      <c r="D34" s="6"/>
+      <c r="D34" s="8"/>
       <c r="E34" s="8"/>
       <c r="F34" s="8"/>
       <c r="G34" s="8"/>
-      <c r="H34" s="8"/>
-      <c r="I34" s="6"/>
+      <c r="H34" s="6"/>
+      <c r="I34" s="5"/>
       <c r="J34" s="5"/>
       <c r="K34" s="5"/>
       <c r="L34" s="5"/>
@@ -1777,48 +1753,93 @@
       <c r="V34" s="5"/>
       <c r="W34" s="5"/>
       <c r="X34" s="5"/>
-      <c r="Y34" s="5"/>
-    </row>
-    <row r="35" spans="1:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C35" s="4"/>
-    </row>
-    <row r="36" spans="1:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C36" s="4"/>
-    </row>
-    <row r="37" spans="1:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="35" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="6"/>
+      <c r="B35" s="6"/>
+      <c r="C35" s="7"/>
+      <c r="D35" s="8"/>
+      <c r="E35" s="8"/>
+      <c r="F35" s="8"/>
+      <c r="G35" s="8"/>
+      <c r="H35" s="6"/>
+      <c r="I35" s="5"/>
+      <c r="J35" s="5"/>
+      <c r="K35" s="5"/>
+      <c r="L35" s="5"/>
+      <c r="M35" s="5"/>
+      <c r="N35" s="5"/>
+      <c r="O35" s="5"/>
+      <c r="P35" s="5"/>
+      <c r="Q35" s="5"/>
+      <c r="R35" s="5"/>
+      <c r="S35" s="5"/>
+      <c r="T35" s="5"/>
+      <c r="U35" s="5"/>
+      <c r="V35" s="5"/>
+      <c r="W35" s="5"/>
+      <c r="X35" s="5"/>
+    </row>
+    <row r="36" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="6"/>
+      <c r="B36" s="6"/>
+      <c r="C36" s="7"/>
+      <c r="D36" s="8"/>
+      <c r="E36" s="8"/>
+      <c r="F36" s="8"/>
+      <c r="G36" s="8"/>
+      <c r="H36" s="6"/>
+      <c r="I36" s="5"/>
+      <c r="J36" s="5"/>
+      <c r="K36" s="5"/>
+      <c r="L36" s="5"/>
+      <c r="M36" s="5"/>
+      <c r="N36" s="5"/>
+      <c r="O36" s="5"/>
+      <c r="P36" s="5"/>
+      <c r="Q36" s="5"/>
+      <c r="R36" s="5"/>
+      <c r="S36" s="5"/>
+      <c r="T36" s="5"/>
+      <c r="U36" s="5"/>
+      <c r="V36" s="5"/>
+      <c r="W36" s="5"/>
+      <c r="X36" s="5"/>
+    </row>
+    <row r="37" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C37" s="4"/>
     </row>
-    <row r="38" spans="1:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C38" s="4"/>
     </row>
-    <row r="39" spans="1:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C39" s="4"/>
     </row>
-    <row r="40" spans="1:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C40" s="4"/>
     </row>
-    <row r="41" spans="1:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C41" s="4"/>
     </row>
-    <row r="42" spans="1:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C42" s="4"/>
     </row>
-    <row r="43" spans="1:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C43" s="4"/>
     </row>
-    <row r="44" spans="1:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C44" s="4"/>
     </row>
-    <row r="45" spans="1:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C45" s="4"/>
     </row>
-    <row r="46" spans="1:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C46" s="4"/>
     </row>
-    <row r="47" spans="1:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C47" s="4"/>
     </row>
-    <row r="48" spans="1:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C48" s="4"/>
     </row>
     <row r="49" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -4686,17 +4707,23 @@
     <row r="1003" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C1003" s="4"/>
     </row>
+    <row r="1004" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C1004" s="4"/>
+    </row>
+    <row r="1005" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C1005" s="4"/>
+    </row>
   </sheetData>
   <mergeCells count="4">
-    <mergeCell ref="A1:I1"/>
-    <mergeCell ref="A2:I2"/>
-    <mergeCell ref="A3:I3"/>
-    <mergeCell ref="C4:I4"/>
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="A2:H2"/>
+    <mergeCell ref="A3:H3"/>
+    <mergeCell ref="C4:H4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
-  <pageSetup orientation="landscape"/>
+  <pageSetup orientation="landscape" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
file picker in android 12 added, scan audio file first time fixed
</commit_message>
<xml_diff>
--- a/PlanExcel/plan.xlsx
+++ b/PlanExcel/plan.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="49">
   <si>
     <t>KHOA CÔNG NGHỆ THÔNG TIN</t>
   </si>
@@ -178,6 +178,9 @@
   </si>
   <si>
     <t>24/11</t>
+  </si>
+  <si>
+    <t>25/11</t>
   </si>
 </sst>
 </file>
@@ -616,8 +619,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X1005"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B16" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F30" sqref="F30"/>
+    <sheetView tabSelected="1" topLeftCell="B22" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1650,7 +1653,9 @@
       <c r="E30" s="19">
         <v>44894</v>
       </c>
-      <c r="F30" s="19"/>
+      <c r="F30" s="19" t="s">
+        <v>48</v>
+      </c>
       <c r="G30" s="19"/>
       <c r="H30" s="16"/>
       <c r="I30" s="5"/>

</xml_diff>